<commit_message>
commit atualizacao tesouro dia 06/05
</commit_message>
<xml_diff>
--- a/TESOURO DIRETO_0519 - Compra.xlsx
+++ b/TESOURO DIRETO_0519 - Compra.xlsx
@@ -5,27 +5,28 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RHF Talentos\Downloads\tesouroDireto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suporte\Downloads\tesouro\tesourodireto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="020519" sheetId="21" r:id="rId1"/>
     <sheet name="030519" sheetId="22" r:id="rId2"/>
-    <sheet name="COMPARAÇÃO DIA A DIA" sheetId="4" r:id="rId3"/>
-    <sheet name="TESOURO IPCA" sheetId="5" r:id="rId4"/>
-    <sheet name="TESOURO IPCA JUROS SEMESTRAIS" sheetId="6" r:id="rId5"/>
-    <sheet name="TESOURO PREFIXADOS" sheetId="7" r:id="rId6"/>
-    <sheet name="TESOURO SELIC" sheetId="8" r:id="rId7"/>
+    <sheet name="060519" sheetId="23" r:id="rId3"/>
+    <sheet name="COMPARAÇÃO DIA A DIA" sheetId="4" r:id="rId4"/>
+    <sheet name="TESOURO IPCA" sheetId="5" r:id="rId5"/>
+    <sheet name="TESOURO IPCA JUROS SEMESTRAIS" sheetId="6" r:id="rId6"/>
+    <sheet name="TESOURO PREFIXADOS" sheetId="7" r:id="rId7"/>
+    <sheet name="TESOURO SELIC" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="24">
   <si>
     <t>Vencimento</t>
   </si>
@@ -83,18 +84,33 @@
   <si>
     <t>Dia/Mês</t>
   </si>
+  <si>
+    <t>DATA COMPRA</t>
+  </si>
+  <si>
+    <t>VALOR COMPRADO</t>
+  </si>
+  <si>
+    <t>FRAÇÃO</t>
+  </si>
+  <si>
+    <t>VALOR COMPRA</t>
+  </si>
+  <si>
+    <t>Compra 02/05/2019</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="164" formatCode="&quot;R$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="dd/mm"/>
-    <numFmt numFmtId="166" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00"/>
+    <numFmt numFmtId="8" formatCode="&quot;R$&quot;#,##0.00;[Red]\-&quot;R$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;R$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="dd/mm"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -124,8 +140,14 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,8 +184,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAECC53"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -496,11 +524,111 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -511,7 +639,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -520,43 +648,43 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -580,7 +708,7 @@
     <xf numFmtId="14" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -595,31 +723,31 @@
     <xf numFmtId="14" fontId="2" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -637,7 +765,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="2" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="3" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -682,10 +810,10 @@
     <xf numFmtId="14" fontId="2" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="3" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -703,10 +831,10 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -726,6 +854,57 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="3" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -928,7 +1107,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1128,7 +1306,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1328,7 +1505,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1528,7 +1704,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1728,7 +1903,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1928,7 +2102,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2044,11 +2217,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="240775968"/>
-        <c:axId val="240623152"/>
+        <c:axId val="911051792"/>
+        <c:axId val="911052880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="240775968"/>
+        <c:axId val="911051792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2090,7 +2263,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240623152"/>
+        <c:crossAx val="911052880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2098,7 +2271,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="240623152"/>
+        <c:axId val="911052880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2148,7 +2321,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240775968"/>
+        <c:crossAx val="911051792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2254,7 +2427,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2359,7 +2531,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2496,8 +2667,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="242540440"/>
-        <c:axId val="242540832"/>
+        <c:axId val="966173056"/>
+        <c:axId val="966170880"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -2902,7 +3073,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="242540440"/>
+        <c:axId val="966173056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2936,7 +3107,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242540832"/>
+        <c:crossAx val="966170880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2944,7 +3115,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="242540832"/>
+        <c:axId val="966170880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2954,7 +3125,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242540440"/>
+        <c:crossAx val="966173056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2968,7 +3139,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3046,7 +3216,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3151,7 +3320,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3288,8 +3456,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="242541616"/>
-        <c:axId val="242542008"/>
+        <c:axId val="966171424"/>
+        <c:axId val="966183936"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3694,7 +3862,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="242541616"/>
+        <c:axId val="966171424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3728,7 +3896,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242542008"/>
+        <c:crossAx val="966183936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3736,7 +3904,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="242542008"/>
+        <c:axId val="966183936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3746,7 +3914,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242541616"/>
+        <c:crossAx val="966171424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3760,7 +3928,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3878,7 +4045,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4004,7 +4170,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4189,7 +4354,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4374,7 +4538,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4491,11 +4654,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="242542792"/>
-        <c:axId val="242543184"/>
+        <c:axId val="966181760"/>
+        <c:axId val="966170336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="242542792"/>
+        <c:axId val="966181760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4538,7 +4701,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242543184"/>
+        <c:crossAx val="966170336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4546,7 +4709,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="242543184"/>
+        <c:axId val="966170336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4556,7 +4719,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242542792"/>
+        <c:crossAx val="966181760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4570,7 +4733,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4652,7 +4814,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4757,7 +4918,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4894,11 +5054,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="241986208"/>
-        <c:axId val="241986600"/>
+        <c:axId val="966168704"/>
+        <c:axId val="966182304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="241986208"/>
+        <c:axId val="966168704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4932,7 +5092,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241986600"/>
+        <c:crossAx val="966182304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4940,7 +5100,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241986600"/>
+        <c:axId val="966182304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4950,7 +5110,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241986208"/>
+        <c:crossAx val="966168704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4964,7 +5124,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5042,7 +5201,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5147,7 +5305,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -5284,8 +5441,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="241987384"/>
-        <c:axId val="241987776"/>
+        <c:axId val="966177952"/>
+        <c:axId val="966173600"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -5690,7 +5847,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="241987384"/>
+        <c:axId val="966177952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5724,7 +5881,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241987776"/>
+        <c:crossAx val="966173600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5732,7 +5889,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241987776"/>
+        <c:axId val="966173600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5742,7 +5899,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241987384"/>
+        <c:crossAx val="966177952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5756,7 +5913,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5834,7 +5990,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5939,7 +6094,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -6076,8 +6230,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="241988560"/>
-        <c:axId val="241988952"/>
+        <c:axId val="966169248"/>
+        <c:axId val="966171968"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -6482,7 +6636,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="241988560"/>
+        <c:axId val="966169248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6516,7 +6670,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241988952"/>
+        <c:crossAx val="966171968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6524,7 +6678,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241988952"/>
+        <c:axId val="966171968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6534,7 +6688,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241988560"/>
+        <c:crossAx val="966169248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6548,7 +6702,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6626,7 +6779,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6731,7 +6883,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -6868,8 +7019,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="241989736"/>
-        <c:axId val="243490368"/>
+        <c:axId val="966169792"/>
+        <c:axId val="966172512"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -7274,7 +7425,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="241989736"/>
+        <c:axId val="966169792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7308,7 +7459,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243490368"/>
+        <c:crossAx val="966172512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7316,7 +7467,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243490368"/>
+        <c:axId val="966172512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7326,7 +7477,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241989736"/>
+        <c:crossAx val="966169792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7340,7 +7491,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7418,7 +7568,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7523,7 +7672,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -7660,8 +7808,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="243491152"/>
-        <c:axId val="243491544"/>
+        <c:axId val="966175776"/>
+        <c:axId val="966174144"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -8066,7 +8214,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="243491152"/>
+        <c:axId val="966175776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8100,7 +8248,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243491544"/>
+        <c:crossAx val="966174144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8108,7 +8256,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243491544"/>
+        <c:axId val="966174144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8118,7 +8266,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="243491152"/>
+        <c:crossAx val="966175776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8132,7 +8280,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8210,7 +8357,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8315,7 +8461,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -8452,11 +8597,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="243492328"/>
-        <c:axId val="243492720"/>
+        <c:axId val="966178496"/>
+        <c:axId val="966180128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="243492328"/>
+        <c:axId val="966178496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8490,7 +8635,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243492720"/>
+        <c:crossAx val="966180128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8498,7 +8643,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243492720"/>
+        <c:axId val="966180128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8508,7 +8653,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="243492328"/>
+        <c:crossAx val="966178496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8522,7 +8667,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8600,7 +8744,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8705,7 +8848,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -8842,8 +8984,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="243493504"/>
-        <c:axId val="243493896"/>
+        <c:axId val="966174688"/>
+        <c:axId val="966175232"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -9248,7 +9390,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="243493504"/>
+        <c:axId val="966174688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9282,7 +9424,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243493896"/>
+        <c:crossAx val="966175232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9290,7 +9432,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243493896"/>
+        <c:axId val="966175232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9300,7 +9442,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="243493504"/>
+        <c:crossAx val="966174688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9314,7 +9456,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9827,11 +9968,11 @@
         </c:dLbls>
         <c:gapWidth val="315"/>
         <c:overlap val="-40"/>
-        <c:axId val="184023656"/>
-        <c:axId val="184023264"/>
+        <c:axId val="911054512"/>
+        <c:axId val="911053424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="184023656"/>
+        <c:axId val="911054512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9892,7 +10033,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184023264"/>
+        <c:crossAx val="911053424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9900,7 +10041,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="184023264"/>
+        <c:axId val="911053424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9961,7 +10102,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184023656"/>
+        <c:crossAx val="911054512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10058,7 +10199,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10163,7 +10303,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -10300,8 +10439,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="243793880"/>
-        <c:axId val="243794272"/>
+        <c:axId val="966176320"/>
+        <c:axId val="966177408"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -10706,7 +10845,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="243793880"/>
+        <c:axId val="966176320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10740,7 +10879,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243794272"/>
+        <c:crossAx val="966177408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10748,7 +10887,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243794272"/>
+        <c:axId val="966177408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10758,7 +10897,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="243793880"/>
+        <c:crossAx val="966176320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10772,7 +10911,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10850,7 +10988,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10955,7 +11092,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -11092,8 +11228,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="243795056"/>
-        <c:axId val="243795448"/>
+        <c:axId val="966176864"/>
+        <c:axId val="966179040"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -11498,7 +11634,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="243795056"/>
+        <c:axId val="966176864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11532,7 +11668,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243795448"/>
+        <c:crossAx val="966179040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11540,7 +11676,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243795448"/>
+        <c:axId val="966179040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11550,7 +11686,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="243795056"/>
+        <c:crossAx val="966176864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11564,7 +11700,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11642,7 +11777,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11747,7 +11881,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -11884,8 +12017,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="243796232"/>
-        <c:axId val="243797016"/>
+        <c:axId val="966179584"/>
+        <c:axId val="966180672"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -12290,7 +12423,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="243796232"/>
+        <c:axId val="966179584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12324,7 +12457,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243797016"/>
+        <c:crossAx val="966180672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12332,7 +12465,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243797016"/>
+        <c:axId val="966180672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12342,7 +12475,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="243796232"/>
+        <c:crossAx val="966179584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12356,7 +12489,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12434,7 +12566,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12539,7 +12670,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -12676,8 +12806,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="244094368"/>
-        <c:axId val="244094760"/>
+        <c:axId val="966739424"/>
+        <c:axId val="966734528"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -13082,7 +13212,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="244094368"/>
+        <c:axId val="966739424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13116,7 +13246,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244094760"/>
+        <c:crossAx val="966734528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13124,7 +13254,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244094760"/>
+        <c:axId val="966734528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13134,7 +13264,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244094368"/>
+        <c:crossAx val="966739424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13148,7 +13278,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13226,7 +13355,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13331,7 +13459,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -13468,8 +13595,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="244095544"/>
-        <c:axId val="244095936"/>
+        <c:axId val="966735616"/>
+        <c:axId val="966744320"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -13874,7 +14001,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="244095544"/>
+        <c:axId val="966735616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13908,7 +14035,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244095936"/>
+        <c:crossAx val="966744320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13916,7 +14043,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244095936"/>
+        <c:axId val="966744320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13926,7 +14053,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244095544"/>
+        <c:crossAx val="966735616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13940,7 +14067,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14018,7 +14144,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14123,7 +14248,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -14260,8 +14384,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="244096720"/>
-        <c:axId val="244097112"/>
+        <c:axId val="966744864"/>
+        <c:axId val="966745952"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -14666,7 +14790,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="244096720"/>
+        <c:axId val="966744864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14700,7 +14824,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244097112"/>
+        <c:crossAx val="966745952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14708,7 +14832,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244097112"/>
+        <c:axId val="966745952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14718,7 +14842,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244096720"/>
+        <c:crossAx val="966744864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14732,7 +14856,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14810,7 +14933,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14915,7 +15037,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -15052,8 +15173,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="244379248"/>
-        <c:axId val="244379640"/>
+        <c:axId val="966735072"/>
+        <c:axId val="966748672"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -15458,7 +15579,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="244379248"/>
+        <c:axId val="966735072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15492,7 +15613,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244379640"/>
+        <c:crossAx val="966748672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15500,7 +15621,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244379640"/>
+        <c:axId val="966748672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15510,7 +15631,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244379248"/>
+        <c:crossAx val="966735072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15524,7 +15645,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15602,7 +15722,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15707,7 +15826,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -15844,8 +15962,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="244380424"/>
-        <c:axId val="244380816"/>
+        <c:axId val="966736160"/>
+        <c:axId val="966737248"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -16250,7 +16368,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="244380424"/>
+        <c:axId val="966736160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16284,7 +16402,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244380816"/>
+        <c:crossAx val="966737248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16292,7 +16410,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244380816"/>
+        <c:axId val="966737248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16302,7 +16420,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244380424"/>
+        <c:crossAx val="966736160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16316,7 +16434,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16634,8 +16751,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="244381600"/>
-        <c:axId val="244381992"/>
+        <c:axId val="966742688"/>
+        <c:axId val="966736704"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -17040,7 +17157,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="244381600"/>
+        <c:axId val="966742688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17074,7 +17191,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244381992"/>
+        <c:crossAx val="966736704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17082,7 +17199,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244381992"/>
+        <c:axId val="966736704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17092,7 +17209,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244381600"/>
+        <c:crossAx val="966742688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17423,8 +17540,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="244382776"/>
-        <c:axId val="244637304"/>
+        <c:axId val="966747040"/>
+        <c:axId val="966746496"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -17829,7 +17946,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="244382776"/>
+        <c:axId val="966747040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17863,7 +17980,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244637304"/>
+        <c:crossAx val="966746496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17871,7 +17988,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244637304"/>
+        <c:axId val="966746496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17881,7 +17998,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244382776"/>
+        <c:crossAx val="966747040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17972,7 +18089,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18077,7 +18193,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -18214,11 +18329,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="184022088"/>
-        <c:axId val="242166432"/>
+        <c:axId val="911052336"/>
+        <c:axId val="911053968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="184022088"/>
+        <c:axId val="911052336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18252,7 +18367,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242166432"/>
+        <c:crossAx val="911053968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18260,7 +18375,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="242166432"/>
+        <c:axId val="911053968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18270,7 +18385,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184022088"/>
+        <c:crossAx val="911052336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18284,7 +18399,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18602,8 +18716,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="244638088"/>
-        <c:axId val="244638480"/>
+        <c:axId val="966741600"/>
+        <c:axId val="966747584"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -19008,7 +19122,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="244638088"/>
+        <c:axId val="966741600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19042,7 +19156,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244638480"/>
+        <c:crossAx val="966747584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19050,7 +19164,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244638480"/>
+        <c:axId val="966747584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19060,7 +19174,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244638088"/>
+        <c:crossAx val="966741600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19151,7 +19265,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19266,7 +19379,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -19404,11 +19516,11 @@
         </c:dropLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="244639264"/>
-        <c:axId val="244640048"/>
+        <c:axId val="966743232"/>
+        <c:axId val="966739968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="244639264"/>
+        <c:axId val="966743232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19442,7 +19554,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244640048"/>
+        <c:crossAx val="966739968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19450,7 +19562,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244640048"/>
+        <c:axId val="966739968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19460,7 +19572,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244639264"/>
+        <c:crossAx val="966743232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19523,7 +19635,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19628,7 +19739,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -19765,11 +19875,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="244640832"/>
-        <c:axId val="244788912"/>
+        <c:axId val="966748128"/>
+        <c:axId val="966749216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="244640832"/>
+        <c:axId val="966748128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19803,7 +19913,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244788912"/>
+        <c:crossAx val="966749216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19811,7 +19921,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244788912"/>
+        <c:axId val="966749216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19821,7 +19931,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244640832"/>
+        <c:crossAx val="966748128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19884,7 +19994,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20125,11 +20234,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="244789696"/>
-        <c:axId val="244790088"/>
+        <c:axId val="966745408"/>
+        <c:axId val="966742144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="244789696"/>
+        <c:axId val="966745408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20163,7 +20272,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244790088"/>
+        <c:crossAx val="966742144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20171,7 +20280,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244790088"/>
+        <c:axId val="966742144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20181,7 +20290,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244789696"/>
+        <c:crossAx val="966745408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20244,7 +20353,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20349,7 +20457,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -20486,11 +20593,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="242167216"/>
-        <c:axId val="242167608"/>
+        <c:axId val="911056144"/>
+        <c:axId val="911055600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="242167216"/>
+        <c:axId val="911056144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20524,7 +20631,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242167608"/>
+        <c:crossAx val="911055600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20532,7 +20639,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="242167608"/>
+        <c:axId val="911055600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20542,7 +20649,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242167216"/>
+        <c:crossAx val="911056144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20556,7 +20663,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20634,7 +20740,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20739,7 +20844,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -20876,11 +20980,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="242624624"/>
-        <c:axId val="242625016"/>
+        <c:axId val="911051248"/>
+        <c:axId val="911049072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="242624624"/>
+        <c:axId val="911051248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20914,7 +21018,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242625016"/>
+        <c:crossAx val="911049072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20922,7 +21026,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="242625016"/>
+        <c:axId val="911049072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20932,7 +21036,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242624624"/>
+        <c:crossAx val="911051248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20946,7 +21050,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21264,11 +21367,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="242625800"/>
-        <c:axId val="242626192"/>
+        <c:axId val="618989104"/>
+        <c:axId val="618987472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="242625800"/>
+        <c:axId val="618989104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21302,7 +21405,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242626192"/>
+        <c:crossAx val="618987472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21310,7 +21413,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="242626192"/>
+        <c:axId val="618987472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21320,7 +21423,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242625800"/>
+        <c:crossAx val="618989104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21411,7 +21514,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21516,7 +21618,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -21653,8 +21754,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="242169568"/>
-        <c:axId val="242169176"/>
+        <c:axId val="618990192"/>
+        <c:axId val="838560832"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -22059,7 +22160,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="242169568"/>
+        <c:axId val="618990192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22093,7 +22194,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242169176"/>
+        <c:crossAx val="838560832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22101,7 +22202,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="242169176"/>
+        <c:axId val="838560832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22111,7 +22212,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242169568"/>
+        <c:crossAx val="618990192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22125,7 +22226,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -22203,7 +22303,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -22308,7 +22407,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -22445,8 +22543,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="242169960"/>
-        <c:axId val="242168392"/>
+        <c:axId val="838552128"/>
+        <c:axId val="966182848"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -22851,7 +22949,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="242169960"/>
+        <c:axId val="838552128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22885,7 +22983,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242168392"/>
+        <c:crossAx val="966182848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22893,7 +22991,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="242168392"/>
+        <c:axId val="966182848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22903,7 +23001,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242169960"/>
+        <c:crossAx val="838552128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22917,7 +23015,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -22995,7 +23092,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -23100,7 +23196,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -23237,8 +23332,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="242627368"/>
-        <c:axId val="242627760"/>
+        <c:axId val="966181216"/>
+        <c:axId val="966183392"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -23643,7 +23738,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="242627368"/>
+        <c:axId val="966181216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23677,7 +23772,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242627760"/>
+        <c:crossAx val="966183392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23685,7 +23780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="242627760"/>
+        <c:axId val="966183392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23695,7 +23790,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242627368"/>
+        <c:crossAx val="966181216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23709,7 +23804,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -43323,17 +43417,640 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="77" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="79" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="79" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="79" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="79" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+    </row>
+    <row r="3" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="85" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="86">
+        <v>45519</v>
+      </c>
+      <c r="C3" s="87">
+        <v>4.09</v>
+      </c>
+      <c r="D3" s="88">
+        <v>52.14</v>
+      </c>
+      <c r="E3" s="88">
+        <v>2607.0700000000002</v>
+      </c>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+    </row>
+    <row r="4" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="85" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="86">
+        <v>49444</v>
+      </c>
+      <c r="C4" s="87">
+        <v>4.42</v>
+      </c>
+      <c r="D4" s="88">
+        <v>32.26</v>
+      </c>
+      <c r="E4" s="88">
+        <v>1613.35</v>
+      </c>
+      <c r="F4" s="80" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="81">
+        <v>401.79</v>
+      </c>
+      <c r="H4" s="82">
+        <v>0.25</v>
+      </c>
+      <c r="I4" s="81">
+        <v>1613.35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="85" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="86">
+        <v>53097</v>
+      </c>
+      <c r="C5" s="87">
+        <v>4.42</v>
+      </c>
+      <c r="D5" s="88">
+        <v>31.44</v>
+      </c>
+      <c r="E5" s="88">
+        <v>1048.1199999999999</v>
+      </c>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+    </row>
+    <row r="6" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="85" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="86">
+        <v>46249</v>
+      </c>
+      <c r="C6" s="87">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="D6" s="88">
+        <v>36.33</v>
+      </c>
+      <c r="E6" s="88">
+        <v>3633.42</v>
+      </c>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="80"/>
+    </row>
+    <row r="7" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="85" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="86">
+        <v>49444</v>
+      </c>
+      <c r="C7" s="87">
+        <v>4.33</v>
+      </c>
+      <c r="D7" s="88">
+        <v>39.18</v>
+      </c>
+      <c r="E7" s="88">
+        <v>3918.25</v>
+      </c>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+    </row>
+    <row r="8" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="85" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="86">
+        <v>55015</v>
+      </c>
+      <c r="C8" s="87">
+        <v>4.43</v>
+      </c>
+      <c r="D8" s="88">
+        <v>41.04</v>
+      </c>
+      <c r="E8" s="88">
+        <v>4104.07</v>
+      </c>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="80"/>
+    </row>
+    <row r="9" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="89" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="90"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="90"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
+    </row>
+    <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="85" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="86">
+        <v>44562</v>
+      </c>
+      <c r="C10" s="87">
+        <v>7.74</v>
+      </c>
+      <c r="D10" s="88">
+        <v>32.79</v>
+      </c>
+      <c r="E10" s="88">
+        <v>819.95</v>
+      </c>
+      <c r="F10" s="80"/>
+      <c r="G10" s="80"/>
+      <c r="H10" s="80"/>
+      <c r="I10" s="80"/>
+    </row>
+    <row r="11" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="85" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="86">
+        <v>45658</v>
+      </c>
+      <c r="C11" s="87">
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="D11" s="88">
+        <v>31.16</v>
+      </c>
+      <c r="E11" s="88">
+        <v>623.27</v>
+      </c>
+      <c r="F11" s="80"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="80"/>
+      <c r="I11" s="80"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="85" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="86">
+        <v>47119</v>
+      </c>
+      <c r="C12" s="87">
+        <v>8.91</v>
+      </c>
+      <c r="D12" s="88">
+        <v>33.04</v>
+      </c>
+      <c r="E12" s="88">
+        <v>1101.3900000000001</v>
+      </c>
+      <c r="F12" s="80"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="80"/>
+      <c r="I12" s="80"/>
+    </row>
+    <row r="13" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="89" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="90"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="80"/>
+      <c r="H13" s="80"/>
+      <c r="I13" s="80"/>
+    </row>
+    <row r="14" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="85" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="86">
+        <v>45717</v>
+      </c>
+      <c r="C14" s="87">
+        <v>0.02</v>
+      </c>
+      <c r="D14" s="88">
+        <v>100.77</v>
+      </c>
+      <c r="E14" s="88">
+        <v>10077.66</v>
+      </c>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A13:E13"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="91" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="79" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="79" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="79" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="79" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="85" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="86">
+        <v>45519</v>
+      </c>
+      <c r="C3" s="87">
+        <v>4.04</v>
+      </c>
+      <c r="D3" s="88">
+        <v>52.29</v>
+      </c>
+      <c r="E3" s="88">
+        <v>2614.62</v>
+      </c>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="85" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="86">
+        <v>49444</v>
+      </c>
+      <c r="C4" s="87">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D4" s="88">
+        <v>32.369999999999997</v>
+      </c>
+      <c r="E4" s="88">
+        <v>1618.9</v>
+      </c>
+      <c r="F4" s="80" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="81">
+        <v>401.79</v>
+      </c>
+      <c r="H4" s="82">
+        <v>0.25</v>
+      </c>
+      <c r="I4" s="81">
+        <v>1618.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="85" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="86">
+        <v>53097</v>
+      </c>
+      <c r="C5" s="87">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D5" s="88">
+        <v>31.61</v>
+      </c>
+      <c r="E5" s="88">
+        <v>1053.74</v>
+      </c>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="85" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="86">
+        <v>46249</v>
+      </c>
+      <c r="C6" s="87">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="D6" s="88">
+        <v>36.450000000000003</v>
+      </c>
+      <c r="E6" s="88">
+        <v>3645.27</v>
+      </c>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="80"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="85" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="86">
+        <v>49444</v>
+      </c>
+      <c r="C7" s="87">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="D7" s="88">
+        <v>39.270000000000003</v>
+      </c>
+      <c r="E7" s="88">
+        <v>3927.82</v>
+      </c>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="85" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="86">
+        <v>55015</v>
+      </c>
+      <c r="C8" s="87">
+        <v>4.42</v>
+      </c>
+      <c r="D8" s="88">
+        <v>41.11</v>
+      </c>
+      <c r="E8" s="88">
+        <v>4111.95</v>
+      </c>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="80"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="89" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="90"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="90"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="85" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="86">
+        <v>44562</v>
+      </c>
+      <c r="C10" s="87">
+        <v>7.69</v>
+      </c>
+      <c r="D10" s="88">
+        <v>32.840000000000003</v>
+      </c>
+      <c r="E10" s="88">
+        <v>821.21</v>
+      </c>
+      <c r="F10" s="80"/>
+      <c r="G10" s="80"/>
+      <c r="H10" s="80"/>
+      <c r="I10" s="80"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="85" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="86">
+        <v>45658</v>
+      </c>
+      <c r="C11" s="87">
+        <v>8.67</v>
+      </c>
+      <c r="D11" s="88">
+        <v>31.25</v>
+      </c>
+      <c r="E11" s="88">
+        <v>625.1</v>
+      </c>
+      <c r="F11" s="80"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="80"/>
+      <c r="I11" s="80"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="85" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="86">
+        <v>47119</v>
+      </c>
+      <c r="C12" s="87">
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="D12" s="88">
+        <v>33.130000000000003</v>
+      </c>
+      <c r="E12" s="88">
+        <v>1104.3399999999999</v>
+      </c>
+      <c r="F12" s="80"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="80"/>
+      <c r="I12" s="80"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="89" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="90"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="80"/>
+      <c r="H13" s="80"/>
+      <c r="I13" s="80"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="85" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="86">
+        <v>45717</v>
+      </c>
+      <c r="C14" s="87">
+        <v>0.02</v>
+      </c>
+      <c r="D14" s="88">
+        <v>100.8</v>
+      </c>
+      <c r="E14" s="88">
+        <v>10080.15</v>
+      </c>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A13:E13"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -44789,7 +45506,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>
@@ -45362,7 +46079,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>
@@ -45911,7 +46628,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>
@@ -46460,7 +47177,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>

</xml_diff>

<commit_message>
Commit atualizacao tabela tesouro para data 09/05
</commit_message>
<xml_diff>
--- a/TESOURO DIRETO_0519 - Compra.xlsx
+++ b/TESOURO DIRETO_0519 - Compra.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" firstSheet="6" activeTab="9"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="020519" sheetId="21" r:id="rId1"/>
@@ -17,18 +17,19 @@
     <sheet name="060519" sheetId="23" r:id="rId3"/>
     <sheet name="070519" sheetId="24" r:id="rId4"/>
     <sheet name="080519" sheetId="25" r:id="rId5"/>
-    <sheet name="COMPARAÇÃO DIA A DIA" sheetId="4" r:id="rId6"/>
-    <sheet name="TESOURO IPCA" sheetId="5" r:id="rId7"/>
-    <sheet name="TESOURO IPCA JUROS SEMESTRAIS" sheetId="6" r:id="rId8"/>
-    <sheet name="TESOURO PREFIXADOS" sheetId="7" r:id="rId9"/>
-    <sheet name="TESOURO SELIC" sheetId="8" r:id="rId10"/>
+    <sheet name="090519" sheetId="26" r:id="rId6"/>
+    <sheet name="COMPARAÇÃO DIA A DIA" sheetId="4" r:id="rId7"/>
+    <sheet name="TESOURO IPCA" sheetId="5" r:id="rId8"/>
+    <sheet name="TESOURO IPCA JUROS SEMESTRAIS" sheetId="6" r:id="rId9"/>
+    <sheet name="TESOURO PREFIXADOS" sheetId="7" r:id="rId10"/>
+    <sheet name="TESOURO SELIC" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="24">
   <si>
     <t>Vencimento</t>
   </si>
@@ -861,7 +862,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1325,6 +1326,9 @@
     <xf numFmtId="14" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="2" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1394,9 +1398,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1460,7 +1462,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1598,7 +1599,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1822,7 +1822,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2046,7 +2045,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2270,7 +2268,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2494,7 +2491,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2718,7 +2714,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2858,11 +2853,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="-842328048"/>
-        <c:axId val="-842334032"/>
+        <c:axId val="1908240144"/>
+        <c:axId val="1908241232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-842328048"/>
+        <c:axId val="1908240144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2904,7 +2899,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-842334032"/>
+        <c:crossAx val="1908241232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2912,7 +2907,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-842334032"/>
+        <c:axId val="1908241232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2962,7 +2957,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-842328048"/>
+        <c:crossAx val="1908240144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2976,7 +2971,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3068,7 +3062,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3173,7 +3166,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3334,8 +3326,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-842322608"/>
-        <c:axId val="-822510176"/>
+        <c:axId val="82854576"/>
+        <c:axId val="82850224"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3788,7 +3780,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-842322608"/>
+        <c:axId val="82854576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3822,7 +3814,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-822510176"/>
+        <c:crossAx val="82850224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3830,7 +3822,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-822510176"/>
+        <c:axId val="82850224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3840,7 +3832,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-842322608"/>
+        <c:crossAx val="82854576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3854,7 +3846,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4196,8 +4187,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-822506912"/>
-        <c:axId val="-822519968"/>
+        <c:axId val="82862192"/>
+        <c:axId val="82855120"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -4650,7 +4641,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-822506912"/>
+        <c:axId val="82862192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4684,7 +4675,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-822519968"/>
+        <c:crossAx val="82855120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4692,7 +4683,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-822519968"/>
+        <c:axId val="82855120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4702,7 +4693,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-822506912"/>
+        <c:crossAx val="82862192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5514,11 +5505,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-822509088"/>
-        <c:axId val="-822512896"/>
+        <c:axId val="82859472"/>
+        <c:axId val="82863280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-822509088"/>
+        <c:axId val="82859472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5561,7 +5552,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-822512896"/>
+        <c:crossAx val="82863280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5569,7 +5560,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-822512896"/>
+        <c:axId val="82863280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5579,7 +5570,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-822509088"/>
+        <c:crossAx val="82859472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5938,11 +5929,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-822513440"/>
-        <c:axId val="-822516160"/>
+        <c:axId val="82863824"/>
+        <c:axId val="82864912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-822513440"/>
+        <c:axId val="82863824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5976,7 +5967,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-822516160"/>
+        <c:crossAx val="82864912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5984,7 +5975,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-822516160"/>
+        <c:axId val="82864912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5994,7 +5985,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-822513440"/>
+        <c:crossAx val="82863824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6349,8 +6340,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-822512352"/>
-        <c:axId val="-822509632"/>
+        <c:axId val="82852944"/>
+        <c:axId val="82850768"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -6803,7 +6794,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-822512352"/>
+        <c:axId val="82852944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6837,7 +6828,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-822509632"/>
+        <c:crossAx val="82850768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6845,7 +6836,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-822509632"/>
+        <c:axId val="82850768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6855,7 +6846,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-822512352"/>
+        <c:crossAx val="82852944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7210,8 +7201,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-822510720"/>
-        <c:axId val="-822507456"/>
+        <c:axId val="82855664"/>
+        <c:axId val="82856208"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -7664,7 +7655,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-822510720"/>
+        <c:axId val="82855664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7698,7 +7689,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-822507456"/>
+        <c:crossAx val="82856208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7706,7 +7697,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-822507456"/>
+        <c:axId val="82856208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7716,7 +7707,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-822510720"/>
+        <c:crossAx val="82855664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8071,8 +8062,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-822508000"/>
-        <c:axId val="-822508544"/>
+        <c:axId val="82856752"/>
+        <c:axId val="82857296"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -8525,7 +8516,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-822508000"/>
+        <c:axId val="82856752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8559,7 +8550,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-822508544"/>
+        <c:crossAx val="82857296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8567,7 +8558,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-822508544"/>
+        <c:axId val="82857296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8577,7 +8568,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-822508000"/>
+        <c:crossAx val="82856752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8668,7 +8659,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8773,7 +8763,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -8934,8 +8923,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-822518336"/>
-        <c:axId val="-822522144"/>
+        <c:axId val="82857840"/>
+        <c:axId val="2123219600"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -9388,7 +9377,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-822518336"/>
+        <c:axId val="82857840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9422,7 +9411,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-822522144"/>
+        <c:crossAx val="2123219600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9430,7 +9419,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-822522144"/>
+        <c:axId val="2123219600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9440,7 +9429,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-822518336"/>
+        <c:crossAx val="82857840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9454,7 +9443,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9532,7 +9520,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9637,7 +9624,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -9798,11 +9784,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-822511808"/>
-        <c:axId val="-822514528"/>
+        <c:axId val="2123222864"/>
+        <c:axId val="2123233744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-822511808"/>
+        <c:axId val="2123222864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9836,7 +9822,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-822514528"/>
+        <c:crossAx val="2123233744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9844,7 +9830,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-822514528"/>
+        <c:axId val="2123233744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9854,7 +9840,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-822511808"/>
+        <c:crossAx val="2123222864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9868,7 +9854,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9946,7 +9931,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10051,7 +10035,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -10212,8 +10195,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-822516704"/>
-        <c:axId val="-822515072"/>
+        <c:axId val="2123221776"/>
+        <c:axId val="2123219056"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -10666,7 +10649,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-822516704"/>
+        <c:axId val="2123221776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10700,7 +10683,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-822515072"/>
+        <c:crossAx val="2123219056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10708,7 +10691,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-822515072"/>
+        <c:axId val="2123219056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10718,7 +10701,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-822516704"/>
+        <c:crossAx val="2123221776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10732,7 +10715,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11317,11 +11299,11 @@
         </c:dLbls>
         <c:gapWidth val="315"/>
         <c:overlap val="-40"/>
-        <c:axId val="-842330224"/>
-        <c:axId val="-842329680"/>
+        <c:axId val="1889590352"/>
+        <c:axId val="1889591440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-842330224"/>
+        <c:axId val="1889590352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11382,7 +11364,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-842329680"/>
+        <c:crossAx val="1889591440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11390,7 +11372,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-842329680"/>
+        <c:axId val="1889591440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11451,7 +11433,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-842330224"/>
+        <c:crossAx val="1889590352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11548,7 +11530,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11653,7 +11634,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -11814,8 +11794,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-822521600"/>
-        <c:axId val="-822511264"/>
+        <c:axId val="2123223408"/>
+        <c:axId val="2123231024"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -12268,7 +12248,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-822521600"/>
+        <c:axId val="2123223408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12302,7 +12282,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-822511264"/>
+        <c:crossAx val="2123231024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12310,7 +12290,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-822511264"/>
+        <c:axId val="2123231024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12320,7 +12300,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-822521600"/>
+        <c:crossAx val="2123223408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12334,7 +12314,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12676,8 +12655,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-822521056"/>
-        <c:axId val="-822520512"/>
+        <c:axId val="2123218512"/>
+        <c:axId val="2123229936"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -13130,7 +13109,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-822521056"/>
+        <c:axId val="2123218512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13164,7 +13143,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-822520512"/>
+        <c:crossAx val="2123229936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13172,7 +13151,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-822520512"/>
+        <c:axId val="2123229936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13182,7 +13161,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-822521056"/>
+        <c:crossAx val="2123218512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13273,7 +13252,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13378,7 +13356,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -13539,8 +13516,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-822513984"/>
-        <c:axId val="-822518880"/>
+        <c:axId val="2123230480"/>
+        <c:axId val="2123222320"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -13993,7 +13970,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-822513984"/>
+        <c:axId val="2123230480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14027,7 +14004,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-822518880"/>
+        <c:crossAx val="2123222320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14035,7 +14012,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-822518880"/>
+        <c:axId val="2123222320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14045,7 +14022,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-822513984"/>
+        <c:crossAx val="2123230480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14059,7 +14036,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14137,7 +14113,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14242,7 +14217,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -14403,8 +14377,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-822519424"/>
-        <c:axId val="-822517792"/>
+        <c:axId val="2123220144"/>
+        <c:axId val="2123231568"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -14857,7 +14831,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-822519424"/>
+        <c:axId val="2123220144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14891,7 +14865,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-822517792"/>
+        <c:crossAx val="2123231568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14899,7 +14873,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-822517792"/>
+        <c:axId val="2123231568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14909,7 +14883,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-822519424"/>
+        <c:crossAx val="2123220144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14923,7 +14897,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15265,8 +15238,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-822517248"/>
-        <c:axId val="-822515616"/>
+        <c:axId val="2123229392"/>
+        <c:axId val="2123228848"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -15719,7 +15692,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-822517248"/>
+        <c:axId val="2123229392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15753,7 +15726,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-822515616"/>
+        <c:crossAx val="2123228848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15761,7 +15734,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-822515616"/>
+        <c:axId val="2123228848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15771,7 +15744,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-822517248"/>
+        <c:crossAx val="2123229392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15862,7 +15835,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15967,7 +15939,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -16128,8 +16099,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-818744656"/>
-        <c:axId val="-818730512"/>
+        <c:axId val="2123227760"/>
+        <c:axId val="2123224496"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -16582,7 +16553,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-818744656"/>
+        <c:axId val="2123227760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16616,7 +16587,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-818730512"/>
+        <c:crossAx val="2123224496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16624,7 +16595,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-818730512"/>
+        <c:axId val="2123224496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16634,7 +16605,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-818744656"/>
+        <c:crossAx val="2123227760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16648,7 +16619,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16726,7 +16696,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16831,7 +16800,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -16992,8 +16960,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-818735952"/>
-        <c:axId val="-818741392"/>
+        <c:axId val="2123233200"/>
+        <c:axId val="2123221232"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -17446,7 +17414,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-818735952"/>
+        <c:axId val="2123233200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17480,7 +17448,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-818741392"/>
+        <c:crossAx val="2123221232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17488,7 +17456,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-818741392"/>
+        <c:axId val="2123221232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17498,7 +17466,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-818735952"/>
+        <c:crossAx val="2123233200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17512,7 +17480,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17854,8 +17821,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-818745200"/>
-        <c:axId val="-818733776"/>
+        <c:axId val="2123223952"/>
+        <c:axId val="2123228304"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -18308,7 +18275,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-818745200"/>
+        <c:axId val="2123223952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18342,7 +18309,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-818733776"/>
+        <c:crossAx val="2123228304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18350,7 +18317,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-818733776"/>
+        <c:axId val="2123228304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18360,7 +18327,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-818745200"/>
+        <c:crossAx val="2123223952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18715,8 +18682,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-818736496"/>
-        <c:axId val="-818743568"/>
+        <c:axId val="2123220688"/>
+        <c:axId val="2123225040"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -19169,7 +19136,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-818736496"/>
+        <c:axId val="2123220688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19203,7 +19170,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-818743568"/>
+        <c:crossAx val="2123225040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19211,7 +19178,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-818743568"/>
+        <c:axId val="2123225040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19221,7 +19188,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-818736496"/>
+        <c:crossAx val="2123220688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19576,8 +19543,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-818737584"/>
-        <c:axId val="-818744112"/>
+        <c:axId val="2123232112"/>
+        <c:axId val="2123226672"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -20030,7 +19997,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-818737584"/>
+        <c:axId val="2123232112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20064,7 +20031,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-818744112"/>
+        <c:crossAx val="2123226672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20072,7 +20039,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-818744112"/>
+        <c:axId val="2123226672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20082,7 +20049,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-818737584"/>
+        <c:crossAx val="2123232112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20173,7 +20140,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20278,7 +20244,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -20439,11 +20404,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-842335664"/>
-        <c:axId val="-842323152"/>
+        <c:axId val="82861104"/>
+        <c:axId val="82861648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-842335664"/>
+        <c:axId val="82861104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20477,7 +20442,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-842323152"/>
+        <c:crossAx val="82861648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20485,7 +20450,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-842323152"/>
+        <c:axId val="82861648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20495,7 +20460,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-842335664"/>
+        <c:crossAx val="82861104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20509,7 +20474,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20851,8 +20815,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-818738128"/>
-        <c:axId val="-818737040"/>
+        <c:axId val="2123232656"/>
+        <c:axId val="2123227216"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -21305,7 +21269,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-818738128"/>
+        <c:axId val="2123232656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21339,7 +21303,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-818737040"/>
+        <c:crossAx val="2123227216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21347,7 +21311,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-818737040"/>
+        <c:axId val="2123227216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21357,7 +21321,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-818738128"/>
+        <c:crossAx val="2123232656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21725,11 +21689,11 @@
         </c:dropLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-818735408"/>
-        <c:axId val="-818732688"/>
+        <c:axId val="2123225584"/>
+        <c:axId val="2123226128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-818735408"/>
+        <c:axId val="2123225584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21763,7 +21727,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-818732688"/>
+        <c:crossAx val="2123226128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21771,7 +21735,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-818732688"/>
+        <c:axId val="2123226128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21781,7 +21745,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-818735408"/>
+        <c:crossAx val="2123225584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22110,11 +22074,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-818740848"/>
-        <c:axId val="-818741936"/>
+        <c:axId val="85698480"/>
+        <c:axId val="85687600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-818740848"/>
+        <c:axId val="85698480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22148,7 +22112,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-818741936"/>
+        <c:crossAx val="85687600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22156,7 +22120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-818741936"/>
+        <c:axId val="85687600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22166,7 +22130,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-818740848"/>
+        <c:crossAx val="85698480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22493,11 +22457,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-818732144"/>
-        <c:axId val="-818731056"/>
+        <c:axId val="85688144"/>
+        <c:axId val="85689232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-818732144"/>
+        <c:axId val="85688144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22531,7 +22495,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-818731056"/>
+        <c:crossAx val="85689232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22539,7 +22503,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-818731056"/>
+        <c:axId val="85689232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22549,7 +22513,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-818732144"/>
+        <c:crossAx val="85688144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22612,7 +22576,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -22717,7 +22680,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -22878,11 +22840,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-842335120"/>
-        <c:axId val="-842326416"/>
+        <c:axId val="82854032"/>
+        <c:axId val="82858384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-842335120"/>
+        <c:axId val="82854032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22916,7 +22878,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-842326416"/>
+        <c:crossAx val="82858384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22924,7 +22886,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-842326416"/>
+        <c:axId val="82858384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22934,7 +22896,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-842335120"/>
+        <c:crossAx val="82854032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22948,7 +22910,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -23026,7 +22987,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -23131,7 +23091,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -23292,11 +23251,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-842330768"/>
-        <c:axId val="-842325328"/>
+        <c:axId val="82864368"/>
+        <c:axId val="82853488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-842330768"/>
+        <c:axId val="82864368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23330,7 +23289,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-842325328"/>
+        <c:crossAx val="82853488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23338,7 +23297,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-842325328"/>
+        <c:axId val="82853488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23348,7 +23307,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-842330768"/>
+        <c:crossAx val="82864368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23362,7 +23321,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -23704,11 +23662,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-842332944"/>
-        <c:axId val="-842322064"/>
+        <c:axId val="82862736"/>
+        <c:axId val="82851856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-842332944"/>
+        <c:axId val="82862736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23742,7 +23700,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-842322064"/>
+        <c:crossAx val="82851856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23750,7 +23708,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-842322064"/>
+        <c:axId val="82851856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23760,7 +23718,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-842332944"/>
+        <c:crossAx val="82862736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23851,7 +23809,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -23956,7 +23913,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -24117,8 +24073,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-842333488"/>
-        <c:axId val="-842331856"/>
+        <c:axId val="82851312"/>
+        <c:axId val="82860016"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -24571,7 +24527,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-842333488"/>
+        <c:axId val="82851312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24605,7 +24561,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-842331856"/>
+        <c:crossAx val="82860016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -24613,7 +24569,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-842331856"/>
+        <c:axId val="82860016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24623,7 +24579,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-842333488"/>
+        <c:crossAx val="82851312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -24637,7 +24593,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -24979,8 +24934,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-842329136"/>
-        <c:axId val="-842326960"/>
+        <c:axId val="82849680"/>
+        <c:axId val="82858928"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -25433,7 +25388,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-842329136"/>
+        <c:axId val="82849680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25467,7 +25422,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-842326960"/>
+        <c:crossAx val="82858928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25475,7 +25430,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-842326960"/>
+        <c:axId val="82858928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25485,7 +25440,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-842329136"/>
+        <c:crossAx val="82849680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -25576,7 +25531,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -25681,7 +25635,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -25842,8 +25795,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-842324240"/>
-        <c:axId val="-842323696"/>
+        <c:axId val="82852400"/>
+        <c:axId val="82860560"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -26296,7 +26249,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-842324240"/>
+        <c:axId val="82852400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26330,7 +26283,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-842323696"/>
+        <c:crossAx val="82860560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -26338,7 +26291,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-842323696"/>
+        <c:axId val="82860560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26348,7 +26301,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-842324240"/>
+        <c:crossAx val="82852400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -26362,7 +26315,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -45984,13 +45936,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="156" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="156"/>
-      <c r="C1" s="156"/>
-      <c r="D1" s="156"/>
-      <c r="E1" s="157"/>
+      <c r="B1" s="157"/>
+      <c r="C1" s="157"/>
+      <c r="D1" s="157"/>
+      <c r="E1" s="158"/>
       <c r="F1" s="51" t="s">
         <v>19</v>
       </c>
@@ -46160,13 +46112,13 @@
       <c r="I8" s="52"/>
     </row>
     <row r="9" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="158" t="s">
+      <c r="A9" s="159" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="159"/>
-      <c r="C9" s="159"/>
-      <c r="D9" s="159"/>
-      <c r="E9" s="160"/>
+      <c r="B9" s="160"/>
+      <c r="C9" s="160"/>
+      <c r="D9" s="160"/>
+      <c r="E9" s="161"/>
       <c r="F9" s="52"/>
       <c r="G9" s="52"/>
       <c r="H9" s="52"/>
@@ -46257,13 +46209,13 @@
       <c r="I13" s="52"/>
     </row>
     <row r="14" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="158" t="s">
+      <c r="A14" s="159" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="159"/>
-      <c r="C14" s="159"/>
-      <c r="D14" s="159"/>
-      <c r="E14" s="160"/>
+      <c r="B14" s="160"/>
+      <c r="C14" s="160"/>
+      <c r="D14" s="160"/>
+      <c r="E14" s="161"/>
       <c r="F14" s="52"/>
       <c r="G14" s="52"/>
       <c r="H14" s="52"/>
@@ -46325,7 +46277,664 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3:Q6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="12" max="12" width="28.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" customWidth="1"/>
+    <col min="15" max="15" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="178" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+      <c r="H1" s="178"/>
+      <c r="I1" s="178"/>
+      <c r="J1" s="178"/>
+      <c r="K1" s="178"/>
+      <c r="L1" s="178"/>
+      <c r="M1" s="178"/>
+      <c r="N1" s="178"/>
+      <c r="O1" s="178"/>
+      <c r="P1" s="178"/>
+      <c r="Q1" s="178"/>
+      <c r="R1" s="178"/>
+      <c r="S1" s="178"/>
+      <c r="T1" s="178"/>
+      <c r="U1" s="178"/>
+      <c r="V1" s="178"/>
+      <c r="W1" s="178"/>
+      <c r="X1" s="178"/>
+      <c r="Y1" s="178"/>
+      <c r="Z1" s="178"/>
+      <c r="AA1" s="178"/>
+      <c r="AB1" s="178"/>
+      <c r="AC1" s="178"/>
+      <c r="AD1" s="178"/>
+      <c r="AE1" s="178"/>
+      <c r="AF1" s="178"/>
+      <c r="AG1" s="178"/>
+      <c r="AH1" s="178"/>
+      <c r="AI1" s="178"/>
+      <c r="AJ1" s="178"/>
+      <c r="AK1" s="178"/>
+      <c r="AL1" s="178"/>
+      <c r="AM1" s="178"/>
+      <c r="AN1" s="178"/>
+      <c r="AO1" s="178"/>
+      <c r="AP1" s="178"/>
+      <c r="AQ1" s="178"/>
+      <c r="AR1" s="178"/>
+      <c r="AS1" s="178"/>
+      <c r="AT1" s="178"/>
+      <c r="AU1" s="178"/>
+    </row>
+    <row r="2" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="R2" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="T2" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="V2" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="X2" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y2" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z2" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA2" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC2" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD2" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE2" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF2" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG2" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI2" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ2" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK2" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL2" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM2" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="AN2" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO2" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP2" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ2" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR2" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="AS2" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU2" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="4">
+        <v>43587</v>
+      </c>
+      <c r="D3" s="4">
+        <v>43587</v>
+      </c>
+      <c r="E3" s="5">
+        <v>43587</v>
+      </c>
+      <c r="F3" s="3">
+        <v>43588</v>
+      </c>
+      <c r="G3" s="4">
+        <v>43588</v>
+      </c>
+      <c r="H3" s="5">
+        <v>43588</v>
+      </c>
+      <c r="I3" s="109">
+        <v>43591</v>
+      </c>
+      <c r="J3" s="109">
+        <v>43591</v>
+      </c>
+      <c r="K3" s="109">
+        <v>43591</v>
+      </c>
+      <c r="L3" s="3">
+        <v>43592</v>
+      </c>
+      <c r="M3" s="4">
+        <v>43592</v>
+      </c>
+      <c r="N3" s="4">
+        <v>43592</v>
+      </c>
+      <c r="O3" s="27">
+        <v>43593</v>
+      </c>
+      <c r="P3" s="28">
+        <v>43593</v>
+      </c>
+      <c r="Q3" s="155">
+        <v>43593</v>
+      </c>
+      <c r="R3" s="27"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="27"/>
+      <c r="V3" s="28"/>
+      <c r="W3" s="29"/>
+      <c r="X3" s="27"/>
+      <c r="Y3" s="28"/>
+      <c r="Z3" s="29"/>
+      <c r="AA3" s="27"/>
+      <c r="AB3" s="28"/>
+      <c r="AC3" s="29"/>
+      <c r="AD3" s="27"/>
+      <c r="AE3" s="28"/>
+      <c r="AF3" s="29"/>
+      <c r="AG3" s="27"/>
+      <c r="AH3" s="28"/>
+      <c r="AI3" s="29"/>
+      <c r="AJ3" s="27"/>
+      <c r="AK3" s="28"/>
+      <c r="AL3" s="29"/>
+      <c r="AM3" s="27"/>
+      <c r="AN3" s="28"/>
+      <c r="AO3" s="29"/>
+      <c r="AP3" s="27"/>
+      <c r="AQ3" s="28"/>
+      <c r="AR3" s="29"/>
+      <c r="AS3" s="27"/>
+      <c r="AT3" s="28"/>
+      <c r="AU3" s="29"/>
+    </row>
+    <row r="4" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="7">
+        <v>44562</v>
+      </c>
+      <c r="C4" s="115">
+        <v>7.8</v>
+      </c>
+      <c r="D4" s="116">
+        <v>32.729999999999997</v>
+      </c>
+      <c r="E4" s="133">
+        <v>818.49</v>
+      </c>
+      <c r="F4" s="131">
+        <v>7.74</v>
+      </c>
+      <c r="G4" s="117">
+        <v>32.79</v>
+      </c>
+      <c r="H4" s="118">
+        <v>819.95</v>
+      </c>
+      <c r="I4" s="47">
+        <v>7.69</v>
+      </c>
+      <c r="J4" s="117">
+        <v>32.840000000000003</v>
+      </c>
+      <c r="K4" s="118">
+        <v>821.21</v>
+      </c>
+      <c r="L4" s="142">
+        <v>7.67</v>
+      </c>
+      <c r="M4" s="143">
+        <v>32.869999999999997</v>
+      </c>
+      <c r="N4" s="144">
+        <v>821.85</v>
+      </c>
+      <c r="O4" s="142">
+        <v>7.66</v>
+      </c>
+      <c r="P4" s="143">
+        <v>32.89</v>
+      </c>
+      <c r="Q4" s="144">
+        <v>822.3</v>
+      </c>
+      <c r="R4" s="21"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="21"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="21"/>
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="21"/>
+      <c r="AE4" s="12"/>
+      <c r="AF4" s="22"/>
+      <c r="AG4" s="21"/>
+      <c r="AH4" s="12"/>
+      <c r="AI4" s="22"/>
+      <c r="AJ4" s="21"/>
+      <c r="AK4" s="12"/>
+      <c r="AL4" s="22"/>
+      <c r="AM4" s="21"/>
+      <c r="AN4" s="12"/>
+      <c r="AO4" s="22"/>
+      <c r="AP4" s="21"/>
+      <c r="AQ4" s="12"/>
+      <c r="AR4" s="22"/>
+      <c r="AS4" s="21"/>
+      <c r="AT4" s="12"/>
+      <c r="AU4" s="22"/>
+    </row>
+    <row r="5" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="7">
+        <v>45658</v>
+      </c>
+      <c r="C5" s="119">
+        <v>8.76</v>
+      </c>
+      <c r="D5" s="66">
+        <v>31.08</v>
+      </c>
+      <c r="E5" s="134">
+        <v>621.77</v>
+      </c>
+      <c r="F5" s="57">
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="G5" s="58">
+        <v>31.16</v>
+      </c>
+      <c r="H5" s="120">
+        <v>623.27</v>
+      </c>
+      <c r="I5" s="21">
+        <v>8.67</v>
+      </c>
+      <c r="J5" s="58">
+        <v>31.25</v>
+      </c>
+      <c r="K5" s="120">
+        <v>625.1</v>
+      </c>
+      <c r="L5" s="145">
+        <v>8.65</v>
+      </c>
+      <c r="M5" s="141">
+        <v>31.29</v>
+      </c>
+      <c r="N5" s="146">
+        <v>625.95000000000005</v>
+      </c>
+      <c r="O5" s="145">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="P5" s="141">
+        <v>31.34</v>
+      </c>
+      <c r="Q5" s="146">
+        <v>626.80999999999995</v>
+      </c>
+      <c r="R5" s="21"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="21"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="22"/>
+      <c r="AA5" s="21"/>
+      <c r="AB5" s="12"/>
+      <c r="AC5" s="22"/>
+      <c r="AD5" s="21"/>
+      <c r="AE5" s="12"/>
+      <c r="AF5" s="22"/>
+      <c r="AG5" s="21"/>
+      <c r="AH5" s="12"/>
+      <c r="AI5" s="22"/>
+      <c r="AJ5" s="21"/>
+      <c r="AK5" s="12"/>
+      <c r="AL5" s="22"/>
+      <c r="AM5" s="21"/>
+      <c r="AN5" s="12"/>
+      <c r="AO5" s="22"/>
+      <c r="AP5" s="21"/>
+      <c r="AQ5" s="12"/>
+      <c r="AR5" s="22"/>
+      <c r="AS5" s="21"/>
+      <c r="AT5" s="12"/>
+      <c r="AU5" s="22"/>
+    </row>
+    <row r="6" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="9">
+        <v>47119</v>
+      </c>
+      <c r="C6" s="121">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="D6" s="122">
+        <v>32.93</v>
+      </c>
+      <c r="E6" s="135">
+        <v>1097.8</v>
+      </c>
+      <c r="F6" s="132">
+        <v>8.91</v>
+      </c>
+      <c r="G6" s="123">
+        <v>33.04</v>
+      </c>
+      <c r="H6" s="124">
+        <v>1101.3900000000001</v>
+      </c>
+      <c r="I6" s="16">
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="J6" s="123">
+        <v>33.130000000000003</v>
+      </c>
+      <c r="K6" s="124">
+        <v>1104.3399999999999</v>
+      </c>
+      <c r="L6" s="147">
+        <v>8.83</v>
+      </c>
+      <c r="M6" s="148">
+        <v>33.21</v>
+      </c>
+      <c r="N6" s="149">
+        <v>1107.3</v>
+      </c>
+      <c r="O6" s="147">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="P6" s="148">
+        <v>33.28</v>
+      </c>
+      <c r="Q6" s="149">
+        <v>1109.6199999999999</v>
+      </c>
+      <c r="R6" s="16"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="18"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="18"/>
+      <c r="AD6" s="16"/>
+      <c r="AE6" s="17"/>
+      <c r="AF6" s="18"/>
+      <c r="AG6" s="16"/>
+      <c r="AH6" s="17"/>
+      <c r="AI6" s="18"/>
+      <c r="AJ6" s="16"/>
+      <c r="AK6" s="17"/>
+      <c r="AL6" s="18"/>
+      <c r="AM6" s="16"/>
+      <c r="AN6" s="17"/>
+      <c r="AO6" s="18"/>
+      <c r="AP6" s="16"/>
+      <c r="AQ6" s="17"/>
+      <c r="AR6" s="18"/>
+      <c r="AS6" s="16"/>
+      <c r="AT6" s="17"/>
+      <c r="AU6" s="18"/>
+    </row>
+    <row r="7" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:AU1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AU100"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="O3" sqref="O3:Q4"/>
     </sheetView>
   </sheetViews>
@@ -46351,55 +46960,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="173"/>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
-      <c r="I1" s="173"/>
-      <c r="J1" s="173"/>
-      <c r="K1" s="173"/>
-      <c r="L1" s="173"/>
-      <c r="M1" s="173"/>
-      <c r="N1" s="173"/>
-      <c r="O1" s="173"/>
-      <c r="P1" s="173"/>
-      <c r="Q1" s="173"/>
-      <c r="R1" s="173"/>
-      <c r="S1" s="173"/>
-      <c r="T1" s="173"/>
-      <c r="U1" s="173"/>
-      <c r="V1" s="173"/>
-      <c r="W1" s="173"/>
-      <c r="X1" s="173"/>
-      <c r="Y1" s="173"/>
-      <c r="Z1" s="173"/>
-      <c r="AA1" s="173"/>
-      <c r="AB1" s="173"/>
-      <c r="AC1" s="173"/>
-      <c r="AD1" s="173"/>
-      <c r="AE1" s="173"/>
-      <c r="AF1" s="173"/>
-      <c r="AG1" s="173"/>
-      <c r="AH1" s="173"/>
-      <c r="AI1" s="173"/>
-      <c r="AJ1" s="173"/>
-      <c r="AK1" s="173"/>
-      <c r="AL1" s="173"/>
-      <c r="AM1" s="173"/>
-      <c r="AN1" s="173"/>
-      <c r="AO1" s="173"/>
-      <c r="AP1" s="173"/>
-      <c r="AQ1" s="173"/>
-      <c r="AR1" s="173"/>
-      <c r="AS1" s="173"/>
-      <c r="AT1" s="173"/>
-      <c r="AU1" s="174"/>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
+      <c r="H1" s="174"/>
+      <c r="I1" s="174"/>
+      <c r="J1" s="174"/>
+      <c r="K1" s="174"/>
+      <c r="L1" s="174"/>
+      <c r="M1" s="174"/>
+      <c r="N1" s="174"/>
+      <c r="O1" s="174"/>
+      <c r="P1" s="174"/>
+      <c r="Q1" s="174"/>
+      <c r="R1" s="174"/>
+      <c r="S1" s="174"/>
+      <c r="T1" s="174"/>
+      <c r="U1" s="174"/>
+      <c r="V1" s="174"/>
+      <c r="W1" s="174"/>
+      <c r="X1" s="174"/>
+      <c r="Y1" s="174"/>
+      <c r="Z1" s="174"/>
+      <c r="AA1" s="174"/>
+      <c r="AB1" s="174"/>
+      <c r="AC1" s="174"/>
+      <c r="AD1" s="174"/>
+      <c r="AE1" s="174"/>
+      <c r="AF1" s="174"/>
+      <c r="AG1" s="174"/>
+      <c r="AH1" s="174"/>
+      <c r="AI1" s="174"/>
+      <c r="AJ1" s="174"/>
+      <c r="AK1" s="174"/>
+      <c r="AL1" s="174"/>
+      <c r="AM1" s="174"/>
+      <c r="AN1" s="174"/>
+      <c r="AO1" s="174"/>
+      <c r="AP1" s="174"/>
+      <c r="AQ1" s="174"/>
+      <c r="AR1" s="174"/>
+      <c r="AS1" s="174"/>
+      <c r="AT1" s="174"/>
+      <c r="AU1" s="175"/>
     </row>
     <row r="2" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
@@ -46865,13 +47474,13 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="161" t="s">
+      <c r="A2" s="162" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="162"/>
-      <c r="C2" s="162"/>
-      <c r="D2" s="162"/>
-      <c r="E2" s="163"/>
+      <c r="B2" s="163"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="164"/>
       <c r="F2" s="52"/>
       <c r="G2" s="52"/>
       <c r="H2" s="52"/>
@@ -47012,13 +47621,13 @@
       <c r="I8" s="52"/>
     </row>
     <row r="9" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="164" t="s">
+      <c r="A9" s="165" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="165"/>
-      <c r="C9" s="165"/>
-      <c r="D9" s="165"/>
-      <c r="E9" s="166"/>
+      <c r="B9" s="166"/>
+      <c r="C9" s="166"/>
+      <c r="D9" s="166"/>
+      <c r="E9" s="167"/>
       <c r="F9" s="52"/>
       <c r="G9" s="52"/>
       <c r="H9" s="52"/>
@@ -47088,13 +47697,13 @@
       <c r="I12" s="52"/>
     </row>
     <row r="13" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="161" t="s">
+      <c r="A13" s="162" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="162"/>
-      <c r="C13" s="162"/>
-      <c r="D13" s="162"/>
-      <c r="E13" s="163"/>
+      <c r="B13" s="163"/>
+      <c r="C13" s="163"/>
+      <c r="D13" s="163"/>
+      <c r="E13" s="164"/>
       <c r="F13" s="52"/>
       <c r="G13" s="52"/>
       <c r="H13" s="52"/>
@@ -47183,13 +47792,13 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="167" t="s">
+      <c r="A2" s="168" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="168"/>
-      <c r="C2" s="168"/>
-      <c r="D2" s="168"/>
-      <c r="E2" s="168"/>
+      <c r="B2" s="169"/>
+      <c r="C2" s="169"/>
+      <c r="D2" s="169"/>
+      <c r="E2" s="169"/>
       <c r="F2" s="52"/>
       <c r="G2" s="52"/>
       <c r="H2" s="52"/>
@@ -47330,13 +47939,13 @@
       <c r="I8" s="52"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="169" t="s">
+      <c r="A9" s="170" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="170"/>
-      <c r="C9" s="170"/>
-      <c r="D9" s="170"/>
-      <c r="E9" s="170"/>
+      <c r="B9" s="171"/>
+      <c r="C9" s="171"/>
+      <c r="D9" s="171"/>
+      <c r="E9" s="171"/>
       <c r="F9" s="52"/>
       <c r="G9" s="52"/>
       <c r="H9" s="52"/>
@@ -47406,13 +48015,13 @@
       <c r="I12" s="52"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="169" t="s">
+      <c r="A13" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="170"/>
-      <c r="C13" s="170"/>
-      <c r="D13" s="170"/>
-      <c r="E13" s="170"/>
+      <c r="B13" s="171"/>
+      <c r="C13" s="171"/>
+      <c r="D13" s="171"/>
+      <c r="E13" s="171"/>
       <c r="F13" s="52"/>
       <c r="G13" s="52"/>
       <c r="H13" s="52"/>
@@ -47484,13 +48093,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="171"/>
-      <c r="C2" s="171"/>
-      <c r="D2" s="171"/>
-      <c r="E2" s="171"/>
+      <c r="B2" s="172"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="172"/>
+      <c r="E2" s="172"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="138" t="s">
@@ -47595,13 +48204,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="171" t="s">
+      <c r="A9" s="172" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="171"/>
-      <c r="C9" s="171"/>
-      <c r="D9" s="171"/>
-      <c r="E9" s="171"/>
+      <c r="B9" s="172"/>
+      <c r="C9" s="172"/>
+      <c r="D9" s="172"/>
+      <c r="E9" s="172"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="138" t="s">
@@ -47655,13 +48264,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="171" t="s">
+      <c r="A13" s="172" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="171"/>
-      <c r="C13" s="171"/>
-      <c r="D13" s="171"/>
-      <c r="E13" s="171"/>
+      <c r="B13" s="172"/>
+      <c r="C13" s="172"/>
+      <c r="D13" s="172"/>
+      <c r="E13" s="172"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="138" t="s">
@@ -47726,13 +48335,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="171"/>
-      <c r="C2" s="171"/>
-      <c r="D2" s="171"/>
-      <c r="E2" s="171"/>
+      <c r="B2" s="172"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="172"/>
+      <c r="E2" s="172"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="138" t="s">
@@ -47837,13 +48446,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="171" t="s">
+      <c r="A9" s="172" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="171"/>
-      <c r="C9" s="171"/>
-      <c r="D9" s="171"/>
-      <c r="E9" s="171"/>
+      <c r="B9" s="172"/>
+      <c r="C9" s="172"/>
+      <c r="D9" s="172"/>
+      <c r="E9" s="172"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="138" t="s">
@@ -47897,13 +48506,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="171" t="s">
+      <c r="A13" s="172" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="171"/>
-      <c r="C13" s="171"/>
-      <c r="D13" s="171"/>
-      <c r="E13" s="171"/>
+      <c r="B13" s="172"/>
+      <c r="C13" s="172"/>
+      <c r="D13" s="172"/>
+      <c r="E13" s="172"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="138" t="s">
@@ -47934,6 +48543,232 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40" style="179" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="179" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" style="179" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="179" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="179" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="179"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="137" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="137" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="137" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="137" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="137" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="172" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="172"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="172"/>
+      <c r="E2" s="172"/>
+    </row>
+    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="138" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="139">
+        <v>45519</v>
+      </c>
+      <c r="C3" s="140">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="D3" s="141">
+        <v>52.4</v>
+      </c>
+      <c r="E3" s="141">
+        <v>2620.09</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="138" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="139">
+        <v>49444</v>
+      </c>
+      <c r="C4" s="140">
+        <v>4.37</v>
+      </c>
+      <c r="D4" s="141">
+        <v>32.56</v>
+      </c>
+      <c r="E4" s="141">
+        <v>1628.17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="138" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="139">
+        <v>53097</v>
+      </c>
+      <c r="C5" s="140">
+        <v>4.37</v>
+      </c>
+      <c r="D5" s="141">
+        <v>31.88</v>
+      </c>
+      <c r="E5" s="141">
+        <v>1062.81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="138" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="139">
+        <v>46249</v>
+      </c>
+      <c r="C6" s="140">
+        <v>4.07</v>
+      </c>
+      <c r="D6" s="141">
+        <v>36.47</v>
+      </c>
+      <c r="E6" s="141">
+        <v>3647.11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="138" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="139">
+        <v>55015</v>
+      </c>
+      <c r="C7" s="140">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D7" s="141">
+        <v>41.29</v>
+      </c>
+      <c r="E7" s="141">
+        <v>4129.3100000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="172" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="172"/>
+      <c r="C8" s="172"/>
+      <c r="D8" s="172"/>
+      <c r="E8" s="172"/>
+    </row>
+    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="138" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="139">
+        <v>44562</v>
+      </c>
+      <c r="C9" s="140">
+        <v>7.62</v>
+      </c>
+      <c r="D9" s="141">
+        <v>32.93</v>
+      </c>
+      <c r="E9" s="141">
+        <v>823.35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="138" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="139">
+        <v>45658</v>
+      </c>
+      <c r="C10" s="140">
+        <v>8.6</v>
+      </c>
+      <c r="D10" s="141">
+        <v>31.39</v>
+      </c>
+      <c r="E10" s="141">
+        <v>627.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="138" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="139">
+        <v>47119</v>
+      </c>
+      <c r="C11" s="140">
+        <v>8.7899999999999991</v>
+      </c>
+      <c r="D11" s="141">
+        <v>33.31</v>
+      </c>
+      <c r="E11" s="141">
+        <v>1110.6400000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="172" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="172"/>
+      <c r="C12" s="172"/>
+      <c r="D12" s="172"/>
+      <c r="E12" s="172"/>
+    </row>
+    <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="138" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="139">
+        <v>45717</v>
+      </c>
+      <c r="C13" s="140">
+        <v>0.02</v>
+      </c>
+      <c r="D13" s="141">
+        <v>100.87</v>
+      </c>
+      <c r="E13" s="141">
+        <v>10087.620000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A12:E12"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -47996,55 +48831,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="173" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="173"/>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
-      <c r="I1" s="173"/>
-      <c r="J1" s="173"/>
-      <c r="K1" s="173"/>
-      <c r="L1" s="173"/>
-      <c r="M1" s="173"/>
-      <c r="N1" s="173"/>
-      <c r="O1" s="173"/>
-      <c r="P1" s="173"/>
-      <c r="Q1" s="173"/>
-      <c r="R1" s="173"/>
-      <c r="S1" s="173"/>
-      <c r="T1" s="173"/>
-      <c r="U1" s="173"/>
-      <c r="V1" s="173"/>
-      <c r="W1" s="173"/>
-      <c r="X1" s="173"/>
-      <c r="Y1" s="173"/>
-      <c r="Z1" s="173"/>
-      <c r="AA1" s="173"/>
-      <c r="AB1" s="173"/>
-      <c r="AC1" s="173"/>
-      <c r="AD1" s="173"/>
-      <c r="AE1" s="173"/>
-      <c r="AF1" s="173"/>
-      <c r="AG1" s="173"/>
-      <c r="AH1" s="173"/>
-      <c r="AI1" s="173"/>
-      <c r="AJ1" s="173"/>
-      <c r="AK1" s="173"/>
-      <c r="AL1" s="173"/>
-      <c r="AM1" s="173"/>
-      <c r="AN1" s="173"/>
-      <c r="AO1" s="173"/>
-      <c r="AP1" s="173"/>
-      <c r="AQ1" s="173"/>
-      <c r="AR1" s="173"/>
-      <c r="AS1" s="173"/>
-      <c r="AT1" s="173"/>
-      <c r="AU1" s="174"/>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
+      <c r="H1" s="174"/>
+      <c r="I1" s="174"/>
+      <c r="J1" s="174"/>
+      <c r="K1" s="174"/>
+      <c r="L1" s="174"/>
+      <c r="M1" s="174"/>
+      <c r="N1" s="174"/>
+      <c r="O1" s="174"/>
+      <c r="P1" s="174"/>
+      <c r="Q1" s="174"/>
+      <c r="R1" s="174"/>
+      <c r="S1" s="174"/>
+      <c r="T1" s="174"/>
+      <c r="U1" s="174"/>
+      <c r="V1" s="174"/>
+      <c r="W1" s="174"/>
+      <c r="X1" s="174"/>
+      <c r="Y1" s="174"/>
+      <c r="Z1" s="174"/>
+      <c r="AA1" s="174"/>
+      <c r="AB1" s="174"/>
+      <c r="AC1" s="174"/>
+      <c r="AD1" s="174"/>
+      <c r="AE1" s="174"/>
+      <c r="AF1" s="174"/>
+      <c r="AG1" s="174"/>
+      <c r="AH1" s="174"/>
+      <c r="AI1" s="174"/>
+      <c r="AJ1" s="174"/>
+      <c r="AK1" s="174"/>
+      <c r="AL1" s="174"/>
+      <c r="AM1" s="174"/>
+      <c r="AN1" s="174"/>
+      <c r="AO1" s="174"/>
+      <c r="AP1" s="174"/>
+      <c r="AQ1" s="174"/>
+      <c r="AR1" s="174"/>
+      <c r="AS1" s="174"/>
+      <c r="AT1" s="174"/>
+      <c r="AU1" s="175"/>
     </row>
     <row r="2" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="129" t="s">
@@ -48769,55 +49604,55 @@
       <c r="AU9" s="18"/>
     </row>
     <row r="10" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="175" t="s">
+      <c r="A10" s="176" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="176"/>
-      <c r="C10" s="176"/>
-      <c r="D10" s="176"/>
-      <c r="E10" s="176"/>
-      <c r="F10" s="176"/>
-      <c r="G10" s="176"/>
-      <c r="H10" s="176"/>
-      <c r="I10" s="176"/>
-      <c r="J10" s="176"/>
-      <c r="K10" s="176"/>
-      <c r="L10" s="176"/>
-      <c r="M10" s="176"/>
-      <c r="N10" s="176"/>
-      <c r="O10" s="176"/>
-      <c r="P10" s="176"/>
-      <c r="Q10" s="176"/>
-      <c r="R10" s="176"/>
-      <c r="S10" s="176"/>
-      <c r="T10" s="176"/>
-      <c r="U10" s="176"/>
-      <c r="V10" s="176"/>
-      <c r="W10" s="176"/>
-      <c r="X10" s="176"/>
-      <c r="Y10" s="176"/>
-      <c r="Z10" s="176"/>
-      <c r="AA10" s="176"/>
-      <c r="AB10" s="176"/>
-      <c r="AC10" s="176"/>
-      <c r="AD10" s="176"/>
-      <c r="AE10" s="176"/>
-      <c r="AF10" s="176"/>
-      <c r="AG10" s="176"/>
-      <c r="AH10" s="176"/>
-      <c r="AI10" s="176"/>
-      <c r="AJ10" s="176"/>
-      <c r="AK10" s="176"/>
-      <c r="AL10" s="176"/>
-      <c r="AM10" s="176"/>
-      <c r="AN10" s="176"/>
-      <c r="AO10" s="176"/>
-      <c r="AP10" s="176"/>
-      <c r="AQ10" s="176"/>
-      <c r="AR10" s="176"/>
-      <c r="AS10" s="176"/>
-      <c r="AT10" s="176"/>
-      <c r="AU10" s="176"/>
+      <c r="B10" s="177"/>
+      <c r="C10" s="177"/>
+      <c r="D10" s="177"/>
+      <c r="E10" s="177"/>
+      <c r="F10" s="177"/>
+      <c r="G10" s="177"/>
+      <c r="H10" s="177"/>
+      <c r="I10" s="177"/>
+      <c r="J10" s="177"/>
+      <c r="K10" s="177"/>
+      <c r="L10" s="177"/>
+      <c r="M10" s="177"/>
+      <c r="N10" s="177"/>
+      <c r="O10" s="177"/>
+      <c r="P10" s="177"/>
+      <c r="Q10" s="177"/>
+      <c r="R10" s="177"/>
+      <c r="S10" s="177"/>
+      <c r="T10" s="177"/>
+      <c r="U10" s="177"/>
+      <c r="V10" s="177"/>
+      <c r="W10" s="177"/>
+      <c r="X10" s="177"/>
+      <c r="Y10" s="177"/>
+      <c r="Z10" s="177"/>
+      <c r="AA10" s="177"/>
+      <c r="AB10" s="177"/>
+      <c r="AC10" s="177"/>
+      <c r="AD10" s="177"/>
+      <c r="AE10" s="177"/>
+      <c r="AF10" s="177"/>
+      <c r="AG10" s="177"/>
+      <c r="AH10" s="177"/>
+      <c r="AI10" s="177"/>
+      <c r="AJ10" s="177"/>
+      <c r="AK10" s="177"/>
+      <c r="AL10" s="177"/>
+      <c r="AM10" s="177"/>
+      <c r="AN10" s="177"/>
+      <c r="AO10" s="177"/>
+      <c r="AP10" s="177"/>
+      <c r="AQ10" s="177"/>
+      <c r="AR10" s="177"/>
+      <c r="AS10" s="177"/>
+      <c r="AT10" s="177"/>
+      <c r="AU10" s="177"/>
     </row>
     <row r="11" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
@@ -49009,7 +49844,7 @@
       <c r="P12" s="28">
         <v>43593</v>
       </c>
-      <c r="Q12" s="178">
+      <c r="Q12" s="155">
         <v>43593</v>
       </c>
       <c r="R12" s="27"/>
@@ -49293,55 +50128,55 @@
       <c r="AU15" s="18"/>
     </row>
     <row r="16" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="175" t="s">
+      <c r="A16" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="176"/>
-      <c r="C16" s="176"/>
-      <c r="D16" s="176"/>
-      <c r="E16" s="176"/>
-      <c r="F16" s="176"/>
-      <c r="G16" s="176"/>
-      <c r="H16" s="176"/>
-      <c r="I16" s="176"/>
-      <c r="J16" s="176"/>
-      <c r="K16" s="176"/>
-      <c r="L16" s="176"/>
-      <c r="M16" s="176"/>
-      <c r="N16" s="176"/>
-      <c r="O16" s="176"/>
-      <c r="P16" s="176"/>
-      <c r="Q16" s="176"/>
-      <c r="R16" s="176"/>
-      <c r="S16" s="176"/>
-      <c r="T16" s="176"/>
-      <c r="U16" s="176"/>
-      <c r="V16" s="176"/>
-      <c r="W16" s="176"/>
-      <c r="X16" s="176"/>
-      <c r="Y16" s="176"/>
-      <c r="Z16" s="176"/>
-      <c r="AA16" s="176"/>
-      <c r="AB16" s="176"/>
-      <c r="AC16" s="176"/>
-      <c r="AD16" s="176"/>
-      <c r="AE16" s="176"/>
-      <c r="AF16" s="176"/>
-      <c r="AG16" s="176"/>
-      <c r="AH16" s="176"/>
-      <c r="AI16" s="176"/>
-      <c r="AJ16" s="176"/>
-      <c r="AK16" s="176"/>
-      <c r="AL16" s="176"/>
-      <c r="AM16" s="176"/>
-      <c r="AN16" s="176"/>
-      <c r="AO16" s="176"/>
-      <c r="AP16" s="176"/>
-      <c r="AQ16" s="176"/>
-      <c r="AR16" s="176"/>
-      <c r="AS16" s="176"/>
-      <c r="AT16" s="176"/>
-      <c r="AU16" s="176"/>
+      <c r="B16" s="177"/>
+      <c r="C16" s="177"/>
+      <c r="D16" s="177"/>
+      <c r="E16" s="177"/>
+      <c r="F16" s="177"/>
+      <c r="G16" s="177"/>
+      <c r="H16" s="177"/>
+      <c r="I16" s="177"/>
+      <c r="J16" s="177"/>
+      <c r="K16" s="177"/>
+      <c r="L16" s="177"/>
+      <c r="M16" s="177"/>
+      <c r="N16" s="177"/>
+      <c r="O16" s="177"/>
+      <c r="P16" s="177"/>
+      <c r="Q16" s="177"/>
+      <c r="R16" s="177"/>
+      <c r="S16" s="177"/>
+      <c r="T16" s="177"/>
+      <c r="U16" s="177"/>
+      <c r="V16" s="177"/>
+      <c r="W16" s="177"/>
+      <c r="X16" s="177"/>
+      <c r="Y16" s="177"/>
+      <c r="Z16" s="177"/>
+      <c r="AA16" s="177"/>
+      <c r="AB16" s="177"/>
+      <c r="AC16" s="177"/>
+      <c r="AD16" s="177"/>
+      <c r="AE16" s="177"/>
+      <c r="AF16" s="177"/>
+      <c r="AG16" s="177"/>
+      <c r="AH16" s="177"/>
+      <c r="AI16" s="177"/>
+      <c r="AJ16" s="177"/>
+      <c r="AK16" s="177"/>
+      <c r="AL16" s="177"/>
+      <c r="AM16" s="177"/>
+      <c r="AN16" s="177"/>
+      <c r="AO16" s="177"/>
+      <c r="AP16" s="177"/>
+      <c r="AQ16" s="177"/>
+      <c r="AR16" s="177"/>
+      <c r="AS16" s="177"/>
+      <c r="AT16" s="177"/>
+      <c r="AU16" s="177"/>
     </row>
     <row r="17" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
@@ -49743,7 +50578,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>
@@ -49797,55 +50632,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="176" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="176"/>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="176"/>
-      <c r="H1" s="176"/>
-      <c r="I1" s="176"/>
-      <c r="J1" s="176"/>
-      <c r="K1" s="176"/>
-      <c r="L1" s="176"/>
-      <c r="M1" s="176"/>
-      <c r="N1" s="176"/>
-      <c r="O1" s="176"/>
-      <c r="P1" s="176"/>
-      <c r="Q1" s="176"/>
-      <c r="R1" s="176"/>
-      <c r="S1" s="176"/>
-      <c r="T1" s="176"/>
-      <c r="U1" s="176"/>
-      <c r="V1" s="176"/>
-      <c r="W1" s="176"/>
-      <c r="X1" s="176"/>
-      <c r="Y1" s="176"/>
-      <c r="Z1" s="176"/>
-      <c r="AA1" s="176"/>
-      <c r="AB1" s="176"/>
-      <c r="AC1" s="176"/>
-      <c r="AD1" s="176"/>
-      <c r="AE1" s="176"/>
-      <c r="AF1" s="176"/>
-      <c r="AG1" s="176"/>
-      <c r="AH1" s="176"/>
-      <c r="AI1" s="176"/>
-      <c r="AJ1" s="176"/>
-      <c r="AK1" s="176"/>
-      <c r="AL1" s="176"/>
-      <c r="AM1" s="176"/>
-      <c r="AN1" s="176"/>
-      <c r="AO1" s="176"/>
-      <c r="AP1" s="176"/>
-      <c r="AQ1" s="176"/>
-      <c r="AR1" s="176"/>
-      <c r="AS1" s="176"/>
-      <c r="AT1" s="176"/>
-      <c r="AU1" s="176"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
+      <c r="P1" s="177"/>
+      <c r="Q1" s="177"/>
+      <c r="R1" s="177"/>
+      <c r="S1" s="177"/>
+      <c r="T1" s="177"/>
+      <c r="U1" s="177"/>
+      <c r="V1" s="177"/>
+      <c r="W1" s="177"/>
+      <c r="X1" s="177"/>
+      <c r="Y1" s="177"/>
+      <c r="Z1" s="177"/>
+      <c r="AA1" s="177"/>
+      <c r="AB1" s="177"/>
+      <c r="AC1" s="177"/>
+      <c r="AD1" s="177"/>
+      <c r="AE1" s="177"/>
+      <c r="AF1" s="177"/>
+      <c r="AG1" s="177"/>
+      <c r="AH1" s="177"/>
+      <c r="AI1" s="177"/>
+      <c r="AJ1" s="177"/>
+      <c r="AK1" s="177"/>
+      <c r="AL1" s="177"/>
+      <c r="AM1" s="177"/>
+      <c r="AN1" s="177"/>
+      <c r="AO1" s="177"/>
+      <c r="AP1" s="177"/>
+      <c r="AQ1" s="177"/>
+      <c r="AR1" s="177"/>
+      <c r="AS1" s="177"/>
+      <c r="AT1" s="177"/>
+      <c r="AU1" s="177"/>
     </row>
     <row r="2" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
@@ -50424,7 +51259,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>
@@ -50454,55 +51289,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="177"/>
-      <c r="E1" s="177"/>
-      <c r="F1" s="177"/>
-      <c r="G1" s="177"/>
-      <c r="H1" s="177"/>
-      <c r="I1" s="177"/>
-      <c r="J1" s="177"/>
-      <c r="K1" s="177"/>
-      <c r="L1" s="177"/>
-      <c r="M1" s="177"/>
-      <c r="N1" s="177"/>
-      <c r="O1" s="177"/>
-      <c r="P1" s="177"/>
-      <c r="Q1" s="177"/>
-      <c r="R1" s="177"/>
-      <c r="S1" s="177"/>
-      <c r="T1" s="177"/>
-      <c r="U1" s="177"/>
-      <c r="V1" s="177"/>
-      <c r="W1" s="177"/>
-      <c r="X1" s="177"/>
-      <c r="Y1" s="177"/>
-      <c r="Z1" s="177"/>
-      <c r="AA1" s="177"/>
-      <c r="AB1" s="177"/>
-      <c r="AC1" s="177"/>
-      <c r="AD1" s="177"/>
-      <c r="AE1" s="177"/>
-      <c r="AF1" s="177"/>
-      <c r="AG1" s="177"/>
-      <c r="AH1" s="177"/>
-      <c r="AI1" s="177"/>
-      <c r="AJ1" s="177"/>
-      <c r="AK1" s="177"/>
-      <c r="AL1" s="177"/>
-      <c r="AM1" s="177"/>
-      <c r="AN1" s="177"/>
-      <c r="AO1" s="177"/>
-      <c r="AP1" s="177"/>
-      <c r="AQ1" s="177"/>
-      <c r="AR1" s="177"/>
-      <c r="AS1" s="177"/>
-      <c r="AT1" s="177"/>
-      <c r="AU1" s="177"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+      <c r="H1" s="178"/>
+      <c r="I1" s="178"/>
+      <c r="J1" s="178"/>
+      <c r="K1" s="178"/>
+      <c r="L1" s="178"/>
+      <c r="M1" s="178"/>
+      <c r="N1" s="178"/>
+      <c r="O1" s="178"/>
+      <c r="P1" s="178"/>
+      <c r="Q1" s="178"/>
+      <c r="R1" s="178"/>
+      <c r="S1" s="178"/>
+      <c r="T1" s="178"/>
+      <c r="U1" s="178"/>
+      <c r="V1" s="178"/>
+      <c r="W1" s="178"/>
+      <c r="X1" s="178"/>
+      <c r="Y1" s="178"/>
+      <c r="Z1" s="178"/>
+      <c r="AA1" s="178"/>
+      <c r="AB1" s="178"/>
+      <c r="AC1" s="178"/>
+      <c r="AD1" s="178"/>
+      <c r="AE1" s="178"/>
+      <c r="AF1" s="178"/>
+      <c r="AG1" s="178"/>
+      <c r="AH1" s="178"/>
+      <c r="AI1" s="178"/>
+      <c r="AJ1" s="178"/>
+      <c r="AK1" s="178"/>
+      <c r="AL1" s="178"/>
+      <c r="AM1" s="178"/>
+      <c r="AN1" s="178"/>
+      <c r="AO1" s="178"/>
+      <c r="AP1" s="178"/>
+      <c r="AQ1" s="178"/>
+      <c r="AR1" s="178"/>
+      <c r="AS1" s="178"/>
+      <c r="AT1" s="178"/>
+      <c r="AU1" s="178"/>
     </row>
     <row r="2" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -51079,661 +51914,4 @@
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU100"/>
-  <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:Q6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="28.85546875" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" customWidth="1"/>
-    <col min="12" max="12" width="28.85546875" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" customWidth="1"/>
-    <col min="15" max="15" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="177" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="177"/>
-      <c r="E1" s="177"/>
-      <c r="F1" s="177"/>
-      <c r="G1" s="177"/>
-      <c r="H1" s="177"/>
-      <c r="I1" s="177"/>
-      <c r="J1" s="177"/>
-      <c r="K1" s="177"/>
-      <c r="L1" s="177"/>
-      <c r="M1" s="177"/>
-      <c r="N1" s="177"/>
-      <c r="O1" s="177"/>
-      <c r="P1" s="177"/>
-      <c r="Q1" s="177"/>
-      <c r="R1" s="177"/>
-      <c r="S1" s="177"/>
-      <c r="T1" s="177"/>
-      <c r="U1" s="177"/>
-      <c r="V1" s="177"/>
-      <c r="W1" s="177"/>
-      <c r="X1" s="177"/>
-      <c r="Y1" s="177"/>
-      <c r="Z1" s="177"/>
-      <c r="AA1" s="177"/>
-      <c r="AB1" s="177"/>
-      <c r="AC1" s="177"/>
-      <c r="AD1" s="177"/>
-      <c r="AE1" s="177"/>
-      <c r="AF1" s="177"/>
-      <c r="AG1" s="177"/>
-      <c r="AH1" s="177"/>
-      <c r="AI1" s="177"/>
-      <c r="AJ1" s="177"/>
-      <c r="AK1" s="177"/>
-      <c r="AL1" s="177"/>
-      <c r="AM1" s="177"/>
-      <c r="AN1" s="177"/>
-      <c r="AO1" s="177"/>
-      <c r="AP1" s="177"/>
-      <c r="AQ1" s="177"/>
-      <c r="AR1" s="177"/>
-      <c r="AS1" s="177"/>
-      <c r="AT1" s="177"/>
-      <c r="AU1" s="177"/>
-    </row>
-    <row r="2" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="P2" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q2" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="R2" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="S2" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="T2" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="U2" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="V2" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="W2" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="X2" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y2" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z2" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA2" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB2" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC2" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD2" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE2" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="AF2" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG2" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="AI2" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ2" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK2" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL2" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="AM2" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="AN2" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="AO2" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="AP2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="AQ2" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="AR2" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="AS2" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT2" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="AU2" s="26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="4">
-        <v>43587</v>
-      </c>
-      <c r="D3" s="4">
-        <v>43587</v>
-      </c>
-      <c r="E3" s="5">
-        <v>43587</v>
-      </c>
-      <c r="F3" s="3">
-        <v>43588</v>
-      </c>
-      <c r="G3" s="4">
-        <v>43588</v>
-      </c>
-      <c r="H3" s="5">
-        <v>43588</v>
-      </c>
-      <c r="I3" s="109">
-        <v>43591</v>
-      </c>
-      <c r="J3" s="109">
-        <v>43591</v>
-      </c>
-      <c r="K3" s="109">
-        <v>43591</v>
-      </c>
-      <c r="L3" s="3">
-        <v>43592</v>
-      </c>
-      <c r="M3" s="4">
-        <v>43592</v>
-      </c>
-      <c r="N3" s="4">
-        <v>43592</v>
-      </c>
-      <c r="O3" s="27">
-        <v>43593</v>
-      </c>
-      <c r="P3" s="28">
-        <v>43593</v>
-      </c>
-      <c r="Q3" s="178">
-        <v>43593</v>
-      </c>
-      <c r="R3" s="27"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="27"/>
-      <c r="V3" s="28"/>
-      <c r="W3" s="29"/>
-      <c r="X3" s="27"/>
-      <c r="Y3" s="28"/>
-      <c r="Z3" s="29"/>
-      <c r="AA3" s="27"/>
-      <c r="AB3" s="28"/>
-      <c r="AC3" s="29"/>
-      <c r="AD3" s="27"/>
-      <c r="AE3" s="28"/>
-      <c r="AF3" s="29"/>
-      <c r="AG3" s="27"/>
-      <c r="AH3" s="28"/>
-      <c r="AI3" s="29"/>
-      <c r="AJ3" s="27"/>
-      <c r="AK3" s="28"/>
-      <c r="AL3" s="29"/>
-      <c r="AM3" s="27"/>
-      <c r="AN3" s="28"/>
-      <c r="AO3" s="29"/>
-      <c r="AP3" s="27"/>
-      <c r="AQ3" s="28"/>
-      <c r="AR3" s="29"/>
-      <c r="AS3" s="27"/>
-      <c r="AT3" s="28"/>
-      <c r="AU3" s="29"/>
-    </row>
-    <row r="4" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="7">
-        <v>44562</v>
-      </c>
-      <c r="C4" s="115">
-        <v>7.8</v>
-      </c>
-      <c r="D4" s="116">
-        <v>32.729999999999997</v>
-      </c>
-      <c r="E4" s="133">
-        <v>818.49</v>
-      </c>
-      <c r="F4" s="131">
-        <v>7.74</v>
-      </c>
-      <c r="G4" s="117">
-        <v>32.79</v>
-      </c>
-      <c r="H4" s="118">
-        <v>819.95</v>
-      </c>
-      <c r="I4" s="47">
-        <v>7.69</v>
-      </c>
-      <c r="J4" s="117">
-        <v>32.840000000000003</v>
-      </c>
-      <c r="K4" s="118">
-        <v>821.21</v>
-      </c>
-      <c r="L4" s="142">
-        <v>7.67</v>
-      </c>
-      <c r="M4" s="143">
-        <v>32.869999999999997</v>
-      </c>
-      <c r="N4" s="144">
-        <v>821.85</v>
-      </c>
-      <c r="O4" s="142">
-        <v>7.66</v>
-      </c>
-      <c r="P4" s="143">
-        <v>32.89</v>
-      </c>
-      <c r="Q4" s="144">
-        <v>822.3</v>
-      </c>
-      <c r="R4" s="21"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="22"/>
-      <c r="X4" s="21"/>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="21"/>
-      <c r="AB4" s="12"/>
-      <c r="AC4" s="22"/>
-      <c r="AD4" s="21"/>
-      <c r="AE4" s="12"/>
-      <c r="AF4" s="22"/>
-      <c r="AG4" s="21"/>
-      <c r="AH4" s="12"/>
-      <c r="AI4" s="22"/>
-      <c r="AJ4" s="21"/>
-      <c r="AK4" s="12"/>
-      <c r="AL4" s="22"/>
-      <c r="AM4" s="21"/>
-      <c r="AN4" s="12"/>
-      <c r="AO4" s="22"/>
-      <c r="AP4" s="21"/>
-      <c r="AQ4" s="12"/>
-      <c r="AR4" s="22"/>
-      <c r="AS4" s="21"/>
-      <c r="AT4" s="12"/>
-      <c r="AU4" s="22"/>
-    </row>
-    <row r="5" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="7">
-        <v>45658</v>
-      </c>
-      <c r="C5" s="119">
-        <v>8.76</v>
-      </c>
-      <c r="D5" s="66">
-        <v>31.08</v>
-      </c>
-      <c r="E5" s="134">
-        <v>621.77</v>
-      </c>
-      <c r="F5" s="57">
-        <v>8.7200000000000006</v>
-      </c>
-      <c r="G5" s="58">
-        <v>31.16</v>
-      </c>
-      <c r="H5" s="120">
-        <v>623.27</v>
-      </c>
-      <c r="I5" s="21">
-        <v>8.67</v>
-      </c>
-      <c r="J5" s="58">
-        <v>31.25</v>
-      </c>
-      <c r="K5" s="120">
-        <v>625.1</v>
-      </c>
-      <c r="L5" s="145">
-        <v>8.65</v>
-      </c>
-      <c r="M5" s="141">
-        <v>31.29</v>
-      </c>
-      <c r="N5" s="146">
-        <v>625.95000000000005</v>
-      </c>
-      <c r="O5" s="145">
-        <v>8.6300000000000008</v>
-      </c>
-      <c r="P5" s="141">
-        <v>31.34</v>
-      </c>
-      <c r="Q5" s="146">
-        <v>626.80999999999995</v>
-      </c>
-      <c r="R5" s="21"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="22"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="22"/>
-      <c r="X5" s="21"/>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="22"/>
-      <c r="AA5" s="21"/>
-      <c r="AB5" s="12"/>
-      <c r="AC5" s="22"/>
-      <c r="AD5" s="21"/>
-      <c r="AE5" s="12"/>
-      <c r="AF5" s="22"/>
-      <c r="AG5" s="21"/>
-      <c r="AH5" s="12"/>
-      <c r="AI5" s="22"/>
-      <c r="AJ5" s="21"/>
-      <c r="AK5" s="12"/>
-      <c r="AL5" s="22"/>
-      <c r="AM5" s="21"/>
-      <c r="AN5" s="12"/>
-      <c r="AO5" s="22"/>
-      <c r="AP5" s="21"/>
-      <c r="AQ5" s="12"/>
-      <c r="AR5" s="22"/>
-      <c r="AS5" s="21"/>
-      <c r="AT5" s="12"/>
-      <c r="AU5" s="22"/>
-    </row>
-    <row r="6" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="9">
-        <v>47119</v>
-      </c>
-      <c r="C6" s="121">
-        <v>8.9600000000000009</v>
-      </c>
-      <c r="D6" s="122">
-        <v>32.93</v>
-      </c>
-      <c r="E6" s="135">
-        <v>1097.8</v>
-      </c>
-      <c r="F6" s="132">
-        <v>8.91</v>
-      </c>
-      <c r="G6" s="123">
-        <v>33.04</v>
-      </c>
-      <c r="H6" s="124">
-        <v>1101.3900000000001</v>
-      </c>
-      <c r="I6" s="16">
-        <v>8.8699999999999992</v>
-      </c>
-      <c r="J6" s="123">
-        <v>33.130000000000003</v>
-      </c>
-      <c r="K6" s="124">
-        <v>1104.3399999999999</v>
-      </c>
-      <c r="L6" s="147">
-        <v>8.83</v>
-      </c>
-      <c r="M6" s="148">
-        <v>33.21</v>
-      </c>
-      <c r="N6" s="149">
-        <v>1107.3</v>
-      </c>
-      <c r="O6" s="147">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="P6" s="148">
-        <v>33.28</v>
-      </c>
-      <c r="Q6" s="149">
-        <v>1109.6199999999999</v>
-      </c>
-      <c r="R6" s="16"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="18"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="17"/>
-      <c r="W6" s="18"/>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="18"/>
-      <c r="AA6" s="16"/>
-      <c r="AB6" s="17"/>
-      <c r="AC6" s="18"/>
-      <c r="AD6" s="16"/>
-      <c r="AE6" s="17"/>
-      <c r="AF6" s="18"/>
-      <c r="AG6" s="16"/>
-      <c r="AH6" s="17"/>
-      <c r="AI6" s="18"/>
-      <c r="AJ6" s="16"/>
-      <c r="AK6" s="17"/>
-      <c r="AL6" s="18"/>
-      <c r="AM6" s="16"/>
-      <c r="AN6" s="17"/>
-      <c r="AO6" s="18"/>
-      <c r="AP6" s="16"/>
-      <c r="AQ6" s="17"/>
-      <c r="AR6" s="18"/>
-      <c r="AS6" s="16"/>
-      <c r="AT6" s="17"/>
-      <c r="AU6" s="18"/>
-    </row>
-    <row r="7" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:AU1"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit atualizacao tesouro dia 10/05
</commit_message>
<xml_diff>
--- a/TESOURO DIRETO_0519 - Compra.xlsx
+++ b/TESOURO DIRETO_0519 - Compra.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="020519" sheetId="21" r:id="rId1"/>
@@ -18,18 +18,19 @@
     <sheet name="070519" sheetId="24" r:id="rId4"/>
     <sheet name="080519" sheetId="25" r:id="rId5"/>
     <sheet name="090519" sheetId="26" r:id="rId6"/>
-    <sheet name="COMPARAÇÃO DIA A DIA" sheetId="4" r:id="rId7"/>
-    <sheet name="TESOURO IPCA" sheetId="5" r:id="rId8"/>
-    <sheet name="TESOURO IPCA JUROS SEMESTRAIS" sheetId="6" r:id="rId9"/>
-    <sheet name="TESOURO PREFIXADOS" sheetId="7" r:id="rId10"/>
-    <sheet name="TESOURO SELIC" sheetId="8" r:id="rId11"/>
+    <sheet name="100519" sheetId="27" r:id="rId7"/>
+    <sheet name="COMPARAÇÃO DIA A DIA" sheetId="4" r:id="rId8"/>
+    <sheet name="TESOURO IPCA" sheetId="5" r:id="rId9"/>
+    <sheet name="TESOURO IPCA JUROS SEMESTRAIS" sheetId="6" r:id="rId10"/>
+    <sheet name="TESOURO PREFIXADOS" sheetId="7" r:id="rId11"/>
+    <sheet name="TESOURO SELIC" sheetId="8" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="24">
   <si>
     <t>Vencimento</t>
   </si>
@@ -1329,6 +1330,7 @@
     <xf numFmtId="16" fontId="2" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1398,7 +1400,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2853,11 +2854,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="1908240144"/>
-        <c:axId val="1908241232"/>
+        <c:axId val="1552334832"/>
+        <c:axId val="1552337008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1908240144"/>
+        <c:axId val="1552334832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2899,7 +2900,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1908241232"/>
+        <c:crossAx val="1552337008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2907,7 +2908,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1908241232"/>
+        <c:axId val="1552337008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2957,7 +2958,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1908240144"/>
+        <c:crossAx val="1552334832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3326,8 +3327,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="82854576"/>
-        <c:axId val="82850224"/>
+        <c:axId val="1607745872"/>
+        <c:axId val="1607746416"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3780,7 +3781,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82854576"/>
+        <c:axId val="1607745872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3814,7 +3815,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82850224"/>
+        <c:crossAx val="1607746416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3822,7 +3823,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82850224"/>
+        <c:axId val="1607746416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3832,7 +3833,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82854576"/>
+        <c:crossAx val="1607745872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4187,8 +4188,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="82862192"/>
-        <c:axId val="82855120"/>
+        <c:axId val="1607742064"/>
+        <c:axId val="1607744784"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -4641,7 +4642,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82862192"/>
+        <c:axId val="1607742064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4675,7 +4676,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82855120"/>
+        <c:crossAx val="1607744784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4683,7 +4684,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82855120"/>
+        <c:axId val="1607744784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4693,7 +4694,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82862192"/>
+        <c:crossAx val="1607742064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5505,11 +5506,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="82859472"/>
-        <c:axId val="82863280"/>
+        <c:axId val="1607745328"/>
+        <c:axId val="1607734448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82859472"/>
+        <c:axId val="1607745328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5552,7 +5553,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82863280"/>
+        <c:crossAx val="1607734448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5560,7 +5561,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82863280"/>
+        <c:axId val="1607734448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5570,7 +5571,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82859472"/>
+        <c:crossAx val="1607745328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5929,11 +5930,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="82863824"/>
-        <c:axId val="82864912"/>
+        <c:axId val="1607746960"/>
+        <c:axId val="1607743152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82863824"/>
+        <c:axId val="1607746960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5967,7 +5968,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82864912"/>
+        <c:crossAx val="1607743152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5975,7 +5976,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82864912"/>
+        <c:axId val="1607743152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5985,7 +5986,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82863824"/>
+        <c:crossAx val="1607746960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6340,8 +6341,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="82852944"/>
-        <c:axId val="82850768"/>
+        <c:axId val="1607743696"/>
+        <c:axId val="1607744240"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -6794,7 +6795,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82852944"/>
+        <c:axId val="1607743696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6828,7 +6829,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82850768"/>
+        <c:crossAx val="1607744240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6836,7 +6837,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82850768"/>
+        <c:axId val="1607744240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6846,7 +6847,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82852944"/>
+        <c:crossAx val="1607743696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7201,8 +7202,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="82855664"/>
-        <c:axId val="82856208"/>
+        <c:axId val="1607736080"/>
+        <c:axId val="1607737712"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -7655,7 +7656,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82855664"/>
+        <c:axId val="1607736080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7689,7 +7690,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82856208"/>
+        <c:crossAx val="1607737712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7697,7 +7698,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82856208"/>
+        <c:axId val="1607737712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7707,7 +7708,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82855664"/>
+        <c:crossAx val="1607736080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8062,8 +8063,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="82856752"/>
-        <c:axId val="82857296"/>
+        <c:axId val="1607748048"/>
+        <c:axId val="1607740432"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -8516,7 +8517,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82856752"/>
+        <c:axId val="1607748048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8550,7 +8551,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82857296"/>
+        <c:crossAx val="1607740432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8558,7 +8559,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82857296"/>
+        <c:axId val="1607740432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8568,7 +8569,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82856752"/>
+        <c:crossAx val="1607748048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8923,8 +8924,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="82857840"/>
-        <c:axId val="2123219600"/>
+        <c:axId val="1607734992"/>
+        <c:axId val="1607735536"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -9377,7 +9378,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82857840"/>
+        <c:axId val="1607734992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9411,7 +9412,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123219600"/>
+        <c:crossAx val="1607735536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9419,7 +9420,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123219600"/>
+        <c:axId val="1607735536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9429,7 +9430,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82857840"/>
+        <c:crossAx val="1607734992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9784,11 +9785,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="2123222864"/>
-        <c:axId val="2123233744"/>
+        <c:axId val="1607738256"/>
+        <c:axId val="1607739888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2123222864"/>
+        <c:axId val="1607738256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9822,7 +9823,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123233744"/>
+        <c:crossAx val="1607739888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9830,7 +9831,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123233744"/>
+        <c:axId val="1607739888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9840,7 +9841,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123222864"/>
+        <c:crossAx val="1607738256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10195,8 +10196,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="2123221776"/>
-        <c:axId val="2123219056"/>
+        <c:axId val="1608775664"/>
+        <c:axId val="1608781648"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -10649,7 +10650,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2123221776"/>
+        <c:axId val="1608775664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10683,7 +10684,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123219056"/>
+        <c:crossAx val="1608781648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10691,7 +10692,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123219056"/>
+        <c:axId val="1608781648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10701,7 +10702,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123221776"/>
+        <c:crossAx val="1608775664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11299,11 +11300,11 @@
         </c:dLbls>
         <c:gapWidth val="315"/>
         <c:overlap val="-40"/>
-        <c:axId val="1889590352"/>
-        <c:axId val="1889591440"/>
+        <c:axId val="1552341904"/>
+        <c:axId val="1552342448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1889590352"/>
+        <c:axId val="1552341904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11364,7 +11365,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1889591440"/>
+        <c:crossAx val="1552342448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11372,7 +11373,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1889591440"/>
+        <c:axId val="1552342448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11433,7 +11434,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1889590352"/>
+        <c:crossAx val="1552341904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11794,8 +11795,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="2123223408"/>
-        <c:axId val="2123231024"/>
+        <c:axId val="1608775120"/>
+        <c:axId val="1608784368"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -12248,7 +12249,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2123223408"/>
+        <c:axId val="1608775120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12282,7 +12283,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123231024"/>
+        <c:crossAx val="1608784368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12290,7 +12291,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123231024"/>
+        <c:axId val="1608784368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12300,7 +12301,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123223408"/>
+        <c:crossAx val="1608775120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12655,8 +12656,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="2123218512"/>
-        <c:axId val="2123229936"/>
+        <c:axId val="1608778384"/>
+        <c:axId val="1608771856"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -13109,7 +13110,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2123218512"/>
+        <c:axId val="1608778384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13143,7 +13144,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123229936"/>
+        <c:crossAx val="1608771856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13151,7 +13152,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123229936"/>
+        <c:axId val="1608771856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13161,7 +13162,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123218512"/>
+        <c:crossAx val="1608778384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13516,8 +13517,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="2123230480"/>
-        <c:axId val="2123222320"/>
+        <c:axId val="1608782192"/>
+        <c:axId val="1608772400"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -13970,7 +13971,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2123230480"/>
+        <c:axId val="1608782192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14004,7 +14005,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123222320"/>
+        <c:crossAx val="1608772400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14012,7 +14013,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123222320"/>
+        <c:axId val="1608772400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14022,7 +14023,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123230480"/>
+        <c:crossAx val="1608782192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14377,8 +14378,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="2123220144"/>
-        <c:axId val="2123231568"/>
+        <c:axId val="1608774576"/>
+        <c:axId val="1608784912"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -14831,7 +14832,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2123220144"/>
+        <c:axId val="1608774576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14865,7 +14866,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123231568"/>
+        <c:crossAx val="1608784912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14873,7 +14874,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123231568"/>
+        <c:axId val="1608784912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14883,7 +14884,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123220144"/>
+        <c:crossAx val="1608774576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15238,8 +15239,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="2123229392"/>
-        <c:axId val="2123228848"/>
+        <c:axId val="1608779472"/>
+        <c:axId val="1608777840"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -15692,7 +15693,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2123229392"/>
+        <c:axId val="1608779472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15726,7 +15727,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123228848"/>
+        <c:crossAx val="1608777840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15734,7 +15735,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123228848"/>
+        <c:axId val="1608777840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15744,7 +15745,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123229392"/>
+        <c:crossAx val="1608779472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16099,8 +16100,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="2123227760"/>
-        <c:axId val="2123224496"/>
+        <c:axId val="1608774032"/>
+        <c:axId val="1608776208"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -16553,7 +16554,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2123227760"/>
+        <c:axId val="1608774032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16587,7 +16588,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123224496"/>
+        <c:crossAx val="1608776208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16595,7 +16596,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123224496"/>
+        <c:axId val="1608776208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16605,7 +16606,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123227760"/>
+        <c:crossAx val="1608774032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16960,8 +16961,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="2123233200"/>
-        <c:axId val="2123221232"/>
+        <c:axId val="1608778928"/>
+        <c:axId val="1608780016"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -17414,7 +17415,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2123233200"/>
+        <c:axId val="1608778928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17448,7 +17449,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123221232"/>
+        <c:crossAx val="1608780016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17456,7 +17457,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123221232"/>
+        <c:axId val="1608780016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17466,7 +17467,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123233200"/>
+        <c:crossAx val="1608778928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17821,8 +17822,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="2123223952"/>
-        <c:axId val="2123228304"/>
+        <c:axId val="1608769680"/>
+        <c:axId val="1608780560"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -18275,7 +18276,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2123223952"/>
+        <c:axId val="1608769680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18309,7 +18310,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123228304"/>
+        <c:crossAx val="1608780560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18317,7 +18318,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123228304"/>
+        <c:axId val="1608780560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18327,7 +18328,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123223952"/>
+        <c:crossAx val="1608769680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18682,8 +18683,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="2123220688"/>
-        <c:axId val="2123225040"/>
+        <c:axId val="1608770768"/>
+        <c:axId val="1608773488"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -19136,7 +19137,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2123220688"/>
+        <c:axId val="1608770768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19170,7 +19171,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123225040"/>
+        <c:crossAx val="1608773488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19178,7 +19179,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123225040"/>
+        <c:axId val="1608773488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19188,7 +19189,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123220688"/>
+        <c:crossAx val="1608770768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19543,8 +19544,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="2123232112"/>
-        <c:axId val="2123226672"/>
+        <c:axId val="1608781104"/>
+        <c:axId val="1608782736"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -19997,7 +19998,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2123232112"/>
+        <c:axId val="1608781104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20031,7 +20032,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123226672"/>
+        <c:crossAx val="1608782736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20039,7 +20040,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123226672"/>
+        <c:axId val="1608782736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20049,7 +20050,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123232112"/>
+        <c:crossAx val="1608781104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20404,11 +20405,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="82861104"/>
-        <c:axId val="82861648"/>
+        <c:axId val="1362705552"/>
+        <c:axId val="1362699568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82861104"/>
+        <c:axId val="1362705552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20442,7 +20443,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82861648"/>
+        <c:crossAx val="1362699568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20450,7 +20451,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82861648"/>
+        <c:axId val="1362699568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20460,7 +20461,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82861104"/>
+        <c:crossAx val="1362705552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20815,8 +20816,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="2123232656"/>
-        <c:axId val="2123227216"/>
+        <c:axId val="1608772944"/>
+        <c:axId val="1608771312"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -21269,7 +21270,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2123232656"/>
+        <c:axId val="1608772944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21303,7 +21304,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123227216"/>
+        <c:crossAx val="1608771312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21311,7 +21312,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123227216"/>
+        <c:axId val="1608771312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21321,7 +21322,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123232656"/>
+        <c:crossAx val="1608772944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21412,7 +21413,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21527,7 +21527,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -21689,11 +21688,11 @@
         </c:dropLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2123225584"/>
-        <c:axId val="2123226128"/>
+        <c:axId val="1608783280"/>
+        <c:axId val="1608776752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2123225584"/>
+        <c:axId val="1608783280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21727,7 +21726,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123226128"/>
+        <c:crossAx val="1608776752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21735,7 +21734,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123226128"/>
+        <c:axId val="1608776752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21745,7 +21744,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123225584"/>
+        <c:crossAx val="1608783280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21808,7 +21807,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21913,7 +21911,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -22074,11 +22071,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="85698480"/>
-        <c:axId val="85687600"/>
+        <c:axId val="1608777296"/>
+        <c:axId val="1608783824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85698480"/>
+        <c:axId val="1608777296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22112,7 +22109,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85687600"/>
+        <c:crossAx val="1608783824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22120,7 +22117,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85687600"/>
+        <c:axId val="1608783824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22130,7 +22127,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85698480"/>
+        <c:crossAx val="1608777296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22457,11 +22454,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="85688144"/>
-        <c:axId val="85689232"/>
+        <c:axId val="1608770224"/>
+        <c:axId val="1606718704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85688144"/>
+        <c:axId val="1608770224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22495,7 +22492,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85689232"/>
+        <c:crossAx val="1606718704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22503,7 +22500,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85689232"/>
+        <c:axId val="1606718704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22513,7 +22510,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85688144"/>
+        <c:crossAx val="1608770224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22840,11 +22837,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="82854032"/>
-        <c:axId val="82858384"/>
+        <c:axId val="1362701200"/>
+        <c:axId val="1607733360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82854032"/>
+        <c:axId val="1362701200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22878,7 +22875,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82858384"/>
+        <c:crossAx val="1607733360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22886,7 +22883,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82858384"/>
+        <c:axId val="1607733360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22896,7 +22893,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82854032"/>
+        <c:crossAx val="1362701200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23251,11 +23248,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="82864368"/>
-        <c:axId val="82853488"/>
+        <c:axId val="1607748592"/>
+        <c:axId val="1607739344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82864368"/>
+        <c:axId val="1607748592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23289,7 +23286,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82853488"/>
+        <c:crossAx val="1607739344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23297,7 +23294,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82853488"/>
+        <c:axId val="1607739344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23307,7 +23304,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82864368"/>
+        <c:crossAx val="1607748592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23662,11 +23659,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="82862736"/>
-        <c:axId val="82851856"/>
+        <c:axId val="1607736624"/>
+        <c:axId val="1607737168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82862736"/>
+        <c:axId val="1607736624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23700,7 +23697,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82851856"/>
+        <c:crossAx val="1607737168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23708,7 +23705,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82851856"/>
+        <c:axId val="1607737168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23718,7 +23715,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82862736"/>
+        <c:crossAx val="1607736624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -24073,8 +24070,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="82851312"/>
-        <c:axId val="82860016"/>
+        <c:axId val="1607733904"/>
+        <c:axId val="1607738800"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -24527,7 +24524,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82851312"/>
+        <c:axId val="1607733904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24561,7 +24558,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82860016"/>
+        <c:crossAx val="1607738800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -24569,7 +24566,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82860016"/>
+        <c:axId val="1607738800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24579,7 +24576,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82851312"/>
+        <c:crossAx val="1607733904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -24934,8 +24931,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="82849680"/>
-        <c:axId val="82858928"/>
+        <c:axId val="1607742608"/>
+        <c:axId val="1607740976"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -25388,7 +25385,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82849680"/>
+        <c:axId val="1607742608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25422,7 +25419,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82858928"/>
+        <c:crossAx val="1607740976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25430,7 +25427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82858928"/>
+        <c:axId val="1607740976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25440,7 +25437,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82849680"/>
+        <c:crossAx val="1607742608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -25795,8 +25792,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="82852400"/>
-        <c:axId val="82860560"/>
+        <c:axId val="1607747504"/>
+        <c:axId val="1607741520"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -26249,7 +26246,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82852400"/>
+        <c:axId val="1607747504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26283,7 +26280,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82860560"/>
+        <c:crossAx val="1607741520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -26291,7 +26288,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82860560"/>
+        <c:axId val="1607741520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26301,7 +26298,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82852400"/>
+        <c:crossAx val="1607747504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -45918,7 +45915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C16" sqref="C16:E16"/>
     </sheetView>
   </sheetViews>
@@ -45936,13 +45933,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="157" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="157"/>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
-      <c r="E1" s="158"/>
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="159"/>
       <c r="F1" s="51" t="s">
         <v>19</v>
       </c>
@@ -46112,13 +46109,13 @@
       <c r="I8" s="52"/>
     </row>
     <row r="9" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="159" t="s">
+      <c r="A9" s="160" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="160"/>
-      <c r="C9" s="160"/>
-      <c r="D9" s="160"/>
-      <c r="E9" s="161"/>
+      <c r="B9" s="161"/>
+      <c r="C9" s="161"/>
+      <c r="D9" s="161"/>
+      <c r="E9" s="162"/>
       <c r="F9" s="52"/>
       <c r="G9" s="52"/>
       <c r="H9" s="52"/>
@@ -46209,13 +46206,13 @@
       <c r="I13" s="52"/>
     </row>
     <row r="14" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="159" t="s">
+      <c r="A14" s="160" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="160"/>
-      <c r="C14" s="160"/>
-      <c r="D14" s="160"/>
-      <c r="E14" s="161"/>
+      <c r="B14" s="161"/>
+      <c r="C14" s="161"/>
+      <c r="D14" s="161"/>
+      <c r="E14" s="162"/>
       <c r="F14" s="52"/>
       <c r="G14" s="52"/>
       <c r="H14" s="52"/>
@@ -46274,6 +46271,663 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AU100"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4:Q6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="12" max="12" width="28.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" customWidth="1"/>
+    <col min="15" max="15" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="179" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="179"/>
+      <c r="C1" s="179"/>
+      <c r="D1" s="179"/>
+      <c r="E1" s="179"/>
+      <c r="F1" s="179"/>
+      <c r="G1" s="179"/>
+      <c r="H1" s="179"/>
+      <c r="I1" s="179"/>
+      <c r="J1" s="179"/>
+      <c r="K1" s="179"/>
+      <c r="L1" s="179"/>
+      <c r="M1" s="179"/>
+      <c r="N1" s="179"/>
+      <c r="O1" s="179"/>
+      <c r="P1" s="179"/>
+      <c r="Q1" s="179"/>
+      <c r="R1" s="179"/>
+      <c r="S1" s="179"/>
+      <c r="T1" s="179"/>
+      <c r="U1" s="179"/>
+      <c r="V1" s="179"/>
+      <c r="W1" s="179"/>
+      <c r="X1" s="179"/>
+      <c r="Y1" s="179"/>
+      <c r="Z1" s="179"/>
+      <c r="AA1" s="179"/>
+      <c r="AB1" s="179"/>
+      <c r="AC1" s="179"/>
+      <c r="AD1" s="179"/>
+      <c r="AE1" s="179"/>
+      <c r="AF1" s="179"/>
+      <c r="AG1" s="179"/>
+      <c r="AH1" s="179"/>
+      <c r="AI1" s="179"/>
+      <c r="AJ1" s="179"/>
+      <c r="AK1" s="179"/>
+      <c r="AL1" s="179"/>
+      <c r="AM1" s="179"/>
+      <c r="AN1" s="179"/>
+      <c r="AO1" s="179"/>
+      <c r="AP1" s="179"/>
+      <c r="AQ1" s="179"/>
+      <c r="AR1" s="179"/>
+      <c r="AS1" s="179"/>
+      <c r="AT1" s="179"/>
+      <c r="AU1" s="179"/>
+    </row>
+    <row r="2" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="T2" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="V2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="X2" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z2" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA2" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC2" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD2" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF2" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG2" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI2" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ2" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL2" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM2" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="AN2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO2" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP2" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR2" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="AS2" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU2" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="4">
+        <v>43587</v>
+      </c>
+      <c r="D3" s="4">
+        <v>43587</v>
+      </c>
+      <c r="E3" s="5">
+        <v>43587</v>
+      </c>
+      <c r="F3" s="3">
+        <v>43588</v>
+      </c>
+      <c r="G3" s="4">
+        <v>43588</v>
+      </c>
+      <c r="H3" s="5">
+        <v>43588</v>
+      </c>
+      <c r="I3" s="109">
+        <v>43591</v>
+      </c>
+      <c r="J3" s="109">
+        <v>43591</v>
+      </c>
+      <c r="K3" s="109">
+        <v>43591</v>
+      </c>
+      <c r="L3" s="3">
+        <v>43592</v>
+      </c>
+      <c r="M3" s="4">
+        <v>43592</v>
+      </c>
+      <c r="N3" s="4">
+        <v>43592</v>
+      </c>
+      <c r="O3" s="27">
+        <v>43593</v>
+      </c>
+      <c r="P3" s="28">
+        <v>43593</v>
+      </c>
+      <c r="Q3" s="28">
+        <v>43593</v>
+      </c>
+      <c r="R3" s="27"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="27"/>
+      <c r="V3" s="28"/>
+      <c r="W3" s="29"/>
+      <c r="X3" s="27"/>
+      <c r="Y3" s="28"/>
+      <c r="Z3" s="29"/>
+      <c r="AA3" s="27"/>
+      <c r="AB3" s="28"/>
+      <c r="AC3" s="29"/>
+      <c r="AD3" s="27"/>
+      <c r="AE3" s="28"/>
+      <c r="AF3" s="29"/>
+      <c r="AG3" s="27"/>
+      <c r="AH3" s="28"/>
+      <c r="AI3" s="29"/>
+      <c r="AJ3" s="27"/>
+      <c r="AK3" s="28"/>
+      <c r="AL3" s="29"/>
+      <c r="AM3" s="27"/>
+      <c r="AN3" s="28"/>
+      <c r="AO3" s="29"/>
+      <c r="AP3" s="46"/>
+      <c r="AQ3" s="46"/>
+      <c r="AR3" s="46"/>
+      <c r="AS3" s="27"/>
+      <c r="AT3" s="28"/>
+      <c r="AU3" s="29"/>
+    </row>
+    <row r="4" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="7">
+        <v>46249</v>
+      </c>
+      <c r="C4" s="119">
+        <v>4.13</v>
+      </c>
+      <c r="D4" s="66">
+        <v>36.26</v>
+      </c>
+      <c r="E4" s="134">
+        <v>3626.43</v>
+      </c>
+      <c r="F4" s="57">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="G4" s="58">
+        <v>36.33</v>
+      </c>
+      <c r="H4" s="120">
+        <v>3633.42</v>
+      </c>
+      <c r="I4" s="21">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="J4" s="58">
+        <v>36.450000000000003</v>
+      </c>
+      <c r="K4" s="120">
+        <v>3645.27</v>
+      </c>
+      <c r="L4" s="142">
+        <v>4.07</v>
+      </c>
+      <c r="M4" s="143">
+        <v>36.44</v>
+      </c>
+      <c r="N4" s="144">
+        <v>3644.48</v>
+      </c>
+      <c r="O4" s="142">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="P4" s="143">
+        <v>36.47</v>
+      </c>
+      <c r="Q4" s="144">
+        <v>3647.91</v>
+      </c>
+      <c r="R4" s="21"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="21"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="21"/>
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="21"/>
+      <c r="AE4" s="12"/>
+      <c r="AF4" s="22"/>
+      <c r="AG4" s="21"/>
+      <c r="AH4" s="12"/>
+      <c r="AI4" s="22"/>
+      <c r="AJ4" s="21"/>
+      <c r="AK4" s="12"/>
+      <c r="AL4" s="22"/>
+      <c r="AM4" s="21"/>
+      <c r="AN4" s="12"/>
+      <c r="AO4" s="22"/>
+      <c r="AP4" s="21"/>
+      <c r="AQ4" s="12"/>
+      <c r="AR4" s="12"/>
+      <c r="AS4" s="21"/>
+      <c r="AT4" s="12"/>
+      <c r="AU4" s="22"/>
+    </row>
+    <row r="5" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="7">
+        <v>49444</v>
+      </c>
+      <c r="C5" s="119">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="D5" s="66">
+        <v>39.07</v>
+      </c>
+      <c r="E5" s="134">
+        <v>3907.12</v>
+      </c>
+      <c r="F5" s="57">
+        <v>4.33</v>
+      </c>
+      <c r="G5" s="58">
+        <v>39.18</v>
+      </c>
+      <c r="H5" s="120">
+        <v>3918.25</v>
+      </c>
+      <c r="I5" s="21">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="J5" s="58">
+        <v>39.270000000000003</v>
+      </c>
+      <c r="K5" s="120">
+        <v>3927.82</v>
+      </c>
+      <c r="L5" s="145">
+        <v>4.29</v>
+      </c>
+      <c r="M5" s="141">
+        <v>39.369999999999997</v>
+      </c>
+      <c r="N5" s="146">
+        <v>3937.41</v>
+      </c>
+      <c r="O5" s="145">
+        <v>4.28</v>
+      </c>
+      <c r="P5" s="141">
+        <v>39.42</v>
+      </c>
+      <c r="Q5" s="146">
+        <v>3942.94</v>
+      </c>
+      <c r="R5" s="21"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="21"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="22"/>
+      <c r="AA5" s="21"/>
+      <c r="AB5" s="12"/>
+      <c r="AC5" s="22"/>
+      <c r="AD5" s="21"/>
+      <c r="AE5" s="12"/>
+      <c r="AF5" s="22"/>
+      <c r="AG5" s="21"/>
+      <c r="AH5" s="12"/>
+      <c r="AI5" s="22"/>
+      <c r="AJ5" s="21"/>
+      <c r="AK5" s="12"/>
+      <c r="AL5" s="22"/>
+      <c r="AM5" s="21"/>
+      <c r="AN5" s="12"/>
+      <c r="AO5" s="22"/>
+      <c r="AP5" s="21"/>
+      <c r="AQ5" s="12"/>
+      <c r="AR5" s="12"/>
+      <c r="AS5" s="21"/>
+      <c r="AT5" s="12"/>
+      <c r="AU5" s="22"/>
+    </row>
+    <row r="6" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="9">
+        <v>55015</v>
+      </c>
+      <c r="C6" s="121">
+        <v>4.45</v>
+      </c>
+      <c r="D6" s="122">
+        <v>40.880000000000003</v>
+      </c>
+      <c r="E6" s="135">
+        <v>4088.23</v>
+      </c>
+      <c r="F6" s="132">
+        <v>4.43</v>
+      </c>
+      <c r="G6" s="123">
+        <v>41.04</v>
+      </c>
+      <c r="H6" s="124">
+        <v>4104.07</v>
+      </c>
+      <c r="I6" s="16">
+        <v>4.42</v>
+      </c>
+      <c r="J6" s="123">
+        <v>41.11</v>
+      </c>
+      <c r="K6" s="124">
+        <v>4111.95</v>
+      </c>
+      <c r="L6" s="147">
+        <v>4.41</v>
+      </c>
+      <c r="M6" s="148">
+        <v>41.19</v>
+      </c>
+      <c r="N6" s="149">
+        <v>4119.8500000000004</v>
+      </c>
+      <c r="O6" s="147">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="P6" s="148">
+        <v>41.27</v>
+      </c>
+      <c r="Q6" s="149">
+        <v>4127.7700000000004</v>
+      </c>
+      <c r="R6" s="16"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="18"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="18"/>
+      <c r="AD6" s="16"/>
+      <c r="AE6" s="17"/>
+      <c r="AF6" s="18"/>
+      <c r="AG6" s="16"/>
+      <c r="AH6" s="17"/>
+      <c r="AI6" s="18"/>
+      <c r="AJ6" s="16"/>
+      <c r="AK6" s="17"/>
+      <c r="AL6" s="18"/>
+      <c r="AM6" s="16"/>
+      <c r="AN6" s="17"/>
+      <c r="AO6" s="18"/>
+      <c r="AP6" s="16"/>
+      <c r="AQ6" s="17"/>
+      <c r="AR6" s="17"/>
+      <c r="AS6" s="16"/>
+      <c r="AT6" s="17"/>
+      <c r="AU6" s="18"/>
+    </row>
+    <row r="7" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:AU1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>
@@ -46303,55 +46957,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="179" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="178"/>
-      <c r="H1" s="178"/>
-      <c r="I1" s="178"/>
-      <c r="J1" s="178"/>
-      <c r="K1" s="178"/>
-      <c r="L1" s="178"/>
-      <c r="M1" s="178"/>
-      <c r="N1" s="178"/>
-      <c r="O1" s="178"/>
-      <c r="P1" s="178"/>
-      <c r="Q1" s="178"/>
-      <c r="R1" s="178"/>
-      <c r="S1" s="178"/>
-      <c r="T1" s="178"/>
-      <c r="U1" s="178"/>
-      <c r="V1" s="178"/>
-      <c r="W1" s="178"/>
-      <c r="X1" s="178"/>
-      <c r="Y1" s="178"/>
-      <c r="Z1" s="178"/>
-      <c r="AA1" s="178"/>
-      <c r="AB1" s="178"/>
-      <c r="AC1" s="178"/>
-      <c r="AD1" s="178"/>
-      <c r="AE1" s="178"/>
-      <c r="AF1" s="178"/>
-      <c r="AG1" s="178"/>
-      <c r="AH1" s="178"/>
-      <c r="AI1" s="178"/>
-      <c r="AJ1" s="178"/>
-      <c r="AK1" s="178"/>
-      <c r="AL1" s="178"/>
-      <c r="AM1" s="178"/>
-      <c r="AN1" s="178"/>
-      <c r="AO1" s="178"/>
-      <c r="AP1" s="178"/>
-      <c r="AQ1" s="178"/>
-      <c r="AR1" s="178"/>
-      <c r="AS1" s="178"/>
-      <c r="AT1" s="178"/>
-      <c r="AU1" s="178"/>
+      <c r="B1" s="179"/>
+      <c r="C1" s="179"/>
+      <c r="D1" s="179"/>
+      <c r="E1" s="179"/>
+      <c r="F1" s="179"/>
+      <c r="G1" s="179"/>
+      <c r="H1" s="179"/>
+      <c r="I1" s="179"/>
+      <c r="J1" s="179"/>
+      <c r="K1" s="179"/>
+      <c r="L1" s="179"/>
+      <c r="M1" s="179"/>
+      <c r="N1" s="179"/>
+      <c r="O1" s="179"/>
+      <c r="P1" s="179"/>
+      <c r="Q1" s="179"/>
+      <c r="R1" s="179"/>
+      <c r="S1" s="179"/>
+      <c r="T1" s="179"/>
+      <c r="U1" s="179"/>
+      <c r="V1" s="179"/>
+      <c r="W1" s="179"/>
+      <c r="X1" s="179"/>
+      <c r="Y1" s="179"/>
+      <c r="Z1" s="179"/>
+      <c r="AA1" s="179"/>
+      <c r="AB1" s="179"/>
+      <c r="AC1" s="179"/>
+      <c r="AD1" s="179"/>
+      <c r="AE1" s="179"/>
+      <c r="AF1" s="179"/>
+      <c r="AG1" s="179"/>
+      <c r="AH1" s="179"/>
+      <c r="AI1" s="179"/>
+      <c r="AJ1" s="179"/>
+      <c r="AK1" s="179"/>
+      <c r="AL1" s="179"/>
+      <c r="AM1" s="179"/>
+      <c r="AN1" s="179"/>
+      <c r="AO1" s="179"/>
+      <c r="AP1" s="179"/>
+      <c r="AQ1" s="179"/>
+      <c r="AR1" s="179"/>
+      <c r="AS1" s="179"/>
+      <c r="AT1" s="179"/>
+      <c r="AU1" s="179"/>
     </row>
     <row r="2" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -46930,7 +47584,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>
@@ -46960,55 +47614,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="174" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="174"/>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
-      <c r="G1" s="174"/>
-      <c r="H1" s="174"/>
-      <c r="I1" s="174"/>
-      <c r="J1" s="174"/>
-      <c r="K1" s="174"/>
-      <c r="L1" s="174"/>
-      <c r="M1" s="174"/>
-      <c r="N1" s="174"/>
-      <c r="O1" s="174"/>
-      <c r="P1" s="174"/>
-      <c r="Q1" s="174"/>
-      <c r="R1" s="174"/>
-      <c r="S1" s="174"/>
-      <c r="T1" s="174"/>
-      <c r="U1" s="174"/>
-      <c r="V1" s="174"/>
-      <c r="W1" s="174"/>
-      <c r="X1" s="174"/>
-      <c r="Y1" s="174"/>
-      <c r="Z1" s="174"/>
-      <c r="AA1" s="174"/>
-      <c r="AB1" s="174"/>
-      <c r="AC1" s="174"/>
-      <c r="AD1" s="174"/>
-      <c r="AE1" s="174"/>
-      <c r="AF1" s="174"/>
-      <c r="AG1" s="174"/>
-      <c r="AH1" s="174"/>
-      <c r="AI1" s="174"/>
-      <c r="AJ1" s="174"/>
-      <c r="AK1" s="174"/>
-      <c r="AL1" s="174"/>
-      <c r="AM1" s="174"/>
-      <c r="AN1" s="174"/>
-      <c r="AO1" s="174"/>
-      <c r="AP1" s="174"/>
-      <c r="AQ1" s="174"/>
-      <c r="AR1" s="174"/>
-      <c r="AS1" s="174"/>
-      <c r="AT1" s="174"/>
-      <c r="AU1" s="175"/>
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="175"/>
+      <c r="H1" s="175"/>
+      <c r="I1" s="175"/>
+      <c r="J1" s="175"/>
+      <c r="K1" s="175"/>
+      <c r="L1" s="175"/>
+      <c r="M1" s="175"/>
+      <c r="N1" s="175"/>
+      <c r="O1" s="175"/>
+      <c r="P1" s="175"/>
+      <c r="Q1" s="175"/>
+      <c r="R1" s="175"/>
+      <c r="S1" s="175"/>
+      <c r="T1" s="175"/>
+      <c r="U1" s="175"/>
+      <c r="V1" s="175"/>
+      <c r="W1" s="175"/>
+      <c r="X1" s="175"/>
+      <c r="Y1" s="175"/>
+      <c r="Z1" s="175"/>
+      <c r="AA1" s="175"/>
+      <c r="AB1" s="175"/>
+      <c r="AC1" s="175"/>
+      <c r="AD1" s="175"/>
+      <c r="AE1" s="175"/>
+      <c r="AF1" s="175"/>
+      <c r="AG1" s="175"/>
+      <c r="AH1" s="175"/>
+      <c r="AI1" s="175"/>
+      <c r="AJ1" s="175"/>
+      <c r="AK1" s="175"/>
+      <c r="AL1" s="175"/>
+      <c r="AM1" s="175"/>
+      <c r="AN1" s="175"/>
+      <c r="AO1" s="175"/>
+      <c r="AP1" s="175"/>
+      <c r="AQ1" s="175"/>
+      <c r="AR1" s="175"/>
+      <c r="AS1" s="175"/>
+      <c r="AT1" s="175"/>
+      <c r="AU1" s="176"/>
     </row>
     <row r="2" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
@@ -47474,13 +48128,13 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="162" t="s">
+      <c r="A2" s="163" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="164"/>
+      <c r="B2" s="164"/>
+      <c r="C2" s="164"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="165"/>
       <c r="F2" s="52"/>
       <c r="G2" s="52"/>
       <c r="H2" s="52"/>
@@ -47621,13 +48275,13 @@
       <c r="I8" s="52"/>
     </row>
     <row r="9" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="165" t="s">
+      <c r="A9" s="166" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="166"/>
-      <c r="C9" s="166"/>
-      <c r="D9" s="166"/>
-      <c r="E9" s="167"/>
+      <c r="B9" s="167"/>
+      <c r="C9" s="167"/>
+      <c r="D9" s="167"/>
+      <c r="E9" s="168"/>
       <c r="F9" s="52"/>
       <c r="G9" s="52"/>
       <c r="H9" s="52"/>
@@ -47697,13 +48351,13 @@
       <c r="I12" s="52"/>
     </row>
     <row r="13" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="162" t="s">
+      <c r="A13" s="163" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="163"/>
-      <c r="C13" s="163"/>
-      <c r="D13" s="163"/>
-      <c r="E13" s="164"/>
+      <c r="B13" s="164"/>
+      <c r="C13" s="164"/>
+      <c r="D13" s="164"/>
+      <c r="E13" s="165"/>
       <c r="F13" s="52"/>
       <c r="G13" s="52"/>
       <c r="H13" s="52"/>
@@ -47792,13 +48446,13 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="168" t="s">
+      <c r="A2" s="169" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
+      <c r="B2" s="170"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
       <c r="F2" s="52"/>
       <c r="G2" s="52"/>
       <c r="H2" s="52"/>
@@ -47939,13 +48593,13 @@
       <c r="I8" s="52"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="170" t="s">
+      <c r="A9" s="171" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="171"/>
-      <c r="C9" s="171"/>
-      <c r="D9" s="171"/>
-      <c r="E9" s="171"/>
+      <c r="B9" s="172"/>
+      <c r="C9" s="172"/>
+      <c r="D9" s="172"/>
+      <c r="E9" s="172"/>
       <c r="F9" s="52"/>
       <c r="G9" s="52"/>
       <c r="H9" s="52"/>
@@ -48015,13 +48669,13 @@
       <c r="I12" s="52"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="170" t="s">
+      <c r="A13" s="171" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="171"/>
-      <c r="C13" s="171"/>
-      <c r="D13" s="171"/>
-      <c r="E13" s="171"/>
+      <c r="B13" s="172"/>
+      <c r="C13" s="172"/>
+      <c r="D13" s="172"/>
+      <c r="E13" s="172"/>
       <c r="F13" s="52"/>
       <c r="G13" s="52"/>
       <c r="H13" s="52"/>
@@ -48093,13 +48747,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="172" t="s">
+      <c r="A2" s="173" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="172"/>
-      <c r="C2" s="172"/>
-      <c r="D2" s="172"/>
-      <c r="E2" s="172"/>
+      <c r="B2" s="173"/>
+      <c r="C2" s="173"/>
+      <c r="D2" s="173"/>
+      <c r="E2" s="173"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="138" t="s">
@@ -48204,13 +48858,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="172" t="s">
+      <c r="A9" s="173" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="172"/>
-      <c r="C9" s="172"/>
-      <c r="D9" s="172"/>
-      <c r="E9" s="172"/>
+      <c r="B9" s="173"/>
+      <c r="C9" s="173"/>
+      <c r="D9" s="173"/>
+      <c r="E9" s="173"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="138" t="s">
@@ -48264,13 +48918,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="172" t="s">
+      <c r="A13" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="172"/>
-      <c r="C13" s="172"/>
-      <c r="D13" s="172"/>
-      <c r="E13" s="172"/>
+      <c r="B13" s="173"/>
+      <c r="C13" s="173"/>
+      <c r="D13" s="173"/>
+      <c r="E13" s="173"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="138" t="s">
@@ -48335,13 +48989,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="172" t="s">
+      <c r="A2" s="173" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="172"/>
-      <c r="C2" s="172"/>
-      <c r="D2" s="172"/>
-      <c r="E2" s="172"/>
+      <c r="B2" s="173"/>
+      <c r="C2" s="173"/>
+      <c r="D2" s="173"/>
+      <c r="E2" s="173"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="138" t="s">
@@ -48446,13 +49100,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="172" t="s">
+      <c r="A9" s="173" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="172"/>
-      <c r="C9" s="172"/>
-      <c r="D9" s="172"/>
-      <c r="E9" s="172"/>
+      <c r="B9" s="173"/>
+      <c r="C9" s="173"/>
+      <c r="D9" s="173"/>
+      <c r="E9" s="173"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="138" t="s">
@@ -48506,13 +49160,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="172" t="s">
+      <c r="A13" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="172"/>
-      <c r="C13" s="172"/>
-      <c r="D13" s="172"/>
-      <c r="E13" s="172"/>
+      <c r="B13" s="173"/>
+      <c r="C13" s="173"/>
+      <c r="D13" s="173"/>
+      <c r="E13" s="173"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="138" t="s">
@@ -48546,18 +49200,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40" style="179" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="179" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" style="179" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="179" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="179" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="179"/>
+    <col min="1" max="1" width="40" style="156" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="156" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" style="156" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="156" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="156" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="156"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -48578,13 +49232,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="172" t="s">
+      <c r="A2" s="173" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="172"/>
-      <c r="C2" s="172"/>
-      <c r="D2" s="172"/>
-      <c r="E2" s="172"/>
+      <c r="B2" s="173"/>
+      <c r="C2" s="173"/>
+      <c r="D2" s="173"/>
+      <c r="E2" s="173"/>
     </row>
     <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="138" t="s">
@@ -48672,13 +49326,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="172" t="s">
+      <c r="A8" s="173" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="172"/>
-      <c r="C8" s="172"/>
-      <c r="D8" s="172"/>
-      <c r="E8" s="172"/>
+      <c r="B8" s="173"/>
+      <c r="C8" s="173"/>
+      <c r="D8" s="173"/>
+      <c r="E8" s="173"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="138" t="s">
@@ -48732,13 +49386,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="172" t="s">
+      <c r="A12" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="172"/>
-      <c r="C12" s="172"/>
-      <c r="D12" s="172"/>
-      <c r="E12" s="172"/>
+      <c r="B12" s="173"/>
+      <c r="C12" s="173"/>
+      <c r="D12" s="173"/>
+      <c r="E12" s="173"/>
     </row>
     <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="138" t="s">
@@ -48769,6 +49423,231 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40" style="156" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="156" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" style="156" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="156" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="156" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="156"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="137" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="137" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="137" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="137" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="137" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="173" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="173"/>
+      <c r="C2" s="173"/>
+      <c r="D2" s="173"/>
+      <c r="E2" s="173"/>
+    </row>
+    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="138" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="139">
+        <v>45519</v>
+      </c>
+      <c r="C3" s="140">
+        <v>3.98</v>
+      </c>
+      <c r="D3" s="141">
+        <v>52.52</v>
+      </c>
+      <c r="E3" s="141">
+        <v>2626.42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="138" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="139">
+        <v>49444</v>
+      </c>
+      <c r="C4" s="140">
+        <v>4.32</v>
+      </c>
+      <c r="D4" s="141">
+        <v>32.82</v>
+      </c>
+      <c r="E4" s="141">
+        <v>1641.34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="138" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="139">
+        <v>53097</v>
+      </c>
+      <c r="C5" s="140">
+        <v>4.32</v>
+      </c>
+      <c r="D5" s="141">
+        <v>32.29</v>
+      </c>
+      <c r="E5" s="141">
+        <v>1076.54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="138" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="139">
+        <v>46249</v>
+      </c>
+      <c r="C6" s="140">
+        <v>4.03</v>
+      </c>
+      <c r="D6" s="141">
+        <v>36.56</v>
+      </c>
+      <c r="E6" s="141">
+        <v>3656.99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="138" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="139">
+        <v>55015</v>
+      </c>
+      <c r="C7" s="140">
+        <v>4.34</v>
+      </c>
+      <c r="D7" s="141">
+        <v>41.69</v>
+      </c>
+      <c r="E7" s="141">
+        <v>4169.58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="173" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="173"/>
+      <c r="C8" s="173"/>
+      <c r="D8" s="173"/>
+      <c r="E8" s="173"/>
+    </row>
+    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="138" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="139">
+        <v>44562</v>
+      </c>
+      <c r="C9" s="140">
+        <v>7.55</v>
+      </c>
+      <c r="D9" s="141">
+        <v>33</v>
+      </c>
+      <c r="E9" s="141">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="138" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="139">
+        <v>45658</v>
+      </c>
+      <c r="C10" s="140">
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="D10" s="141">
+        <v>31.49</v>
+      </c>
+      <c r="E10" s="141">
+        <v>629.83000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="138" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="139">
+        <v>47119</v>
+      </c>
+      <c r="C11" s="140">
+        <v>8.74</v>
+      </c>
+      <c r="D11" s="141">
+        <v>33.42</v>
+      </c>
+      <c r="E11" s="141">
+        <v>1114.27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="173" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="173"/>
+      <c r="C12" s="173"/>
+      <c r="D12" s="173"/>
+      <c r="E12" s="173"/>
+    </row>
+    <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="138" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="139">
+        <v>45717</v>
+      </c>
+      <c r="C13" s="140">
+        <v>0.02</v>
+      </c>
+      <c r="D13" s="141">
+        <v>100.9</v>
+      </c>
+      <c r="E13" s="141">
+        <v>10090.11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A12:E12"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -48831,55 +49710,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="174" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="174"/>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
-      <c r="G1" s="174"/>
-      <c r="H1" s="174"/>
-      <c r="I1" s="174"/>
-      <c r="J1" s="174"/>
-      <c r="K1" s="174"/>
-      <c r="L1" s="174"/>
-      <c r="M1" s="174"/>
-      <c r="N1" s="174"/>
-      <c r="O1" s="174"/>
-      <c r="P1" s="174"/>
-      <c r="Q1" s="174"/>
-      <c r="R1" s="174"/>
-      <c r="S1" s="174"/>
-      <c r="T1" s="174"/>
-      <c r="U1" s="174"/>
-      <c r="V1" s="174"/>
-      <c r="W1" s="174"/>
-      <c r="X1" s="174"/>
-      <c r="Y1" s="174"/>
-      <c r="Z1" s="174"/>
-      <c r="AA1" s="174"/>
-      <c r="AB1" s="174"/>
-      <c r="AC1" s="174"/>
-      <c r="AD1" s="174"/>
-      <c r="AE1" s="174"/>
-      <c r="AF1" s="174"/>
-      <c r="AG1" s="174"/>
-      <c r="AH1" s="174"/>
-      <c r="AI1" s="174"/>
-      <c r="AJ1" s="174"/>
-      <c r="AK1" s="174"/>
-      <c r="AL1" s="174"/>
-      <c r="AM1" s="174"/>
-      <c r="AN1" s="174"/>
-      <c r="AO1" s="174"/>
-      <c r="AP1" s="174"/>
-      <c r="AQ1" s="174"/>
-      <c r="AR1" s="174"/>
-      <c r="AS1" s="174"/>
-      <c r="AT1" s="174"/>
-      <c r="AU1" s="175"/>
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="175"/>
+      <c r="H1" s="175"/>
+      <c r="I1" s="175"/>
+      <c r="J1" s="175"/>
+      <c r="K1" s="175"/>
+      <c r="L1" s="175"/>
+      <c r="M1" s="175"/>
+      <c r="N1" s="175"/>
+      <c r="O1" s="175"/>
+      <c r="P1" s="175"/>
+      <c r="Q1" s="175"/>
+      <c r="R1" s="175"/>
+      <c r="S1" s="175"/>
+      <c r="T1" s="175"/>
+      <c r="U1" s="175"/>
+      <c r="V1" s="175"/>
+      <c r="W1" s="175"/>
+      <c r="X1" s="175"/>
+      <c r="Y1" s="175"/>
+      <c r="Z1" s="175"/>
+      <c r="AA1" s="175"/>
+      <c r="AB1" s="175"/>
+      <c r="AC1" s="175"/>
+      <c r="AD1" s="175"/>
+      <c r="AE1" s="175"/>
+      <c r="AF1" s="175"/>
+      <c r="AG1" s="175"/>
+      <c r="AH1" s="175"/>
+      <c r="AI1" s="175"/>
+      <c r="AJ1" s="175"/>
+      <c r="AK1" s="175"/>
+      <c r="AL1" s="175"/>
+      <c r="AM1" s="175"/>
+      <c r="AN1" s="175"/>
+      <c r="AO1" s="175"/>
+      <c r="AP1" s="175"/>
+      <c r="AQ1" s="175"/>
+      <c r="AR1" s="175"/>
+      <c r="AS1" s="175"/>
+      <c r="AT1" s="175"/>
+      <c r="AU1" s="176"/>
     </row>
     <row r="2" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="129" t="s">
@@ -49604,55 +50483,55 @@
       <c r="AU9" s="18"/>
     </row>
     <row r="10" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="177" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="177"/>
-      <c r="C10" s="177"/>
-      <c r="D10" s="177"/>
-      <c r="E10" s="177"/>
-      <c r="F10" s="177"/>
-      <c r="G10" s="177"/>
-      <c r="H10" s="177"/>
-      <c r="I10" s="177"/>
-      <c r="J10" s="177"/>
-      <c r="K10" s="177"/>
-      <c r="L10" s="177"/>
-      <c r="M10" s="177"/>
-      <c r="N10" s="177"/>
-      <c r="O10" s="177"/>
-      <c r="P10" s="177"/>
-      <c r="Q10" s="177"/>
-      <c r="R10" s="177"/>
-      <c r="S10" s="177"/>
-      <c r="T10" s="177"/>
-      <c r="U10" s="177"/>
-      <c r="V10" s="177"/>
-      <c r="W10" s="177"/>
-      <c r="X10" s="177"/>
-      <c r="Y10" s="177"/>
-      <c r="Z10" s="177"/>
-      <c r="AA10" s="177"/>
-      <c r="AB10" s="177"/>
-      <c r="AC10" s="177"/>
-      <c r="AD10" s="177"/>
-      <c r="AE10" s="177"/>
-      <c r="AF10" s="177"/>
-      <c r="AG10" s="177"/>
-      <c r="AH10" s="177"/>
-      <c r="AI10" s="177"/>
-      <c r="AJ10" s="177"/>
-      <c r="AK10" s="177"/>
-      <c r="AL10" s="177"/>
-      <c r="AM10" s="177"/>
-      <c r="AN10" s="177"/>
-      <c r="AO10" s="177"/>
-      <c r="AP10" s="177"/>
-      <c r="AQ10" s="177"/>
-      <c r="AR10" s="177"/>
-      <c r="AS10" s="177"/>
-      <c r="AT10" s="177"/>
-      <c r="AU10" s="177"/>
+      <c r="B10" s="178"/>
+      <c r="C10" s="178"/>
+      <c r="D10" s="178"/>
+      <c r="E10" s="178"/>
+      <c r="F10" s="178"/>
+      <c r="G10" s="178"/>
+      <c r="H10" s="178"/>
+      <c r="I10" s="178"/>
+      <c r="J10" s="178"/>
+      <c r="K10" s="178"/>
+      <c r="L10" s="178"/>
+      <c r="M10" s="178"/>
+      <c r="N10" s="178"/>
+      <c r="O10" s="178"/>
+      <c r="P10" s="178"/>
+      <c r="Q10" s="178"/>
+      <c r="R10" s="178"/>
+      <c r="S10" s="178"/>
+      <c r="T10" s="178"/>
+      <c r="U10" s="178"/>
+      <c r="V10" s="178"/>
+      <c r="W10" s="178"/>
+      <c r="X10" s="178"/>
+      <c r="Y10" s="178"/>
+      <c r="Z10" s="178"/>
+      <c r="AA10" s="178"/>
+      <c r="AB10" s="178"/>
+      <c r="AC10" s="178"/>
+      <c r="AD10" s="178"/>
+      <c r="AE10" s="178"/>
+      <c r="AF10" s="178"/>
+      <c r="AG10" s="178"/>
+      <c r="AH10" s="178"/>
+      <c r="AI10" s="178"/>
+      <c r="AJ10" s="178"/>
+      <c r="AK10" s="178"/>
+      <c r="AL10" s="178"/>
+      <c r="AM10" s="178"/>
+      <c r="AN10" s="178"/>
+      <c r="AO10" s="178"/>
+      <c r="AP10" s="178"/>
+      <c r="AQ10" s="178"/>
+      <c r="AR10" s="178"/>
+      <c r="AS10" s="178"/>
+      <c r="AT10" s="178"/>
+      <c r="AU10" s="178"/>
     </row>
     <row r="11" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
@@ -50128,55 +51007,55 @@
       <c r="AU15" s="18"/>
     </row>
     <row r="16" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="176" t="s">
+      <c r="A16" s="177" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="177"/>
-      <c r="C16" s="177"/>
-      <c r="D16" s="177"/>
-      <c r="E16" s="177"/>
-      <c r="F16" s="177"/>
-      <c r="G16" s="177"/>
-      <c r="H16" s="177"/>
-      <c r="I16" s="177"/>
-      <c r="J16" s="177"/>
-      <c r="K16" s="177"/>
-      <c r="L16" s="177"/>
-      <c r="M16" s="177"/>
-      <c r="N16" s="177"/>
-      <c r="O16" s="177"/>
-      <c r="P16" s="177"/>
-      <c r="Q16" s="177"/>
-      <c r="R16" s="177"/>
-      <c r="S16" s="177"/>
-      <c r="T16" s="177"/>
-      <c r="U16" s="177"/>
-      <c r="V16" s="177"/>
-      <c r="W16" s="177"/>
-      <c r="X16" s="177"/>
-      <c r="Y16" s="177"/>
-      <c r="Z16" s="177"/>
-      <c r="AA16" s="177"/>
-      <c r="AB16" s="177"/>
-      <c r="AC16" s="177"/>
-      <c r="AD16" s="177"/>
-      <c r="AE16" s="177"/>
-      <c r="AF16" s="177"/>
-      <c r="AG16" s="177"/>
-      <c r="AH16" s="177"/>
-      <c r="AI16" s="177"/>
-      <c r="AJ16" s="177"/>
-      <c r="AK16" s="177"/>
-      <c r="AL16" s="177"/>
-      <c r="AM16" s="177"/>
-      <c r="AN16" s="177"/>
-      <c r="AO16" s="177"/>
-      <c r="AP16" s="177"/>
-      <c r="AQ16" s="177"/>
-      <c r="AR16" s="177"/>
-      <c r="AS16" s="177"/>
-      <c r="AT16" s="177"/>
-      <c r="AU16" s="177"/>
+      <c r="B16" s="178"/>
+      <c r="C16" s="178"/>
+      <c r="D16" s="178"/>
+      <c r="E16" s="178"/>
+      <c r="F16" s="178"/>
+      <c r="G16" s="178"/>
+      <c r="H16" s="178"/>
+      <c r="I16" s="178"/>
+      <c r="J16" s="178"/>
+      <c r="K16" s="178"/>
+      <c r="L16" s="178"/>
+      <c r="M16" s="178"/>
+      <c r="N16" s="178"/>
+      <c r="O16" s="178"/>
+      <c r="P16" s="178"/>
+      <c r="Q16" s="178"/>
+      <c r="R16" s="178"/>
+      <c r="S16" s="178"/>
+      <c r="T16" s="178"/>
+      <c r="U16" s="178"/>
+      <c r="V16" s="178"/>
+      <c r="W16" s="178"/>
+      <c r="X16" s="178"/>
+      <c r="Y16" s="178"/>
+      <c r="Z16" s="178"/>
+      <c r="AA16" s="178"/>
+      <c r="AB16" s="178"/>
+      <c r="AC16" s="178"/>
+      <c r="AD16" s="178"/>
+      <c r="AE16" s="178"/>
+      <c r="AF16" s="178"/>
+      <c r="AG16" s="178"/>
+      <c r="AH16" s="178"/>
+      <c r="AI16" s="178"/>
+      <c r="AJ16" s="178"/>
+      <c r="AK16" s="178"/>
+      <c r="AL16" s="178"/>
+      <c r="AM16" s="178"/>
+      <c r="AN16" s="178"/>
+      <c r="AO16" s="178"/>
+      <c r="AP16" s="178"/>
+      <c r="AQ16" s="178"/>
+      <c r="AR16" s="178"/>
+      <c r="AS16" s="178"/>
+      <c r="AT16" s="178"/>
+      <c r="AU16" s="178"/>
     </row>
     <row r="17" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
@@ -50578,7 +51457,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>
@@ -50632,55 +51511,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="177" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="177"/>
-      <c r="E1" s="177"/>
-      <c r="F1" s="177"/>
-      <c r="G1" s="177"/>
-      <c r="H1" s="177"/>
-      <c r="I1" s="177"/>
-      <c r="J1" s="177"/>
-      <c r="K1" s="177"/>
-      <c r="L1" s="177"/>
-      <c r="M1" s="177"/>
-      <c r="N1" s="177"/>
-      <c r="O1" s="177"/>
-      <c r="P1" s="177"/>
-      <c r="Q1" s="177"/>
-      <c r="R1" s="177"/>
-      <c r="S1" s="177"/>
-      <c r="T1" s="177"/>
-      <c r="U1" s="177"/>
-      <c r="V1" s="177"/>
-      <c r="W1" s="177"/>
-      <c r="X1" s="177"/>
-      <c r="Y1" s="177"/>
-      <c r="Z1" s="177"/>
-      <c r="AA1" s="177"/>
-      <c r="AB1" s="177"/>
-      <c r="AC1" s="177"/>
-      <c r="AD1" s="177"/>
-      <c r="AE1" s="177"/>
-      <c r="AF1" s="177"/>
-      <c r="AG1" s="177"/>
-      <c r="AH1" s="177"/>
-      <c r="AI1" s="177"/>
-      <c r="AJ1" s="177"/>
-      <c r="AK1" s="177"/>
-      <c r="AL1" s="177"/>
-      <c r="AM1" s="177"/>
-      <c r="AN1" s="177"/>
-      <c r="AO1" s="177"/>
-      <c r="AP1" s="177"/>
-      <c r="AQ1" s="177"/>
-      <c r="AR1" s="177"/>
-      <c r="AS1" s="177"/>
-      <c r="AT1" s="177"/>
-      <c r="AU1" s="177"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+      <c r="H1" s="178"/>
+      <c r="I1" s="178"/>
+      <c r="J1" s="178"/>
+      <c r="K1" s="178"/>
+      <c r="L1" s="178"/>
+      <c r="M1" s="178"/>
+      <c r="N1" s="178"/>
+      <c r="O1" s="178"/>
+      <c r="P1" s="178"/>
+      <c r="Q1" s="178"/>
+      <c r="R1" s="178"/>
+      <c r="S1" s="178"/>
+      <c r="T1" s="178"/>
+      <c r="U1" s="178"/>
+      <c r="V1" s="178"/>
+      <c r="W1" s="178"/>
+      <c r="X1" s="178"/>
+      <c r="Y1" s="178"/>
+      <c r="Z1" s="178"/>
+      <c r="AA1" s="178"/>
+      <c r="AB1" s="178"/>
+      <c r="AC1" s="178"/>
+      <c r="AD1" s="178"/>
+      <c r="AE1" s="178"/>
+      <c r="AF1" s="178"/>
+      <c r="AG1" s="178"/>
+      <c r="AH1" s="178"/>
+      <c r="AI1" s="178"/>
+      <c r="AJ1" s="178"/>
+      <c r="AK1" s="178"/>
+      <c r="AL1" s="178"/>
+      <c r="AM1" s="178"/>
+      <c r="AN1" s="178"/>
+      <c r="AO1" s="178"/>
+      <c r="AP1" s="178"/>
+      <c r="AQ1" s="178"/>
+      <c r="AR1" s="178"/>
+      <c r="AS1" s="178"/>
+      <c r="AT1" s="178"/>
+      <c r="AU1" s="178"/>
     </row>
     <row r="2" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
@@ -51257,661 +52136,4 @@
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU100"/>
-  <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4:Q6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="37.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="28.85546875" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" customWidth="1"/>
-    <col min="12" max="12" width="28.85546875" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" customWidth="1"/>
-    <col min="15" max="15" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="178" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="178"/>
-      <c r="H1" s="178"/>
-      <c r="I1" s="178"/>
-      <c r="J1" s="178"/>
-      <c r="K1" s="178"/>
-      <c r="L1" s="178"/>
-      <c r="M1" s="178"/>
-      <c r="N1" s="178"/>
-      <c r="O1" s="178"/>
-      <c r="P1" s="178"/>
-      <c r="Q1" s="178"/>
-      <c r="R1" s="178"/>
-      <c r="S1" s="178"/>
-      <c r="T1" s="178"/>
-      <c r="U1" s="178"/>
-      <c r="V1" s="178"/>
-      <c r="W1" s="178"/>
-      <c r="X1" s="178"/>
-      <c r="Y1" s="178"/>
-      <c r="Z1" s="178"/>
-      <c r="AA1" s="178"/>
-      <c r="AB1" s="178"/>
-      <c r="AC1" s="178"/>
-      <c r="AD1" s="178"/>
-      <c r="AE1" s="178"/>
-      <c r="AF1" s="178"/>
-      <c r="AG1" s="178"/>
-      <c r="AH1" s="178"/>
-      <c r="AI1" s="178"/>
-      <c r="AJ1" s="178"/>
-      <c r="AK1" s="178"/>
-      <c r="AL1" s="178"/>
-      <c r="AM1" s="178"/>
-      <c r="AN1" s="178"/>
-      <c r="AO1" s="178"/>
-      <c r="AP1" s="178"/>
-      <c r="AQ1" s="178"/>
-      <c r="AR1" s="178"/>
-      <c r="AS1" s="178"/>
-      <c r="AT1" s="178"/>
-      <c r="AU1" s="178"/>
-    </row>
-    <row r="2" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="N2" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="P2" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q2" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="R2" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="S2" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="T2" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="U2" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="V2" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="W2" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="X2" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="Y2" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z2" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA2" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB2" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC2" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD2" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE2" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="AF2" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG2" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="AI2" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ2" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK2" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL2" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="AM2" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="AN2" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="AO2" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="AP2" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="AQ2" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="AR2" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="AS2" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT2" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="AU2" s="26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="4">
-        <v>43587</v>
-      </c>
-      <c r="D3" s="4">
-        <v>43587</v>
-      </c>
-      <c r="E3" s="5">
-        <v>43587</v>
-      </c>
-      <c r="F3" s="3">
-        <v>43588</v>
-      </c>
-      <c r="G3" s="4">
-        <v>43588</v>
-      </c>
-      <c r="H3" s="5">
-        <v>43588</v>
-      </c>
-      <c r="I3" s="109">
-        <v>43591</v>
-      </c>
-      <c r="J3" s="109">
-        <v>43591</v>
-      </c>
-      <c r="K3" s="109">
-        <v>43591</v>
-      </c>
-      <c r="L3" s="3">
-        <v>43592</v>
-      </c>
-      <c r="M3" s="4">
-        <v>43592</v>
-      </c>
-      <c r="N3" s="4">
-        <v>43592</v>
-      </c>
-      <c r="O3" s="27">
-        <v>43593</v>
-      </c>
-      <c r="P3" s="28">
-        <v>43593</v>
-      </c>
-      <c r="Q3" s="28">
-        <v>43593</v>
-      </c>
-      <c r="R3" s="27"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="27"/>
-      <c r="V3" s="28"/>
-      <c r="W3" s="29"/>
-      <c r="X3" s="27"/>
-      <c r="Y3" s="28"/>
-      <c r="Z3" s="29"/>
-      <c r="AA3" s="27"/>
-      <c r="AB3" s="28"/>
-      <c r="AC3" s="29"/>
-      <c r="AD3" s="27"/>
-      <c r="AE3" s="28"/>
-      <c r="AF3" s="29"/>
-      <c r="AG3" s="27"/>
-      <c r="AH3" s="28"/>
-      <c r="AI3" s="29"/>
-      <c r="AJ3" s="27"/>
-      <c r="AK3" s="28"/>
-      <c r="AL3" s="29"/>
-      <c r="AM3" s="27"/>
-      <c r="AN3" s="28"/>
-      <c r="AO3" s="29"/>
-      <c r="AP3" s="46"/>
-      <c r="AQ3" s="46"/>
-      <c r="AR3" s="46"/>
-      <c r="AS3" s="27"/>
-      <c r="AT3" s="28"/>
-      <c r="AU3" s="29"/>
-    </row>
-    <row r="4" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="7">
-        <v>46249</v>
-      </c>
-      <c r="C4" s="119">
-        <v>4.13</v>
-      </c>
-      <c r="D4" s="66">
-        <v>36.26</v>
-      </c>
-      <c r="E4" s="134">
-        <v>3626.43</v>
-      </c>
-      <c r="F4" s="57">
-        <v>4.1100000000000003</v>
-      </c>
-      <c r="G4" s="58">
-        <v>36.33</v>
-      </c>
-      <c r="H4" s="120">
-        <v>3633.42</v>
-      </c>
-      <c r="I4" s="21">
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="J4" s="58">
-        <v>36.450000000000003</v>
-      </c>
-      <c r="K4" s="120">
-        <v>3645.27</v>
-      </c>
-      <c r="L4" s="142">
-        <v>4.07</v>
-      </c>
-      <c r="M4" s="143">
-        <v>36.44</v>
-      </c>
-      <c r="N4" s="144">
-        <v>3644.48</v>
-      </c>
-      <c r="O4" s="142">
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="P4" s="143">
-        <v>36.47</v>
-      </c>
-      <c r="Q4" s="144">
-        <v>3647.91</v>
-      </c>
-      <c r="R4" s="21"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="22"/>
-      <c r="X4" s="21"/>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="21"/>
-      <c r="AB4" s="12"/>
-      <c r="AC4" s="22"/>
-      <c r="AD4" s="21"/>
-      <c r="AE4" s="12"/>
-      <c r="AF4" s="22"/>
-      <c r="AG4" s="21"/>
-      <c r="AH4" s="12"/>
-      <c r="AI4" s="22"/>
-      <c r="AJ4" s="21"/>
-      <c r="AK4" s="12"/>
-      <c r="AL4" s="22"/>
-      <c r="AM4" s="21"/>
-      <c r="AN4" s="12"/>
-      <c r="AO4" s="22"/>
-      <c r="AP4" s="21"/>
-      <c r="AQ4" s="12"/>
-      <c r="AR4" s="12"/>
-      <c r="AS4" s="21"/>
-      <c r="AT4" s="12"/>
-      <c r="AU4" s="22"/>
-    </row>
-    <row r="5" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="7">
-        <v>49444</v>
-      </c>
-      <c r="C5" s="119">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="D5" s="66">
-        <v>39.07</v>
-      </c>
-      <c r="E5" s="134">
-        <v>3907.12</v>
-      </c>
-      <c r="F5" s="57">
-        <v>4.33</v>
-      </c>
-      <c r="G5" s="58">
-        <v>39.18</v>
-      </c>
-      <c r="H5" s="120">
-        <v>3918.25</v>
-      </c>
-      <c r="I5" s="21">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="J5" s="58">
-        <v>39.270000000000003</v>
-      </c>
-      <c r="K5" s="120">
-        <v>3927.82</v>
-      </c>
-      <c r="L5" s="145">
-        <v>4.29</v>
-      </c>
-      <c r="M5" s="141">
-        <v>39.369999999999997</v>
-      </c>
-      <c r="N5" s="146">
-        <v>3937.41</v>
-      </c>
-      <c r="O5" s="145">
-        <v>4.28</v>
-      </c>
-      <c r="P5" s="141">
-        <v>39.42</v>
-      </c>
-      <c r="Q5" s="146">
-        <v>3942.94</v>
-      </c>
-      <c r="R5" s="21"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="22"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="22"/>
-      <c r="X5" s="21"/>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="22"/>
-      <c r="AA5" s="21"/>
-      <c r="AB5" s="12"/>
-      <c r="AC5" s="22"/>
-      <c r="AD5" s="21"/>
-      <c r="AE5" s="12"/>
-      <c r="AF5" s="22"/>
-      <c r="AG5" s="21"/>
-      <c r="AH5" s="12"/>
-      <c r="AI5" s="22"/>
-      <c r="AJ5" s="21"/>
-      <c r="AK5" s="12"/>
-      <c r="AL5" s="22"/>
-      <c r="AM5" s="21"/>
-      <c r="AN5" s="12"/>
-      <c r="AO5" s="22"/>
-      <c r="AP5" s="21"/>
-      <c r="AQ5" s="12"/>
-      <c r="AR5" s="12"/>
-      <c r="AS5" s="21"/>
-      <c r="AT5" s="12"/>
-      <c r="AU5" s="22"/>
-    </row>
-    <row r="6" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="9">
-        <v>55015</v>
-      </c>
-      <c r="C6" s="121">
-        <v>4.45</v>
-      </c>
-      <c r="D6" s="122">
-        <v>40.880000000000003</v>
-      </c>
-      <c r="E6" s="135">
-        <v>4088.23</v>
-      </c>
-      <c r="F6" s="132">
-        <v>4.43</v>
-      </c>
-      <c r="G6" s="123">
-        <v>41.04</v>
-      </c>
-      <c r="H6" s="124">
-        <v>4104.07</v>
-      </c>
-      <c r="I6" s="16">
-        <v>4.42</v>
-      </c>
-      <c r="J6" s="123">
-        <v>41.11</v>
-      </c>
-      <c r="K6" s="124">
-        <v>4111.95</v>
-      </c>
-      <c r="L6" s="147">
-        <v>4.41</v>
-      </c>
-      <c r="M6" s="148">
-        <v>41.19</v>
-      </c>
-      <c r="N6" s="149">
-        <v>4119.8500000000004</v>
-      </c>
-      <c r="O6" s="147">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="P6" s="148">
-        <v>41.27</v>
-      </c>
-      <c r="Q6" s="149">
-        <v>4127.7700000000004</v>
-      </c>
-      <c r="R6" s="16"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="18"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="17"/>
-      <c r="W6" s="18"/>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="18"/>
-      <c r="AA6" s="16"/>
-      <c r="AB6" s="17"/>
-      <c r="AC6" s="18"/>
-      <c r="AD6" s="16"/>
-      <c r="AE6" s="17"/>
-      <c r="AF6" s="18"/>
-      <c r="AG6" s="16"/>
-      <c r="AH6" s="17"/>
-      <c r="AI6" s="18"/>
-      <c r="AJ6" s="16"/>
-      <c r="AK6" s="17"/>
-      <c r="AL6" s="18"/>
-      <c r="AM6" s="16"/>
-      <c r="AN6" s="17"/>
-      <c r="AO6" s="18"/>
-      <c r="AP6" s="16"/>
-      <c r="AQ6" s="17"/>
-      <c r="AR6" s="17"/>
-      <c r="AS6" s="16"/>
-      <c r="AT6" s="17"/>
-      <c r="AU6" s="18"/>
-    </row>
-    <row r="7" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:AU1"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit balanco e anexo mes marco/19 e insercao graficos em venda
</commit_message>
<xml_diff>
--- a/TESOURO DIRETO_0519 - Compra.xlsx
+++ b/TESOURO DIRETO_0519 - Compra.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" firstSheet="11" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="020519" sheetId="21" r:id="rId1"/>
@@ -1472,7 +1472,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1610,7 +1609,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1864,7 +1862,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2118,7 +2115,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2372,7 +2368,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2626,7 +2621,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2868,7 +2862,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3038,11 +3031,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="867193664"/>
-        <c:axId val="867189856"/>
+        <c:axId val="-1424308576"/>
+        <c:axId val="-1424318912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="867193664"/>
+        <c:axId val="-1424308576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3084,7 +3077,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="867189856"/>
+        <c:crossAx val="-1424318912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3092,7 +3085,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="867189856"/>
+        <c:axId val="-1424318912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3142,7 +3135,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="867193664"/>
+        <c:crossAx val="-1424308576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3156,7 +3149,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3248,7 +3240,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3353,7 +3344,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3544,8 +3534,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="867183872"/>
-        <c:axId val="867182784"/>
+        <c:axId val="-1424312384"/>
+        <c:axId val="-1424318368"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -4058,7 +4048,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="867183872"/>
+        <c:axId val="-1424312384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4092,7 +4082,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="867182784"/>
+        <c:crossAx val="-1424318368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4100,7 +4090,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="867182784"/>
+        <c:axId val="-1424318368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4110,7 +4100,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="867183872"/>
+        <c:crossAx val="-1424312384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4124,7 +4114,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4498,8 +4487,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="867187136"/>
-        <c:axId val="867194208"/>
+        <c:axId val="-1424308032"/>
+        <c:axId val="-1424311840"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -5012,7 +5001,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="867187136"/>
+        <c:axId val="-1424308032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5046,7 +5035,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="867194208"/>
+        <c:crossAx val="-1424311840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5054,7 +5043,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="867194208"/>
+        <c:axId val="-1424311840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5064,7 +5053,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="867187136"/>
+        <c:crossAx val="-1424308032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5196,7 +5185,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5322,7 +5310,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -5561,7 +5548,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -5800,7 +5786,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -5971,11 +5956,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="867188224"/>
-        <c:axId val="867189312"/>
+        <c:axId val="-1424306944"/>
+        <c:axId val="-1424306400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="867188224"/>
+        <c:axId val="-1424306944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6018,7 +6003,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="867189312"/>
+        <c:crossAx val="-1424306400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6026,7 +6011,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="867189312"/>
+        <c:axId val="-1424306400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6036,7 +6021,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="867188224"/>
+        <c:crossAx val="-1424306944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6050,7 +6035,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6426,11 +6410,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="867195296"/>
-        <c:axId val="867192032"/>
+        <c:axId val="-1589603680"/>
+        <c:axId val="-1346404624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="867195296"/>
+        <c:axId val="-1589603680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6464,7 +6448,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="867192032"/>
+        <c:crossAx val="-1346404624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6472,7 +6456,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="867192032"/>
+        <c:axId val="-1346404624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6482,7 +6466,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="867195296"/>
+        <c:crossAx val="-1589603680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6855,8 +6839,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="867192576"/>
-        <c:axId val="867195840"/>
+        <c:axId val="-1346413328"/>
+        <c:axId val="-1346412240"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -7369,7 +7353,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="867192576"/>
+        <c:axId val="-1346413328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7403,7 +7387,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="867195840"/>
+        <c:crossAx val="-1346412240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7411,7 +7395,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="867195840"/>
+        <c:axId val="-1346412240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7421,7 +7405,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="867192576"/>
+        <c:crossAx val="-1346413328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7806,8 +7790,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="867184416"/>
-        <c:axId val="868416912"/>
+        <c:axId val="-1346411152"/>
+        <c:axId val="-1346408432"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -8308,7 +8292,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="867184416"/>
+        <c:axId val="-1346411152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8342,7 +8326,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="868416912"/>
+        <c:crossAx val="-1346408432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8350,7 +8334,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="868416912"/>
+        <c:axId val="-1346408432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8360,7 +8344,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="867184416"/>
+        <c:crossAx val="-1346411152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8747,8 +8731,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="868425616"/>
-        <c:axId val="868430512"/>
+        <c:axId val="-1346402992"/>
+        <c:axId val="-1346400816"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -9249,7 +9233,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="868425616"/>
+        <c:axId val="-1346402992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9283,7 +9267,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="868430512"/>
+        <c:crossAx val="-1346400816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9291,7 +9275,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="868430512"/>
+        <c:axId val="-1346400816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9301,7 +9285,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="868425616"/>
+        <c:crossAx val="-1346402992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9677,8 +9661,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="868425072"/>
-        <c:axId val="868420720"/>
+        <c:axId val="-1346412784"/>
+        <c:axId val="-1346405168"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -10191,7 +10175,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="868425072"/>
+        <c:axId val="-1346412784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10225,7 +10209,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="868420720"/>
+        <c:crossAx val="-1346405168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10233,7 +10217,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="868420720"/>
+        <c:axId val="-1346405168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10243,7 +10227,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="868425072"/>
+        <c:crossAx val="-1346412784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10335,6 +10319,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10439,6 +10424,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -10629,11 +10615,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="868421264"/>
-        <c:axId val="868429968"/>
+        <c:axId val="-1346407888"/>
+        <c:axId val="-1346399184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="868421264"/>
+        <c:axId val="-1346407888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10667,7 +10653,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="868429968"/>
+        <c:crossAx val="-1346399184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10675,7 +10661,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="868429968"/>
+        <c:axId val="-1346399184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10685,7 +10671,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="868421264"/>
+        <c:crossAx val="-1346407888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10699,6 +10685,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10776,6 +10763,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10880,6 +10868,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -11070,8 +11059,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="868422896"/>
-        <c:axId val="868426160"/>
+        <c:axId val="-1346408976"/>
+        <c:axId val="-1346398640"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -11572,7 +11561,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="868422896"/>
+        <c:axId val="-1346408976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11606,7 +11595,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="868426160"/>
+        <c:crossAx val="-1346398640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11614,7 +11603,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="868426160"/>
+        <c:axId val="-1346398640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11624,7 +11613,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="868422896"/>
+        <c:crossAx val="-1346408976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11638,6 +11627,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12312,11 +12302,11 @@
         </c:dLbls>
         <c:gapWidth val="315"/>
         <c:overlap val="-40"/>
-        <c:axId val="867187680"/>
-        <c:axId val="867186048"/>
+        <c:axId val="-1424317824"/>
+        <c:axId val="-1424305312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="867187680"/>
+        <c:axId val="-1424317824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12377,7 +12367,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="867186048"/>
+        <c:crossAx val="-1424305312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12385,7 +12375,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="867186048"/>
+        <c:axId val="-1424305312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12446,7 +12436,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="867187680"/>
+        <c:crossAx val="-1424317824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12827,8 +12817,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="868427792"/>
-        <c:axId val="868421808"/>
+        <c:axId val="-1346404080"/>
+        <c:axId val="-1346411696"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -13341,7 +13331,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="868427792"/>
+        <c:axId val="-1346404080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13375,7 +13365,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="868421808"/>
+        <c:crossAx val="-1346411696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13383,7 +13373,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="868421808"/>
+        <c:axId val="-1346411696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13393,7 +13383,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="868427792"/>
+        <c:crossAx val="-1346404080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13781,8 +13771,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="868418544"/>
-        <c:axId val="868422352"/>
+        <c:axId val="-1346410608"/>
+        <c:axId val="-1346410064"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -14283,7 +14273,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="868418544"/>
+        <c:axId val="-1346410608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14317,7 +14307,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="868422352"/>
+        <c:crossAx val="-1346410064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14325,7 +14315,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="868422352"/>
+        <c:axId val="-1346410064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14335,7 +14325,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="868418544"/>
+        <c:crossAx val="-1346410608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14427,7 +14417,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14532,7 +14521,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -14723,8 +14711,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="868431600"/>
-        <c:axId val="868426704"/>
+        <c:axId val="-1346403536"/>
+        <c:axId val="-1346398096"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -15237,7 +15225,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="868431600"/>
+        <c:axId val="-1346403536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15271,7 +15259,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="868426704"/>
+        <c:crossAx val="-1346398096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15279,7 +15267,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="868426704"/>
+        <c:axId val="-1346398096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15289,7 +15277,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="868431600"/>
+        <c:crossAx val="-1346403536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15303,7 +15291,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15381,7 +15368,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15486,7 +15472,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -15677,8 +15662,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="868423440"/>
-        <c:axId val="868419088"/>
+        <c:axId val="-1346409520"/>
+        <c:axId val="-1346407344"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -16191,7 +16176,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="868423440"/>
+        <c:axId val="-1346409520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16225,7 +16210,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="868419088"/>
+        <c:crossAx val="-1346407344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16233,7 +16218,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="868419088"/>
+        <c:axId val="-1346407344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16243,7 +16228,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="868423440"/>
+        <c:crossAx val="-1346409520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16257,7 +16242,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16335,7 +16319,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16440,7 +16423,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -16631,8 +16613,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="868431056"/>
-        <c:axId val="868419632"/>
+        <c:axId val="-1346406800"/>
+        <c:axId val="-1346402448"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -17145,7 +17127,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="868431056"/>
+        <c:axId val="-1346406800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17179,7 +17161,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="868419632"/>
+        <c:crossAx val="-1346402448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17187,7 +17169,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="868419632"/>
+        <c:axId val="-1346402448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17197,7 +17179,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="868431056"/>
+        <c:crossAx val="-1346406800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17211,7 +17193,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17289,7 +17270,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17394,7 +17374,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -17585,8 +17564,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="868417456"/>
-        <c:axId val="868428880"/>
+        <c:axId val="-1346406256"/>
+        <c:axId val="-1346405712"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -18099,7 +18078,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="868417456"/>
+        <c:axId val="-1346406256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18133,7 +18112,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="868428880"/>
+        <c:crossAx val="-1346405712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18141,7 +18120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="868428880"/>
+        <c:axId val="-1346405712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18151,7 +18130,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="868417456"/>
+        <c:crossAx val="-1346406256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18165,7 +18144,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18243,7 +18221,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18348,7 +18325,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -18539,8 +18515,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="868428336"/>
-        <c:axId val="868423984"/>
+        <c:axId val="-1346401904"/>
+        <c:axId val="-1346401360"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -19053,7 +19029,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="868428336"/>
+        <c:axId val="-1346401904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19087,7 +19063,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="868423984"/>
+        <c:crossAx val="-1346401360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19095,7 +19071,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="868423984"/>
+        <c:axId val="-1346401360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19105,7 +19081,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="868428336"/>
+        <c:crossAx val="-1346401904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19119,7 +19095,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19197,7 +19172,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19302,7 +19276,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -19493,8 +19466,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="868424528"/>
-        <c:axId val="868418000"/>
+        <c:axId val="-1346400272"/>
+        <c:axId val="-1346399728"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -20007,7 +19980,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="868424528"/>
+        <c:axId val="-1346400272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20041,7 +20014,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="868418000"/>
+        <c:crossAx val="-1346399728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20049,7 +20022,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="868418000"/>
+        <c:axId val="-1346399728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20059,7 +20032,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="868424528"/>
+        <c:crossAx val="-1346400272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20073,7 +20046,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20445,8 +20417,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="868432144"/>
-        <c:axId val="868427248"/>
+        <c:axId val="-1344448560"/>
+        <c:axId val="-1344460528"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -20959,7 +20931,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="868432144"/>
+        <c:axId val="-1344448560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20993,7 +20965,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="868427248"/>
+        <c:crossAx val="-1344460528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21001,7 +20973,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="868427248"/>
+        <c:axId val="-1344460528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21011,7 +20983,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="868432144"/>
+        <c:crossAx val="-1344448560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21396,8 +21368,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="868429424"/>
-        <c:axId val="868420176"/>
+        <c:axId val="-1344462704"/>
+        <c:axId val="-1344454544"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -21910,7 +21882,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="868429424"/>
+        <c:axId val="-1344462704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21944,7 +21916,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="868420176"/>
+        <c:crossAx val="-1344454544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21952,7 +21924,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="868420176"/>
+        <c:axId val="-1344454544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21962,7 +21934,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="868429424"/>
+        <c:crossAx val="-1344462704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22053,7 +22025,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -22158,7 +22129,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -22349,11 +22319,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="867183328"/>
-        <c:axId val="867193120"/>
+        <c:axId val="-1424310752"/>
+        <c:axId val="-1424316192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="867183328"/>
+        <c:axId val="-1424310752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22387,7 +22357,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="867193120"/>
+        <c:crossAx val="-1424316192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22395,7 +22365,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="867193120"/>
+        <c:axId val="-1424316192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22405,7 +22375,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="867183328"/>
+        <c:crossAx val="-1424310752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22419,7 +22389,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -22791,8 +22760,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="920846048"/>
-        <c:axId val="920849856"/>
+        <c:axId val="-1344454000"/>
+        <c:axId val="-1344449648"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -23305,7 +23274,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="920846048"/>
+        <c:axId val="-1344454000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23339,7 +23308,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="920849856"/>
+        <c:crossAx val="-1344449648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23347,7 +23316,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="920849856"/>
+        <c:axId val="-1344449648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23357,7 +23326,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="920846048"/>
+        <c:crossAx val="-1344454000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23448,7 +23417,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -23563,7 +23531,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -23755,11 +23722,11 @@
         </c:dropLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="920852576"/>
-        <c:axId val="920844960"/>
+        <c:axId val="-1344451824"/>
+        <c:axId val="-1344447472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="920852576"/>
+        <c:axId val="-1344451824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23793,7 +23760,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="920844960"/>
+        <c:crossAx val="-1344447472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23801,7 +23768,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="920844960"/>
+        <c:axId val="-1344447472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23811,7 +23778,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="920852576"/>
+        <c:crossAx val="-1344451824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23874,7 +23841,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -23979,7 +23945,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -24170,11 +24135,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="920849312"/>
-        <c:axId val="920842240"/>
+        <c:axId val="-1344456176"/>
+        <c:axId val="-1344461072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="920849312"/>
+        <c:axId val="-1344456176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24208,7 +24173,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="920842240"/>
+        <c:crossAx val="-1344461072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -24216,7 +24181,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="920842240"/>
+        <c:axId val="-1344461072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24226,7 +24191,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="920849312"/>
+        <c:crossAx val="-1344456176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -24289,7 +24254,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -24394,7 +24358,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -24585,11 +24548,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="920843328"/>
-        <c:axId val="920840064"/>
+        <c:axId val="-1344453456"/>
+        <c:axId val="-1344455632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="920843328"/>
+        <c:axId val="-1344453456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24623,7 +24586,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="920840064"/>
+        <c:crossAx val="-1344455632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -24631,7 +24594,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="920840064"/>
+        <c:axId val="-1344455632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24641,7 +24604,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="920843328"/>
+        <c:crossAx val="-1344453456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -24704,7 +24667,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -24809,7 +24771,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -25000,11 +24961,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="867182240"/>
-        <c:axId val="867190944"/>
+        <c:axId val="-1424317280"/>
+        <c:axId val="-1424307488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="867182240"/>
+        <c:axId val="-1424317280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25038,7 +24999,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="867190944"/>
+        <c:crossAx val="-1424307488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25046,7 +25007,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="867190944"/>
+        <c:axId val="-1424307488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25056,7 +25017,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="867182240"/>
+        <c:crossAx val="-1424317280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -25070,7 +25031,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -25148,7 +25108,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -25253,7 +25212,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -25444,11 +25402,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="867190400"/>
-        <c:axId val="867184960"/>
+        <c:axId val="-1424315648"/>
+        <c:axId val="-1424314016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="867190400"/>
+        <c:axId val="-1424315648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25482,7 +25440,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="867184960"/>
+        <c:crossAx val="-1424314016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25490,7 +25448,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="867184960"/>
+        <c:axId val="-1424314016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25500,7 +25458,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="867190400"/>
+        <c:crossAx val="-1424315648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -25514,7 +25472,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -25592,7 +25549,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -25697,7 +25653,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -25888,11 +25843,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="867196384"/>
-        <c:axId val="867185504"/>
+        <c:axId val="-1424310208"/>
+        <c:axId val="-1424309120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="867196384"/>
+        <c:axId val="-1424310208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25926,7 +25881,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="867185504"/>
+        <c:crossAx val="-1424309120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25934,7 +25889,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="867185504"/>
+        <c:axId val="-1424309120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25944,7 +25899,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="867196384"/>
+        <c:crossAx val="-1424310208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -25958,7 +25913,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -26036,7 +25990,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -26141,7 +26094,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -26332,8 +26284,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="867196928"/>
-        <c:axId val="867188768"/>
+        <c:axId val="-1424315104"/>
+        <c:axId val="-1424313472"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -26846,7 +26798,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="867196928"/>
+        <c:axId val="-1424315104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26880,7 +26832,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="867188768"/>
+        <c:crossAx val="-1424313472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -26888,7 +26840,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="867188768"/>
+        <c:axId val="-1424313472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26898,7 +26850,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="867196928"/>
+        <c:crossAx val="-1424315104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -26912,7 +26864,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -27286,8 +27237,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="867191488"/>
-        <c:axId val="867186592"/>
+        <c:axId val="-1424314560"/>
+        <c:axId val="-1424311296"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -27800,7 +27751,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="867191488"/>
+        <c:axId val="-1424314560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27834,7 +27785,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="867186592"/>
+        <c:crossAx val="-1424311296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -27842,7 +27793,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="867186592"/>
+        <c:axId val="-1424311296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27852,7 +27803,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="867191488"/>
+        <c:crossAx val="-1424314560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -27944,7 +27895,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -28049,7 +27999,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -28240,8 +28189,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="867194752"/>
-        <c:axId val="867181696"/>
+        <c:axId val="-1424305856"/>
+        <c:axId val="-1424312928"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -28754,7 +28703,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="867194752"/>
+        <c:axId val="-1424305856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28788,7 +28737,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="867181696"/>
+        <c:crossAx val="-1424312928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -28796,7 +28745,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="867181696"/>
+        <c:axId val="-1424312928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28806,7 +28755,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="867194752"/>
+        <c:crossAx val="-1424305856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -28820,7 +28769,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -52002,7 +51950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AD4" sqref="AD4:AF6"/>
     </sheetView>
   </sheetViews>
@@ -53556,7 +53504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+    <sheetView topLeftCell="W1" workbookViewId="0">
       <selection activeCell="AD3" sqref="AD3:AF4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Atualizacao tesouro dia 16/05
</commit_message>
<xml_diff>
--- a/TESOURO DIRETO_0519 - Compra.xlsx
+++ b/TESOURO DIRETO_0519 - Compra.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" firstSheet="12" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="020519" sheetId="21" r:id="rId1"/>
@@ -22,18 +22,19 @@
     <sheet name="130519" sheetId="29" r:id="rId8"/>
     <sheet name="140519" sheetId="30" r:id="rId9"/>
     <sheet name="150519" sheetId="32" r:id="rId10"/>
-    <sheet name="COMPARAÇÃO DIA A DIA" sheetId="4" r:id="rId11"/>
-    <sheet name="TESOURO IPCA" sheetId="5" r:id="rId12"/>
-    <sheet name="TESOURO IPCA JUROS SEMESTRAIS" sheetId="6" r:id="rId13"/>
-    <sheet name="TESOURO PREFIXADOS" sheetId="7" r:id="rId14"/>
-    <sheet name="TESOURO SELIC" sheetId="8" r:id="rId15"/>
+    <sheet name="160519" sheetId="33" r:id="rId11"/>
+    <sheet name="COMPARAÇÃO DIA A DIA" sheetId="4" r:id="rId12"/>
+    <sheet name="TESOURO IPCA" sheetId="5" r:id="rId13"/>
+    <sheet name="TESOURO IPCA JUROS SEMESTRAIS" sheetId="6" r:id="rId14"/>
+    <sheet name="TESOURO PREFIXADOS" sheetId="7" r:id="rId15"/>
+    <sheet name="TESOURO SELIC" sheetId="8" r:id="rId16"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="24">
   <si>
     <t>Vencimento</t>
   </si>
@@ -1472,6 +1473,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1609,6 +1611,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1668,6 +1671,9 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1762,6 +1768,9 @@
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
                   <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>3.91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1862,6 +1871,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1921,6 +1931,9 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2014,6 +2027,9 @@
                   <c:v>4.34</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
                   <c:v>4.3</c:v>
                 </c:pt>
               </c:numCache>
@@ -2115,6 +2131,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2174,6 +2191,9 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2267,6 +2287,9 @@
                   <c:v>4.34</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
                   <c:v>4.3</c:v>
                 </c:pt>
               </c:numCache>
@@ -2368,6 +2391,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2427,6 +2451,9 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2520,6 +2547,9 @@
                   <c:v>4.0599999999999996</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
+                  <c:v>3.99</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
                   <c:v>3.99</c:v>
                 </c:pt>
               </c:numCache>
@@ -2621,6 +2651,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2680,6 +2711,9 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2761,6 +2795,9 @@
                   <c:v>4.28</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
+                  <c:v>4.22</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
                   <c:v>4.22</c:v>
                 </c:pt>
               </c:numCache>
@@ -2862,6 +2899,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2921,6 +2959,9 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -3016,6 +3057,9 @@
                 <c:pt idx="9" formatCode="General">
                   <c:v>4.33</c:v>
                 </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>4.3499999999999996</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3031,11 +3075,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="-1424308576"/>
-        <c:axId val="-1424318912"/>
+        <c:axId val="-1004207504"/>
+        <c:axId val="-1004204240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1424308576"/>
+        <c:axId val="-1004207504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3077,7 +3121,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1424318912"/>
+        <c:crossAx val="-1004204240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3085,7 +3129,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1424318912"/>
+        <c:axId val="-1004204240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3135,7 +3179,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1424308576"/>
+        <c:crossAx val="-1004207504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3149,6 +3193,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3404,6 +3449,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3498,6 +3546,9 @@
                 <c:pt idx="9" formatCode="General">
                   <c:v>3.9</c:v>
                 </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>3.91</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3534,8 +3585,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1424312384"/>
-        <c:axId val="-1424318368"/>
+        <c:axId val="-1004208048"/>
+        <c:axId val="-1244174992"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3689,6 +3740,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3783,6 +3837,9 @@
                         <c:v>4.34</c:v>
                       </c:pt>
                       <c:pt idx="9" formatCode="General">
+                        <c:v>4.3</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="General">
                         <c:v>4.3</c:v>
                       </c:pt>
                     </c:numCache>
@@ -3942,6 +3999,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4038,6 +4098,9 @@
                       <c:pt idx="9" formatCode="General">
                         <c:v>4.3</c:v>
                       </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>4.3</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4048,7 +4111,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1424312384"/>
+        <c:axId val="-1004208048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4082,7 +4145,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1424318368"/>
+        <c:crossAx val="-1244174992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4090,7 +4153,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1424318368"/>
+        <c:axId val="-1244174992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4100,7 +4163,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1424312384"/>
+        <c:crossAx val="-1004208048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4357,6 +4420,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -4451,6 +4517,9 @@
                 <c:pt idx="9">
                   <c:v>32.479999999999997</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>32.49</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4487,8 +4556,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1424308032"/>
-        <c:axId val="-1424311840"/>
+        <c:axId val="-1244174448"/>
+        <c:axId val="-1025085488"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -4642,6 +4711,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4737,6 +4809,9 @@
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>52.79</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>52.77</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4895,6 +4970,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4991,6 +5069,9 @@
                       <c:pt idx="9">
                         <c:v>32.950000000000003</c:v>
                       </c:pt>
+                      <c:pt idx="10">
+                        <c:v>32.96</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -5001,7 +5082,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1424308032"/>
+        <c:axId val="-1244174448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5035,7 +5116,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1424311840"/>
+        <c:crossAx val="-1025085488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5043,7 +5124,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1424311840"/>
+        <c:axId val="-1025085488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5053,7 +5134,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1424308032"/>
+        <c:crossAx val="-1244174448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5370,6 +5451,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -5463,6 +5547,9 @@
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
                   <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>3.91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5608,6 +5695,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -5700,6 +5790,9 @@
                   <c:v>4.34</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
                   <c:v>4.3</c:v>
                 </c:pt>
               </c:numCache>
@@ -5846,6 +5939,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -5940,6 +6036,9 @@
                 <c:pt idx="9" formatCode="General">
                   <c:v>4.3</c:v>
                 </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>4.3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5956,11 +6055,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1424306944"/>
-        <c:axId val="-1424306400"/>
+        <c:axId val="-948174672"/>
+        <c:axId val="-948162704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1424306944"/>
+        <c:axId val="-948174672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6003,7 +6102,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1424306400"/>
+        <c:crossAx val="-948162704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6011,7 +6110,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1424306400"/>
+        <c:axId val="-948162704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6021,7 +6120,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1424306944"/>
+        <c:crossAx val="-948174672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6280,6 +6379,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -6374,6 +6476,9 @@
                 <c:pt idx="9">
                   <c:v>3668.9</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>3669.81</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6410,11 +6515,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1589603680"/>
-        <c:axId val="-1346404624"/>
+        <c:axId val="-948174128"/>
+        <c:axId val="-948161616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1589603680"/>
+        <c:axId val="-948174128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6448,7 +6553,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1346404624"/>
+        <c:crossAx val="-948161616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6456,7 +6561,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1346404624"/>
+        <c:axId val="-948161616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6466,7 +6571,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1589603680"/>
+        <c:crossAx val="-948174128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6721,6 +6826,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -6802,6 +6910,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3879.04</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3880.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6839,8 +6950,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1346413328"/>
-        <c:axId val="-1346412240"/>
+        <c:axId val="-948167600"/>
+        <c:axId val="-948173584"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -6994,6 +7105,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -7089,6 +7203,9 @@
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>3668.9</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>3669.81</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -7247,6 +7364,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -7343,6 +7463,9 @@
                       <c:pt idx="9">
                         <c:v>4180.1499999999996</c:v>
                       </c:pt>
+                      <c:pt idx="10">
+                        <c:v>4168.29</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -7353,7 +7476,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1346413328"/>
+        <c:axId val="-948167600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7387,7 +7510,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1346412240"/>
+        <c:crossAx val="-948173584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7395,7 +7518,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1346412240"/>
+        <c:axId val="-948173584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7405,7 +7528,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1346413328"/>
+        <c:crossAx val="-948167600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7660,6 +7783,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -7754,6 +7880,9 @@
                 <c:pt idx="9">
                   <c:v>4180.1499999999996</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>4168.29</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7790,8 +7919,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1346411152"/>
-        <c:axId val="-1346408432"/>
+        <c:axId val="-948167056"/>
+        <c:axId val="-948171408"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -7945,6 +8074,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -8040,6 +8172,9 @@
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>3668.9</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>3669.81</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -8198,6 +8333,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -8282,6 +8420,9 @@
                       <c:pt idx="9">
                         <c:v>3879.04</c:v>
                       </c:pt>
+                      <c:pt idx="10">
+                        <c:v>3880.04</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -8292,7 +8433,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1346411152"/>
+        <c:axId val="-948167056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8326,7 +8467,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1346408432"/>
+        <c:crossAx val="-948171408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8334,7 +8475,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1346408432"/>
+        <c:axId val="-948171408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8344,7 +8485,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1346411152"/>
+        <c:crossAx val="-948167056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8601,6 +8742,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -8695,6 +8839,9 @@
                 <c:pt idx="9">
                   <c:v>41.8</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>41.68</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -8731,8 +8878,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1346402992"/>
-        <c:axId val="-1346400816"/>
+        <c:axId val="-948173040"/>
+        <c:axId val="-948172496"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -8886,6 +9033,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -8981,6 +9131,9 @@
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>36.68</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>36.69</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -9139,6 +9292,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -9223,6 +9379,9 @@
                       <c:pt idx="9">
                         <c:v>38.79</c:v>
                       </c:pt>
+                      <c:pt idx="10">
+                        <c:v>38.799999999999997</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -9233,7 +9392,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1346402992"/>
+        <c:axId val="-948173040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9267,7 +9426,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1346400816"/>
+        <c:crossAx val="-948172496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9275,7 +9434,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1346400816"/>
+        <c:axId val="-948172496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9285,7 +9444,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1346402992"/>
+        <c:crossAx val="-948173040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9543,6 +9702,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -9624,6 +9786,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>38.79</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>38.799999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9661,8 +9826,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1346412784"/>
-        <c:axId val="-1346405168"/>
+        <c:axId val="-948165968"/>
+        <c:axId val="-948166512"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -9816,6 +9981,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -9911,6 +10079,9 @@
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>36.68</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>36.69</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -10069,6 +10240,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -10165,6 +10339,9 @@
                       <c:pt idx="9">
                         <c:v>41.8</c:v>
                       </c:pt>
+                      <c:pt idx="10">
+                        <c:v>41.68</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -10175,7 +10352,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1346412784"/>
+        <c:axId val="-948165968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10209,7 +10386,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1346405168"/>
+        <c:crossAx val="-948166512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10217,7 +10394,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1346405168"/>
+        <c:axId val="-948166512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10227,7 +10404,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1346412784"/>
+        <c:crossAx val="-948165968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10485,6 +10662,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -10579,6 +10759,9 @@
                 <c:pt idx="9">
                   <c:v>36.68</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>36.69</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -10615,11 +10798,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1346407888"/>
-        <c:axId val="-1346399184"/>
+        <c:axId val="-948170864"/>
+        <c:axId val="-948165424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1346407888"/>
+        <c:axId val="-948170864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10653,7 +10836,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1346399184"/>
+        <c:crossAx val="-948165424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10661,7 +10844,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1346399184"/>
+        <c:axId val="-948165424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10671,7 +10854,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1346407888"/>
+        <c:crossAx val="-948170864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10929,6 +11112,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -11023,6 +11209,9 @@
                 <c:pt idx="9" formatCode="General">
                   <c:v>3.99</c:v>
                 </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>3.99</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -11059,8 +11248,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1346408976"/>
-        <c:axId val="-1346398640"/>
+        <c:axId val="-948159440"/>
+        <c:axId val="-948162160"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -11214,6 +11403,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -11296,6 +11488,9 @@
                         <c:v>4.28</c:v>
                       </c:pt>
                       <c:pt idx="9" formatCode="General">
+                        <c:v>4.22</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="General">
                         <c:v>4.22</c:v>
                       </c:pt>
                     </c:numCache>
@@ -11455,6 +11650,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -11551,6 +11749,9 @@
                       <c:pt idx="9" formatCode="General">
                         <c:v>4.33</c:v>
                       </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>4.3499999999999996</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -11561,7 +11762,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1346408976"/>
+        <c:axId val="-948159440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11595,7 +11796,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1346398640"/>
+        <c:crossAx val="-948162160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11603,7 +11804,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1346398640"/>
+        <c:axId val="-948162160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11613,7 +11814,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1346408976"/>
+        <c:crossAx val="-948159440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11842,6 +12043,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -11935,6 +12139,9 @@
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
                   <c:v>7.52</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>7.54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12018,6 +12225,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -12111,6 +12321,9 @@
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
                   <c:v>8.57</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>8.6300000000000008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12194,6 +12407,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -12288,6 +12504,9 @@
                 <c:pt idx="9" formatCode="General">
                   <c:v>8.7899999999999991</c:v>
                 </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>8.85</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -12302,11 +12521,11 @@
         </c:dLbls>
         <c:gapWidth val="315"/>
         <c:overlap val="-40"/>
-        <c:axId val="-1424317824"/>
-        <c:axId val="-1424305312"/>
+        <c:axId val="-1004204784"/>
+        <c:axId val="-1004203152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1424317824"/>
+        <c:axId val="-1004204784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12367,7 +12586,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1424305312"/>
+        <c:crossAx val="-1004203152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12375,7 +12594,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1424305312"/>
+        <c:axId val="-1004203152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12436,7 +12655,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1424317824"/>
+        <c:crossAx val="-1004204784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12699,6 +12918,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -12779,6 +13001,9 @@
                   <c:v>4.28</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
+                  <c:v>4.22</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
                   <c:v>4.22</c:v>
                 </c:pt>
               </c:numCache>
@@ -12817,8 +13042,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1346404080"/>
-        <c:axId val="-1346411696"/>
+        <c:axId val="-948164880"/>
+        <c:axId val="-948161072"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -12972,6 +13197,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -13066,6 +13294,9 @@
                         <c:v>4.0599999999999996</c:v>
                       </c:pt>
                       <c:pt idx="9" formatCode="General">
+                        <c:v>3.99</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="General">
                         <c:v>3.99</c:v>
                       </c:pt>
                     </c:numCache>
@@ -13225,6 +13456,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -13321,6 +13555,9 @@
                       <c:pt idx="9" formatCode="General">
                         <c:v>4.33</c:v>
                       </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>4.3499999999999996</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -13331,7 +13568,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1346404080"/>
+        <c:axId val="-948164880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13365,7 +13602,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1346411696"/>
+        <c:crossAx val="-948161072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13373,7 +13610,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1346411696"/>
+        <c:axId val="-948161072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13383,7 +13620,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1346404080"/>
+        <c:crossAx val="-948164880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13641,6 +13878,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -13735,6 +13975,9 @@
                 <c:pt idx="9" formatCode="General">
                   <c:v>4.33</c:v>
                 </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>4.3499999999999996</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -13771,8 +14014,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1346410608"/>
-        <c:axId val="-1346410064"/>
+        <c:axId val="-948163248"/>
+        <c:axId val="-948171952"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -13926,6 +14169,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -14020,6 +14266,9 @@
                         <c:v>4.0599999999999996</c:v>
                       </c:pt>
                       <c:pt idx="9" formatCode="General">
+                        <c:v>3.99</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="General">
                         <c:v>3.99</c:v>
                       </c:pt>
                     </c:numCache>
@@ -14179,6 +14428,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -14263,6 +14515,9 @@
                       <c:pt idx="9" formatCode="General">
                         <c:v>4.22</c:v>
                       </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>4.22</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -14273,7 +14528,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1346410608"/>
+        <c:axId val="-948163248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14307,7 +14562,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1346410064"/>
+        <c:crossAx val="-948171952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14315,7 +14570,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1346410064"/>
+        <c:axId val="-948171952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14325,7 +14580,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1346410608"/>
+        <c:crossAx val="-948163248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14581,6 +14836,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -14675,6 +14933,9 @@
                 <c:pt idx="9" formatCode="General">
                   <c:v>7.52</c:v>
                 </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>7.54</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -14711,8 +14972,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1346403536"/>
-        <c:axId val="-1346398096"/>
+        <c:axId val="-948164336"/>
+        <c:axId val="-948163792"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -14866,6 +15127,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -14961,6 +15225,9 @@
                       </c:pt>
                       <c:pt idx="9" formatCode="General">
                         <c:v>8.57</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>8.6300000000000008</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -15119,6 +15386,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -15215,6 +15485,9 @@
                       <c:pt idx="9" formatCode="General">
                         <c:v>8.7899999999999991</c:v>
                       </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>8.85</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -15225,7 +15498,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1346403536"/>
+        <c:axId val="-948164336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15259,7 +15532,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1346398096"/>
+        <c:crossAx val="-948163792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15267,7 +15540,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1346398096"/>
+        <c:axId val="-948163792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15277,7 +15550,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1346403536"/>
+        <c:crossAx val="-948164336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15368,6 +15641,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15472,6 +15746,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -15531,6 +15806,9 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -15626,6 +15904,9 @@
                 <c:pt idx="9" formatCode="General">
                   <c:v>8.57</c:v>
                 </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>8.6300000000000008</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -15662,8 +15943,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1346409520"/>
-        <c:axId val="-1346407344"/>
+        <c:axId val="-948160528"/>
+        <c:axId val="-948159984"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -15817,6 +16098,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -15912,6 +16196,9 @@
                       </c:pt>
                       <c:pt idx="9" formatCode="General">
                         <c:v>7.52</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>7.54</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -16070,6 +16357,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -16166,6 +16456,9 @@
                       <c:pt idx="9" formatCode="General">
                         <c:v>8.7899999999999991</c:v>
                       </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>8.85</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -16176,7 +16469,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1346409520"/>
+        <c:axId val="-948160528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16210,7 +16503,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1346407344"/>
+        <c:crossAx val="-948159984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16218,7 +16511,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1346407344"/>
+        <c:axId val="-948159984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16228,7 +16521,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1346409520"/>
+        <c:crossAx val="-948160528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16242,6 +16535,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16319,6 +16613,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16423,6 +16718,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -16482,6 +16778,9 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -16577,6 +16876,9 @@
                 <c:pt idx="9" formatCode="General">
                   <c:v>8.7899999999999991</c:v>
                 </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>8.85</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -16613,8 +16915,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1346406800"/>
-        <c:axId val="-1346402448"/>
+        <c:axId val="-948170320"/>
+        <c:axId val="-948169776"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -16768,6 +17070,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -16863,6 +17168,9 @@
                       </c:pt>
                       <c:pt idx="9" formatCode="General">
                         <c:v>7.52</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>7.54</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -17021,6 +17329,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -17117,6 +17428,9 @@
                       <c:pt idx="9" formatCode="General">
                         <c:v>8.57</c:v>
                       </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>8.6300000000000008</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -17127,7 +17441,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1346406800"/>
+        <c:axId val="-948170320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17161,7 +17475,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1346402448"/>
+        <c:crossAx val="-948169776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17169,7 +17483,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1346402448"/>
+        <c:axId val="-948169776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17179,7 +17493,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1346406800"/>
+        <c:crossAx val="-948170320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17193,6 +17507,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17434,6 +17749,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -17528,6 +17846,9 @@
                 <c:pt idx="9">
                   <c:v>33.049999999999997</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>33.04</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -17564,8 +17885,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1346406256"/>
-        <c:axId val="-1346405712"/>
+        <c:axId val="-948169232"/>
+        <c:axId val="-948168688"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -17719,6 +18040,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -17814,6 +18138,9 @@
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>31.48</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>31.4</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -17972,6 +18299,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -18068,6 +18398,9 @@
                       <c:pt idx="9">
                         <c:v>33.36</c:v>
                       </c:pt>
+                      <c:pt idx="10">
+                        <c:v>33.25</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -18078,7 +18411,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1346406256"/>
+        <c:axId val="-948169232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18112,7 +18445,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1346405712"/>
+        <c:crossAx val="-948168688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18120,7 +18453,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1346405712"/>
+        <c:axId val="-948168688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18130,7 +18463,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1346406256"/>
+        <c:crossAx val="-948169232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18221,6 +18554,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18325,6 +18659,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -18384,6 +18719,9 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -18479,6 +18817,9 @@
                 <c:pt idx="9">
                   <c:v>31.48</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>31.4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -18515,8 +18856,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1346401904"/>
-        <c:axId val="-1346401360"/>
+        <c:axId val="-948168144"/>
+        <c:axId val="-944581488"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -18670,6 +19011,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -18765,6 +19109,9 @@
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>33.049999999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>33.04</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -18923,6 +19270,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -19019,6 +19369,9 @@
                       <c:pt idx="9">
                         <c:v>33.36</c:v>
                       </c:pt>
+                      <c:pt idx="10">
+                        <c:v>33.25</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -19029,7 +19382,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1346401904"/>
+        <c:axId val="-948168144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19063,7 +19416,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1346401360"/>
+        <c:crossAx val="-944581488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19071,7 +19424,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1346401360"/>
+        <c:axId val="-944581488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19081,7 +19434,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1346401904"/>
+        <c:crossAx val="-948168144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19095,6 +19448,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19172,6 +19526,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19276,6 +19631,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -19335,6 +19691,9 @@
                   </c:pt>
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -19430,6 +19789,9 @@
                 <c:pt idx="9">
                   <c:v>33.36</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>33.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -19466,8 +19828,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1346400272"/>
-        <c:axId val="-1346399728"/>
+        <c:axId val="-944589648"/>
+        <c:axId val="-944580944"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -19621,6 +19983,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -19716,6 +20081,9 @@
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>33.049999999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>33.04</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -19874,6 +20242,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -19970,6 +20341,9 @@
                       <c:pt idx="9">
                         <c:v>31.48</c:v>
                       </c:pt>
+                      <c:pt idx="10">
+                        <c:v>31.4</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -19980,7 +20354,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1346400272"/>
+        <c:axId val="-944589648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20014,7 +20388,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1346399728"/>
+        <c:crossAx val="-944580944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20022,7 +20396,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1346399728"/>
+        <c:axId val="-944580944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20032,7 +20406,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1346400272"/>
+        <c:crossAx val="-944589648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20046,6 +20420,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20287,6 +20662,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -20381,6 +20759,9 @@
                 <c:pt idx="9">
                   <c:v>1112.1300000000001</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>1108.6099999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -20417,8 +20798,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1344448560"/>
-        <c:axId val="-1344460528"/>
+        <c:axId val="-944580400"/>
+        <c:axId val="-944590192"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -20572,6 +20953,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -20667,6 +21051,9 @@
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>826.32</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>826.16</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -20825,6 +21212,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -20921,6 +21311,9 @@
                       <c:pt idx="9">
                         <c:v>629.79999999999995</c:v>
                       </c:pt>
+                      <c:pt idx="10">
+                        <c:v>628.04999999999995</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -20931,7 +21324,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1344448560"/>
+        <c:axId val="-944580400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20965,7 +21358,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1344460528"/>
+        <c:crossAx val="-944590192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20973,7 +21366,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1344460528"/>
+        <c:axId val="-944590192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20983,7 +21376,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1344448560"/>
+        <c:crossAx val="-944580400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21238,6 +21631,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -21332,6 +21728,9 @@
                 <c:pt idx="9">
                   <c:v>629.79999999999995</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>628.04999999999995</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -21368,8 +21767,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1344462704"/>
-        <c:axId val="-1344454544"/>
+        <c:axId val="-944579856"/>
+        <c:axId val="-944590736"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -21523,6 +21922,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -21618,6 +22020,9 @@
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>826.32</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>826.16</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -21776,6 +22181,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -21872,6 +22280,9 @@
                       <c:pt idx="9">
                         <c:v>1112.1300000000001</c:v>
                       </c:pt>
+                      <c:pt idx="10">
+                        <c:v>1108.6099999999999</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -21882,7 +22293,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1344462704"/>
+        <c:axId val="-944579856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21916,7 +22327,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1344454544"/>
+        <c:crossAx val="-944590736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21924,7 +22335,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1344454544"/>
+        <c:axId val="-944590736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21934,7 +22345,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1344462704"/>
+        <c:crossAx val="-944579856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22189,6 +22600,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -22283,6 +22697,9 @@
                 <c:pt idx="9">
                   <c:v>52.79</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>52.77</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -22319,11 +22736,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1424310752"/>
-        <c:axId val="-1424316192"/>
+        <c:axId val="-1004211856"/>
+        <c:axId val="-1004203696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1424310752"/>
+        <c:axId val="-1004211856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22357,7 +22774,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1424316192"/>
+        <c:crossAx val="-1004203696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22365,7 +22782,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1424316192"/>
+        <c:axId val="-1004203696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22375,7 +22792,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1424310752"/>
+        <c:crossAx val="-1004211856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22630,6 +23047,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -22724,6 +23144,9 @@
                 <c:pt idx="9">
                   <c:v>826.32</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>826.16</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -22760,8 +23183,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1344454000"/>
-        <c:axId val="-1344449648"/>
+        <c:axId val="-944584752"/>
+        <c:axId val="-944589104"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -22915,6 +23338,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -23010,6 +23436,9 @@
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>629.79999999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>628.04999999999995</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -23168,6 +23597,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -23264,6 +23696,9 @@
                       <c:pt idx="9">
                         <c:v>1112.1300000000001</c:v>
                       </c:pt>
+                      <c:pt idx="10">
+                        <c:v>1108.6099999999999</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -23274,7 +23709,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1344454000"/>
+        <c:axId val="-944584752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23308,7 +23743,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1344449648"/>
+        <c:crossAx val="-944589104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23316,7 +23751,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1344449648"/>
+        <c:axId val="-944589104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23326,7 +23761,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1344454000"/>
+        <c:crossAx val="-944584752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23591,6 +24026,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -23685,6 +24123,9 @@
                 <c:pt idx="9" formatCode="General">
                   <c:v>0.02</c:v>
                 </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>0.02</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -23722,11 +24163,11 @@
         </c:dropLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1344451824"/>
-        <c:axId val="-1344447472"/>
+        <c:axId val="-944576048"/>
+        <c:axId val="-944579312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1344451824"/>
+        <c:axId val="-944576048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23760,7 +24201,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1344447472"/>
+        <c:crossAx val="-944579312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23768,7 +24209,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1344447472"/>
+        <c:axId val="-944579312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23778,7 +24219,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1344451824"/>
+        <c:crossAx val="-944576048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -24005,6 +24446,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -24099,6 +24543,9 @@
                 <c:pt idx="9">
                   <c:v>100.97</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>101</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -24135,11 +24582,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1344456176"/>
-        <c:axId val="-1344461072"/>
+        <c:axId val="-944588560"/>
+        <c:axId val="-944588016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1344456176"/>
+        <c:axId val="-944588560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24173,7 +24620,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1344461072"/>
+        <c:crossAx val="-944588016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -24181,7 +24628,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1344461072"/>
+        <c:axId val="-944588016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24191,7 +24638,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1344456176"/>
+        <c:crossAx val="-944588560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -24418,6 +24865,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -24512,6 +24962,9 @@
                 <c:pt idx="9">
                   <c:v>10097.59</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>10100.08</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -24548,11 +25001,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1344453456"/>
-        <c:axId val="-1344455632"/>
+        <c:axId val="-944578768"/>
+        <c:axId val="-944587472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1344453456"/>
+        <c:axId val="-944578768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24586,7 +25039,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1344455632"/>
+        <c:crossAx val="-944587472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -24594,7 +25047,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1344455632"/>
+        <c:axId val="-944587472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24604,7 +25057,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1344453456"/>
+        <c:crossAx val="-944578768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -24831,6 +25284,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -24925,6 +25381,9 @@
                 <c:pt idx="9">
                   <c:v>32.950000000000003</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>32.96</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -24961,11 +25420,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1424317280"/>
-        <c:axId val="-1424307488"/>
+        <c:axId val="-1004214032"/>
+        <c:axId val="-1004209680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1424317280"/>
+        <c:axId val="-1004214032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24999,7 +25458,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1424307488"/>
+        <c:crossAx val="-1004209680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25007,7 +25466,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1424307488"/>
+        <c:axId val="-1004209680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25017,7 +25476,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1424317280"/>
+        <c:crossAx val="-1004214032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -25272,6 +25731,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -25366,6 +25828,9 @@
                 <c:pt idx="9">
                   <c:v>1647.97</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>1648.4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -25402,11 +25867,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1424315648"/>
-        <c:axId val="-1424314016"/>
+        <c:axId val="-1004215664"/>
+        <c:axId val="-1004206416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1424315648"/>
+        <c:axId val="-1004215664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25440,7 +25905,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1424314016"/>
+        <c:crossAx val="-1004206416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25448,7 +25913,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1424314016"/>
+        <c:axId val="-1004206416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25458,7 +25923,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1424315648"/>
+        <c:crossAx val="-1004215664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -25713,6 +26178,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -25807,6 +26275,9 @@
                 <c:pt idx="9">
                   <c:v>1082.96</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>1083.24</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -25843,11 +26314,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1424310208"/>
-        <c:axId val="-1424309120"/>
+        <c:axId val="-1004210768"/>
+        <c:axId val="-1004206960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1424310208"/>
+        <c:axId val="-1004210768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25881,7 +26352,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1424309120"/>
+        <c:crossAx val="-1004206960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25889,7 +26360,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1424309120"/>
+        <c:axId val="-1004206960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25899,7 +26370,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1424310208"/>
+        <c:crossAx val="-1004210768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -26154,6 +26625,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -26248,6 +26722,9 @@
                 <c:pt idx="9">
                   <c:v>2639.5</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>2638.82</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -26284,8 +26761,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1424315104"/>
-        <c:axId val="-1424313472"/>
+        <c:axId val="-1004212944"/>
+        <c:axId val="-1004208592"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -26439,6 +26916,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -26534,6 +27014,9 @@
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>1647.97</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>1648.4</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -26692,6 +27175,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -26788,6 +27274,9 @@
                       <c:pt idx="9">
                         <c:v>1082.96</c:v>
                       </c:pt>
+                      <c:pt idx="10">
+                        <c:v>1083.24</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -26798,7 +27287,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1424315104"/>
+        <c:axId val="-1004212944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26832,7 +27321,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1424313472"/>
+        <c:crossAx val="-1004208592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -26840,7 +27329,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1424313472"/>
+        <c:axId val="-1004208592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26850,7 +27339,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1424315104"/>
+        <c:crossAx val="-1004212944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -27107,6 +27596,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -27201,6 +27693,9 @@
                 <c:pt idx="9" formatCode="General">
                   <c:v>4.3</c:v>
                 </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>4.3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -27237,8 +27732,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1424314560"/>
-        <c:axId val="-1424311296"/>
+        <c:axId val="-1004202608"/>
+        <c:axId val="-1004214576"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -27392,6 +27887,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -27487,6 +27985,9 @@
                       </c:pt>
                       <c:pt idx="9" formatCode="General">
                         <c:v>3.9</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>3.91</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -27645,6 +28146,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -27741,6 +28245,9 @@
                       <c:pt idx="9" formatCode="General">
                         <c:v>4.3</c:v>
                       </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>4.3</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -27751,7 +28258,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1424314560"/>
+        <c:axId val="-1004202608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27785,7 +28292,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1424311296"/>
+        <c:crossAx val="-1004214576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -27793,7 +28300,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1424311296"/>
+        <c:axId val="-1004214576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27803,7 +28310,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1424314560"/>
+        <c:crossAx val="-1004202608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -28059,6 +28566,9 @@
                   <c:pt idx="9">
                     <c:v>15/mai</c:v>
                   </c:pt>
+                  <c:pt idx="10">
+                    <c:v>16/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -28153,6 +28663,9 @@
                 <c:pt idx="9" formatCode="General">
                   <c:v>4.3</c:v>
                 </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>4.3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -28189,8 +28702,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1424305856"/>
-        <c:axId val="-1424312928"/>
+        <c:axId val="-1004212400"/>
+        <c:axId val="-1004213488"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -28344,6 +28857,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -28439,6 +28955,9 @@
                       </c:pt>
                       <c:pt idx="9" formatCode="General">
                         <c:v>3.9</c:v>
+                      </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>3.91</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -28597,6 +29116,9 @@
                         <c:pt idx="9">
                           <c:v>15/mai</c:v>
                         </c:pt>
+                        <c:pt idx="10">
+                          <c:v>16/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -28693,6 +29215,9 @@
                       <c:pt idx="9" formatCode="General">
                         <c:v>4.3</c:v>
                       </c:pt>
+                      <c:pt idx="10" formatCode="General">
+                        <c:v>4.3</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -28703,7 +29228,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1424305856"/>
+        <c:axId val="-1004212400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28737,7 +29262,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1424312928"/>
+        <c:crossAx val="-1004213488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -28745,7 +29270,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1424312928"/>
+        <c:axId val="-1004213488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28755,7 +29280,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1424305856"/>
+        <c:crossAx val="-1004212400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -48971,13 +49496,255 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="157" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="157" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="157" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="157" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="157" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="175" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="175"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="138" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="139">
+        <v>45519</v>
+      </c>
+      <c r="C3" s="140">
+        <v>3.91</v>
+      </c>
+      <c r="D3" s="141">
+        <v>52.77</v>
+      </c>
+      <c r="E3" s="141">
+        <v>2638.82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="138" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="139">
+        <v>49444</v>
+      </c>
+      <c r="C4" s="140">
+        <v>4.3</v>
+      </c>
+      <c r="D4" s="141">
+        <v>32.96</v>
+      </c>
+      <c r="E4" s="141">
+        <v>1648.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="138" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="139">
+        <v>53097</v>
+      </c>
+      <c r="C5" s="140">
+        <v>4.3</v>
+      </c>
+      <c r="D5" s="141">
+        <v>32.49</v>
+      </c>
+      <c r="E5" s="141">
+        <v>1083.24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="138" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="139">
+        <v>46249</v>
+      </c>
+      <c r="C6" s="140">
+        <v>3.99</v>
+      </c>
+      <c r="D6" s="141">
+        <v>36.69</v>
+      </c>
+      <c r="E6" s="141">
+        <v>3669.81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="138" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="139">
+        <v>49444</v>
+      </c>
+      <c r="C7" s="140">
+        <v>4.22</v>
+      </c>
+      <c r="D7" s="141">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="E7" s="141">
+        <v>3880.04</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="138" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="139">
+        <v>55015</v>
+      </c>
+      <c r="C8" s="140">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="D8" s="141">
+        <v>41.68</v>
+      </c>
+      <c r="E8" s="141">
+        <v>4168.29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="175" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="175"/>
+      <c r="C9" s="175"/>
+      <c r="D9" s="175"/>
+      <c r="E9" s="175"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="138" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="139">
+        <v>44562</v>
+      </c>
+      <c r="C10" s="140">
+        <v>7.54</v>
+      </c>
+      <c r="D10" s="141">
+        <v>33.04</v>
+      </c>
+      <c r="E10" s="141">
+        <v>826.16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="138" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="139">
+        <v>45658</v>
+      </c>
+      <c r="C11" s="140">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="D11" s="141">
+        <v>31.4</v>
+      </c>
+      <c r="E11" s="141">
+        <v>628.04999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="138" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="139">
+        <v>47119</v>
+      </c>
+      <c r="C12" s="140">
+        <v>8.85</v>
+      </c>
+      <c r="D12" s="141">
+        <v>33.25</v>
+      </c>
+      <c r="E12" s="141">
+        <v>1108.6099999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="175" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="175"/>
+      <c r="C13" s="175"/>
+      <c r="D13" s="175"/>
+      <c r="E13" s="175"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="138" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="139">
+        <v>45717</v>
+      </c>
+      <c r="C14" s="140">
+        <v>0.02</v>
+      </c>
+      <c r="D14" s="141">
+        <v>101</v>
+      </c>
+      <c r="E14" s="141">
+        <v>10100.08</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A13:E13"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AU100"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AD18" sqref="AD18:AF19"/>
+    <sheetView topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AG18" sqref="AG18:AI19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -49320,9 +50087,15 @@
       <c r="AF3" s="29">
         <v>43600</v>
       </c>
-      <c r="AG3" s="27"/>
-      <c r="AH3" s="28"/>
-      <c r="AI3" s="29"/>
+      <c r="AG3" s="27">
+        <v>43601</v>
+      </c>
+      <c r="AH3" s="28">
+        <v>43601</v>
+      </c>
+      <c r="AI3" s="29">
+        <v>43601</v>
+      </c>
       <c r="AJ3" s="27"/>
       <c r="AK3" s="28"/>
       <c r="AL3" s="29"/>
@@ -49433,9 +50206,15 @@
       <c r="AF4" s="144">
         <v>2639.5</v>
       </c>
-      <c r="AG4" s="21"/>
-      <c r="AH4" s="12"/>
-      <c r="AI4" s="22"/>
+      <c r="AG4" s="142">
+        <v>3.91</v>
+      </c>
+      <c r="AH4" s="143">
+        <v>52.77</v>
+      </c>
+      <c r="AI4" s="144">
+        <v>2638.82</v>
+      </c>
       <c r="AJ4" s="21"/>
       <c r="AK4" s="12"/>
       <c r="AL4" s="22"/>
@@ -49546,9 +50325,15 @@
       <c r="AF5" s="146">
         <v>1647.97</v>
       </c>
-      <c r="AG5" s="21"/>
-      <c r="AH5" s="12"/>
-      <c r="AI5" s="22"/>
+      <c r="AG5" s="145">
+        <v>4.3</v>
+      </c>
+      <c r="AH5" s="141">
+        <v>32.96</v>
+      </c>
+      <c r="AI5" s="146">
+        <v>1648.4</v>
+      </c>
       <c r="AJ5" s="21"/>
       <c r="AK5" s="12"/>
       <c r="AL5" s="22"/>
@@ -49659,9 +50444,15 @@
       <c r="AF6" s="146">
         <v>1082.96</v>
       </c>
-      <c r="AG6" s="21"/>
-      <c r="AH6" s="12"/>
-      <c r="AI6" s="22"/>
+      <c r="AG6" s="145">
+        <v>4.3</v>
+      </c>
+      <c r="AH6" s="141">
+        <v>32.49</v>
+      </c>
+      <c r="AI6" s="146">
+        <v>1083.24</v>
+      </c>
       <c r="AJ6" s="21"/>
       <c r="AK6" s="12"/>
       <c r="AL6" s="22"/>
@@ -49772,9 +50563,15 @@
       <c r="AF7" s="146">
         <v>3668.9</v>
       </c>
-      <c r="AG7" s="21"/>
-      <c r="AH7" s="12"/>
-      <c r="AI7" s="22"/>
+      <c r="AG7" s="145">
+        <v>3.99</v>
+      </c>
+      <c r="AH7" s="141">
+        <v>36.69</v>
+      </c>
+      <c r="AI7" s="146">
+        <v>3669.81</v>
+      </c>
       <c r="AJ7" s="21"/>
       <c r="AK7" s="12"/>
       <c r="AL7" s="22"/>
@@ -49861,9 +50658,15 @@
       <c r="AF8" s="146">
         <v>3879.04</v>
       </c>
-      <c r="AG8" s="21"/>
-      <c r="AH8" s="12"/>
-      <c r="AI8" s="22"/>
+      <c r="AG8" s="145">
+        <v>4.22</v>
+      </c>
+      <c r="AH8" s="141">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="AI8" s="146">
+        <v>3880.04</v>
+      </c>
       <c r="AJ8" s="21"/>
       <c r="AK8" s="12"/>
       <c r="AL8" s="22"/>
@@ -49974,9 +50777,15 @@
       <c r="AF9" s="149">
         <v>4180.1499999999996</v>
       </c>
-      <c r="AG9" s="21"/>
-      <c r="AH9" s="12"/>
-      <c r="AI9" s="22"/>
+      <c r="AG9" s="147">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="AH9" s="148">
+        <v>41.68</v>
+      </c>
+      <c r="AI9" s="149">
+        <v>4168.29</v>
+      </c>
       <c r="AJ9" s="21"/>
       <c r="AK9" s="12"/>
       <c r="AL9" s="22"/>
@@ -50279,9 +51088,15 @@
       <c r="AF12" s="29">
         <v>43600</v>
       </c>
-      <c r="AG12" s="27"/>
-      <c r="AH12" s="28"/>
-      <c r="AI12" s="29"/>
+      <c r="AG12" s="27">
+        <v>43601</v>
+      </c>
+      <c r="AH12" s="28">
+        <v>43601</v>
+      </c>
+      <c r="AI12" s="29">
+        <v>43601</v>
+      </c>
       <c r="AJ12" s="27"/>
       <c r="AK12" s="28"/>
       <c r="AL12" s="29"/>
@@ -50392,9 +51207,15 @@
       <c r="AF13" s="144">
         <v>826.32</v>
       </c>
-      <c r="AG13" s="21"/>
-      <c r="AH13" s="12"/>
-      <c r="AI13" s="22"/>
+      <c r="AG13" s="142">
+        <v>7.54</v>
+      </c>
+      <c r="AH13" s="143">
+        <v>33.04</v>
+      </c>
+      <c r="AI13" s="144">
+        <v>826.16</v>
+      </c>
       <c r="AJ13" s="21"/>
       <c r="AK13" s="12"/>
       <c r="AL13" s="22"/>
@@ -50505,9 +51326,15 @@
       <c r="AF14" s="146">
         <v>629.79999999999995</v>
       </c>
-      <c r="AG14" s="21"/>
-      <c r="AH14" s="12"/>
-      <c r="AI14" s="22"/>
+      <c r="AG14" s="145">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="AH14" s="141">
+        <v>31.4</v>
+      </c>
+      <c r="AI14" s="146">
+        <v>628.04999999999995</v>
+      </c>
       <c r="AJ14" s="21"/>
       <c r="AK14" s="12"/>
       <c r="AL14" s="22"/>
@@ -50618,9 +51445,15 @@
       <c r="AF15" s="149">
         <v>1112.1300000000001</v>
       </c>
-      <c r="AG15" s="21"/>
-      <c r="AH15" s="12"/>
-      <c r="AI15" s="22"/>
+      <c r="AG15" s="147">
+        <v>8.85</v>
+      </c>
+      <c r="AH15" s="148">
+        <v>33.25</v>
+      </c>
+      <c r="AI15" s="149">
+        <v>1108.6099999999999</v>
+      </c>
       <c r="AJ15" s="21"/>
       <c r="AK15" s="12"/>
       <c r="AL15" s="22"/>
@@ -50923,9 +51756,15 @@
       <c r="AF18" s="29">
         <v>43600</v>
       </c>
-      <c r="AG18" s="27"/>
-      <c r="AH18" s="28"/>
-      <c r="AI18" s="29"/>
+      <c r="AG18" s="27">
+        <v>43601</v>
+      </c>
+      <c r="AH18" s="28">
+        <v>43601</v>
+      </c>
+      <c r="AI18" s="29">
+        <v>43601</v>
+      </c>
       <c r="AJ18" s="27"/>
       <c r="AK18" s="28"/>
       <c r="AL18" s="29"/>
@@ -51036,9 +51875,15 @@
       <c r="AF19" s="152">
         <v>10097.59</v>
       </c>
-      <c r="AG19" s="16"/>
-      <c r="AH19" s="17"/>
-      <c r="AI19" s="18"/>
+      <c r="AG19" s="150">
+        <v>0.02</v>
+      </c>
+      <c r="AH19" s="151">
+        <v>101</v>
+      </c>
+      <c r="AI19" s="152">
+        <v>10100.08</v>
+      </c>
       <c r="AJ19" s="16"/>
       <c r="AK19" s="17"/>
       <c r="AL19" s="18"/>
@@ -51145,12 +51990,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3:AF6"/>
+    <sheetView topLeftCell="AB1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AG3" sqref="AG3:AI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -51487,9 +52332,15 @@
       <c r="AF3" s="29">
         <v>43600</v>
       </c>
-      <c r="AG3" s="43"/>
-      <c r="AH3" s="44"/>
-      <c r="AI3" s="45"/>
+      <c r="AG3" s="27">
+        <v>43601</v>
+      </c>
+      <c r="AH3" s="28">
+        <v>43601</v>
+      </c>
+      <c r="AI3" s="29">
+        <v>43601</v>
+      </c>
       <c r="AJ3" s="43"/>
       <c r="AK3" s="44"/>
       <c r="AL3" s="45"/>
@@ -51600,9 +52451,15 @@
       <c r="AF4" s="144">
         <v>2639.5</v>
       </c>
-      <c r="AG4" s="21"/>
-      <c r="AH4" s="12"/>
-      <c r="AI4" s="22"/>
+      <c r="AG4" s="142">
+        <v>3.91</v>
+      </c>
+      <c r="AH4" s="143">
+        <v>52.77</v>
+      </c>
+      <c r="AI4" s="144">
+        <v>2638.82</v>
+      </c>
       <c r="AJ4" s="21"/>
       <c r="AK4" s="12"/>
       <c r="AL4" s="22"/>
@@ -51713,9 +52570,15 @@
       <c r="AF5" s="146">
         <v>1647.97</v>
       </c>
-      <c r="AG5" s="21"/>
-      <c r="AH5" s="12"/>
-      <c r="AI5" s="22"/>
+      <c r="AG5" s="145">
+        <v>4.3</v>
+      </c>
+      <c r="AH5" s="141">
+        <v>32.96</v>
+      </c>
+      <c r="AI5" s="146">
+        <v>1648.4</v>
+      </c>
       <c r="AJ5" s="21"/>
       <c r="AK5" s="12"/>
       <c r="AL5" s="22"/>
@@ -51826,9 +52689,15 @@
       <c r="AF6" s="149">
         <v>1082.96</v>
       </c>
-      <c r="AG6" s="16"/>
-      <c r="AH6" s="17"/>
-      <c r="AI6" s="18"/>
+      <c r="AG6" s="145">
+        <v>4.3</v>
+      </c>
+      <c r="AH6" s="141">
+        <v>32.49</v>
+      </c>
+      <c r="AI6" s="146">
+        <v>1083.24</v>
+      </c>
       <c r="AJ6" s="16"/>
       <c r="AK6" s="17"/>
       <c r="AL6" s="18"/>
@@ -51946,12 +52815,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD4" sqref="AD4:AF6"/>
+    <sheetView topLeftCell="V1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AG4" sqref="AG4:AI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -52276,9 +53145,15 @@
       <c r="AF3" s="29">
         <v>43600</v>
       </c>
-      <c r="AG3" s="27"/>
-      <c r="AH3" s="28"/>
-      <c r="AI3" s="29"/>
+      <c r="AG3" s="27">
+        <v>43601</v>
+      </c>
+      <c r="AH3" s="28">
+        <v>43601</v>
+      </c>
+      <c r="AI3" s="29">
+        <v>43601</v>
+      </c>
       <c r="AJ3" s="27"/>
       <c r="AK3" s="28"/>
       <c r="AL3" s="29"/>
@@ -52389,9 +53264,15 @@
       <c r="AF4" s="144">
         <v>3668.9</v>
       </c>
-      <c r="AG4" s="21"/>
-      <c r="AH4" s="12"/>
-      <c r="AI4" s="22"/>
+      <c r="AG4" s="142">
+        <v>3.99</v>
+      </c>
+      <c r="AH4" s="143">
+        <v>36.69</v>
+      </c>
+      <c r="AI4" s="144">
+        <v>3669.81</v>
+      </c>
       <c r="AJ4" s="21"/>
       <c r="AK4" s="12"/>
       <c r="AL4" s="22"/>
@@ -52478,9 +53359,15 @@
       <c r="AF5" s="146">
         <v>3879.04</v>
       </c>
-      <c r="AG5" s="21"/>
-      <c r="AH5" s="12"/>
-      <c r="AI5" s="22"/>
+      <c r="AG5" s="145">
+        <v>4.22</v>
+      </c>
+      <c r="AH5" s="141">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="AI5" s="146">
+        <v>3880.04</v>
+      </c>
       <c r="AJ5" s="21"/>
       <c r="AK5" s="12"/>
       <c r="AL5" s="22"/>
@@ -52591,9 +53478,15 @@
       <c r="AF6" s="149">
         <v>4180.1499999999996</v>
       </c>
-      <c r="AG6" s="16"/>
-      <c r="AH6" s="17"/>
-      <c r="AI6" s="18"/>
+      <c r="AG6" s="147">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="AH6" s="148">
+        <v>41.68</v>
+      </c>
+      <c r="AI6" s="149">
+        <v>4168.29</v>
+      </c>
       <c r="AJ6" s="16"/>
       <c r="AK6" s="17"/>
       <c r="AL6" s="18"/>
@@ -52711,12 +53604,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3:AF6"/>
+    <sheetView topLeftCell="AC1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AG3" sqref="AG3:AI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -52750,6 +53643,9 @@
     <col min="27" max="27" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -53041,9 +53937,15 @@
       <c r="AF3" s="29">
         <v>43600</v>
       </c>
-      <c r="AG3" s="27"/>
-      <c r="AH3" s="28"/>
-      <c r="AI3" s="29"/>
+      <c r="AG3" s="27">
+        <v>43601</v>
+      </c>
+      <c r="AH3" s="28">
+        <v>43601</v>
+      </c>
+      <c r="AI3" s="29">
+        <v>43601</v>
+      </c>
       <c r="AJ3" s="27"/>
       <c r="AK3" s="28"/>
       <c r="AL3" s="29"/>
@@ -53154,9 +54056,15 @@
       <c r="AF4" s="144">
         <v>826.32</v>
       </c>
-      <c r="AG4" s="21"/>
-      <c r="AH4" s="12"/>
-      <c r="AI4" s="22"/>
+      <c r="AG4" s="142">
+        <v>7.54</v>
+      </c>
+      <c r="AH4" s="143">
+        <v>33.04</v>
+      </c>
+      <c r="AI4" s="144">
+        <v>826.16</v>
+      </c>
       <c r="AJ4" s="21"/>
       <c r="AK4" s="12"/>
       <c r="AL4" s="22"/>
@@ -53267,9 +54175,15 @@
       <c r="AF5" s="146">
         <v>629.79999999999995</v>
       </c>
-      <c r="AG5" s="21"/>
-      <c r="AH5" s="12"/>
-      <c r="AI5" s="22"/>
+      <c r="AG5" s="145">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="AH5" s="141">
+        <v>31.4</v>
+      </c>
+      <c r="AI5" s="146">
+        <v>628.04999999999995</v>
+      </c>
       <c r="AJ5" s="21"/>
       <c r="AK5" s="12"/>
       <c r="AL5" s="22"/>
@@ -53380,9 +54294,15 @@
       <c r="AF6" s="149">
         <v>1112.1300000000001</v>
       </c>
-      <c r="AG6" s="16"/>
-      <c r="AH6" s="17"/>
-      <c r="AI6" s="18"/>
+      <c r="AG6" s="147">
+        <v>8.85</v>
+      </c>
+      <c r="AH6" s="148">
+        <v>33.25</v>
+      </c>
+      <c r="AI6" s="149">
+        <v>1108.6099999999999</v>
+      </c>
       <c r="AJ6" s="16"/>
       <c r="AK6" s="17"/>
       <c r="AL6" s="18"/>
@@ -53500,12 +54420,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3:AF4"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AG3" sqref="AG3:AI4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -53539,6 +54459,9 @@
     <col min="27" max="27" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -53830,9 +54753,15 @@
       <c r="AF3" s="29">
         <v>43600</v>
       </c>
-      <c r="AG3" s="27"/>
-      <c r="AH3" s="28"/>
-      <c r="AI3" s="29"/>
+      <c r="AG3" s="27">
+        <v>43601</v>
+      </c>
+      <c r="AH3" s="28">
+        <v>43601</v>
+      </c>
+      <c r="AI3" s="29">
+        <v>43601</v>
+      </c>
       <c r="AJ3" s="27"/>
       <c r="AK3" s="28"/>
       <c r="AL3" s="29"/>
@@ -53943,9 +54872,15 @@
       <c r="AF4" s="152">
         <v>10097.59</v>
       </c>
-      <c r="AG4" s="16"/>
-      <c r="AH4" s="17"/>
-      <c r="AI4" s="18"/>
+      <c r="AG4" s="150">
+        <v>0.02</v>
+      </c>
+      <c r="AH4" s="151">
+        <v>101</v>
+      </c>
+      <c r="AI4" s="152">
+        <v>10100.08</v>
+      </c>
       <c r="AJ4" s="16"/>
       <c r="AK4" s="17"/>
       <c r="AL4" s="18"/>

</xml_diff>

<commit_message>
Atualizacao tesouro dia 17/05
</commit_message>
<xml_diff>
--- a/TESOURO DIRETO_0519 - Compra.xlsx
+++ b/TESOURO DIRETO_0519 - Compra.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" firstSheet="12" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" firstSheet="13" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="020519" sheetId="21" r:id="rId1"/>
@@ -23,18 +23,19 @@
     <sheet name="140519" sheetId="30" r:id="rId9"/>
     <sheet name="150519" sheetId="32" r:id="rId10"/>
     <sheet name="160519" sheetId="33" r:id="rId11"/>
-    <sheet name="COMPARAÇÃO DIA A DIA" sheetId="4" r:id="rId12"/>
-    <sheet name="TESOURO IPCA" sheetId="5" r:id="rId13"/>
-    <sheet name="TESOURO IPCA JUROS SEMESTRAIS" sheetId="6" r:id="rId14"/>
-    <sheet name="TESOURO PREFIXADOS" sheetId="7" r:id="rId15"/>
-    <sheet name="TESOURO SELIC" sheetId="8" r:id="rId16"/>
+    <sheet name="170519" sheetId="34" r:id="rId12"/>
+    <sheet name="COMPARAÇÃO DIA A DIA" sheetId="4" r:id="rId13"/>
+    <sheet name="TESOURO IPCA" sheetId="5" r:id="rId14"/>
+    <sheet name="TESOURO IPCA JUROS SEMESTRAIS" sheetId="6" r:id="rId15"/>
+    <sheet name="TESOURO PREFIXADOS" sheetId="7" r:id="rId16"/>
+    <sheet name="TESOURO SELIC" sheetId="8" r:id="rId17"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="24">
   <si>
     <t>Vencimento</t>
   </si>
@@ -867,7 +868,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="182">
+  <cellXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1410,6 +1411,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1473,7 +1480,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1611,7 +1617,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1674,6 +1679,9 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1771,6 +1779,9 @@
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
                   <c:v>3.91</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1871,7 +1882,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1934,6 +1944,9 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2031,6 +2044,9 @@
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
                   <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4.32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2131,7 +2147,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2194,6 +2209,9 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2291,6 +2309,9 @@
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
                   <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4.32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2391,7 +2412,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2454,6 +2474,9 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2551,6 +2574,9 @@
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
                   <c:v>3.99</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4.0599999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2651,7 +2677,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2714,6 +2739,9 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -2799,6 +2827,9 @@
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
                   <c:v>4.22</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2899,7 +2930,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2962,6 +2992,9 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -3060,6 +3093,9 @@
                 <c:pt idx="10" formatCode="General">
                   <c:v>4.3499999999999996</c:v>
                 </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4.3899999999999997</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3075,11 +3111,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="-1004207504"/>
-        <c:axId val="-1004204240"/>
+        <c:axId val="411557680"/>
+        <c:axId val="411558768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1004207504"/>
+        <c:axId val="411557680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3121,7 +3157,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1004204240"/>
+        <c:crossAx val="411558768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3129,7 +3165,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1004204240"/>
+        <c:axId val="411558768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3179,7 +3215,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1004207504"/>
+        <c:crossAx val="411557680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3193,7 +3229,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3452,6 +3487,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -3549,6 +3587,9 @@
                 <c:pt idx="10" formatCode="General">
                   <c:v>3.91</c:v>
                 </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3585,8 +3626,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1004208048"/>
-        <c:axId val="-1244174992"/>
+        <c:axId val="464134880"/>
+        <c:axId val="464140864"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -3743,6 +3784,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -3841,6 +3885,9 @@
                       </c:pt>
                       <c:pt idx="10" formatCode="General">
                         <c:v>4.3</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>4.32</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4002,6 +4049,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4101,6 +4151,9 @@
                       <c:pt idx="10" formatCode="General">
                         <c:v>4.3</c:v>
                       </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>4.32</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -4111,7 +4164,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1004208048"/>
+        <c:axId val="464134880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4145,7 +4198,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1244174992"/>
+        <c:crossAx val="464140864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4153,7 +4206,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1244174992"/>
+        <c:axId val="464140864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4163,7 +4216,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1004208048"/>
+        <c:crossAx val="464134880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4423,6 +4476,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -4520,6 +4576,9 @@
                 <c:pt idx="10">
                   <c:v>32.49</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>32.35</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4556,8 +4615,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1244174448"/>
-        <c:axId val="-1025085488"/>
+        <c:axId val="464127264"/>
+        <c:axId val="464137600"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -4714,6 +4773,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -4812,6 +4874,9 @@
                       </c:pt>
                       <c:pt idx="10">
                         <c:v>52.77</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>52.56</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4973,6 +5038,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -5072,6 +5140,9 @@
                       <c:pt idx="10">
                         <c:v>32.96</c:v>
                       </c:pt>
+                      <c:pt idx="11">
+                        <c:v>32.880000000000003</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -5082,7 +5153,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1244174448"/>
+        <c:axId val="464127264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5116,7 +5187,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1025085488"/>
+        <c:crossAx val="464137600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5124,7 +5195,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1025085488"/>
+        <c:axId val="464137600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5134,7 +5205,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1244174448"/>
+        <c:crossAx val="464127264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5454,6 +5525,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -5550,6 +5624,9 @@
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
                   <c:v>3.91</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5698,6 +5775,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -5794,6 +5874,9 @@
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
                   <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4.32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5942,6 +6025,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -6039,6 +6125,9 @@
                 <c:pt idx="10" formatCode="General">
                   <c:v>4.3</c:v>
                 </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4.32</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6055,11 +6144,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-948174672"/>
-        <c:axId val="-948162704"/>
+        <c:axId val="464137056"/>
+        <c:axId val="464131616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-948174672"/>
+        <c:axId val="464137056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6102,7 +6191,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-948162704"/>
+        <c:crossAx val="464131616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6110,7 +6199,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-948162704"/>
+        <c:axId val="464131616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6120,7 +6209,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-948174672"/>
+        <c:crossAx val="464137056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6382,6 +6471,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -6479,6 +6571,9 @@
                 <c:pt idx="10">
                   <c:v>3669.81</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>3656.64</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6515,11 +6610,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-948174128"/>
-        <c:axId val="-948161616"/>
+        <c:axId val="464138144"/>
+        <c:axId val="464138688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-948174128"/>
+        <c:axId val="464138144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6553,7 +6648,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-948161616"/>
+        <c:crossAx val="464138688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6561,7 +6656,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-948161616"/>
+        <c:axId val="464138688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6571,7 +6666,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-948174128"/>
+        <c:crossAx val="464138144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6829,6 +6924,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -6914,6 +7012,9 @@
                 <c:pt idx="10">
                   <c:v>3880.04</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>3869.45</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6950,8 +7051,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-948167600"/>
-        <c:axId val="-948173584"/>
+        <c:axId val="464132160"/>
+        <c:axId val="464139232"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -7108,6 +7209,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -7206,6 +7310,9 @@
                       </c:pt>
                       <c:pt idx="10">
                         <c:v>3669.81</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>3656.64</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -7367,6 +7474,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -7466,6 +7576,9 @@
                       <c:pt idx="10">
                         <c:v>4168.29</c:v>
                       </c:pt>
+                      <c:pt idx="11">
+                        <c:v>4144.42</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -7476,7 +7589,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-948167600"/>
+        <c:axId val="464132160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7510,7 +7623,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-948173584"/>
+        <c:crossAx val="464139232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7518,7 +7631,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-948173584"/>
+        <c:axId val="464139232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7528,7 +7641,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-948167600"/>
+        <c:crossAx val="464132160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7786,6 +7899,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -7883,6 +7999,9 @@
                 <c:pt idx="10">
                   <c:v>4168.29</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>4144.42</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7919,8 +8038,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-948167056"/>
-        <c:axId val="-948171408"/>
+        <c:axId val="464139776"/>
+        <c:axId val="464140320"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -8077,6 +8196,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -8175,6 +8297,9 @@
                       </c:pt>
                       <c:pt idx="10">
                         <c:v>3669.81</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>3656.64</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -8336,6 +8461,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -8423,6 +8551,9 @@
                       <c:pt idx="10">
                         <c:v>3880.04</c:v>
                       </c:pt>
+                      <c:pt idx="11">
+                        <c:v>3869.45</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -8433,7 +8564,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-948167056"/>
+        <c:axId val="464139776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8467,7 +8598,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-948171408"/>
+        <c:crossAx val="464140320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8475,7 +8606,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-948171408"/>
+        <c:axId val="464140320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8485,7 +8616,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-948167056"/>
+        <c:crossAx val="464139776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8745,6 +8876,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -8842,6 +8976,9 @@
                 <c:pt idx="10">
                   <c:v>41.68</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>41.44</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -8878,8 +9015,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-948173040"/>
-        <c:axId val="-948172496"/>
+        <c:axId val="464141408"/>
+        <c:axId val="464126176"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -9036,6 +9173,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -9134,6 +9274,9 @@
                       </c:pt>
                       <c:pt idx="10">
                         <c:v>36.69</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>36.56</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -9295,6 +9438,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -9382,6 +9528,9 @@
                       <c:pt idx="10">
                         <c:v>38.799999999999997</c:v>
                       </c:pt>
+                      <c:pt idx="11">
+                        <c:v>38.69</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -9392,7 +9541,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-948173040"/>
+        <c:axId val="464141408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9426,7 +9575,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-948172496"/>
+        <c:crossAx val="464126176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9434,7 +9583,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-948172496"/>
+        <c:axId val="464126176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9444,7 +9593,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-948173040"/>
+        <c:crossAx val="464141408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9705,6 +9854,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -9790,6 +9942,9 @@
                 <c:pt idx="10">
                   <c:v>38.799999999999997</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>38.69</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -9826,8 +9981,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-948165968"/>
-        <c:axId val="-948166512"/>
+        <c:axId val="464126720"/>
+        <c:axId val="466207696"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -9984,6 +10139,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -10082,6 +10240,9 @@
                       </c:pt>
                       <c:pt idx="10">
                         <c:v>36.69</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>36.56</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -10243,6 +10404,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -10342,6 +10506,9 @@
                       <c:pt idx="10">
                         <c:v>41.68</c:v>
                       </c:pt>
+                      <c:pt idx="11">
+                        <c:v>41.44</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -10352,7 +10519,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-948165968"/>
+        <c:axId val="464126720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10386,7 +10553,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-948166512"/>
+        <c:crossAx val="466207696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10394,7 +10561,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-948166512"/>
+        <c:axId val="466207696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10404,7 +10571,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-948165968"/>
+        <c:crossAx val="464126720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10496,7 +10663,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10601,7 +10767,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -10664,6 +10829,9 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -10762,6 +10930,9 @@
                 <c:pt idx="10">
                   <c:v>36.69</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>36.56</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -10798,11 +10969,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-948170864"/>
-        <c:axId val="-948165424"/>
+        <c:axId val="466204432"/>
+        <c:axId val="466201712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-948170864"/>
+        <c:axId val="466204432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10836,7 +11007,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-948165424"/>
+        <c:crossAx val="466201712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10844,7 +11015,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-948165424"/>
+        <c:axId val="466201712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10854,7 +11025,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-948170864"/>
+        <c:crossAx val="466204432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10868,7 +11039,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10946,7 +11116,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11051,7 +11220,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -11114,6 +11282,9 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -11212,6 +11383,9 @@
                 <c:pt idx="10" formatCode="General">
                   <c:v>3.99</c:v>
                 </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4.0599999999999996</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -11248,8 +11422,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-948159440"/>
-        <c:axId val="-948162160"/>
+        <c:axId val="466196816"/>
+        <c:axId val="466197904"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -11406,6 +11580,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -11492,6 +11669,9 @@
                       </c:pt>
                       <c:pt idx="10" formatCode="General">
                         <c:v>4.22</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>4.25</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -11653,6 +11833,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -11752,6 +11935,9 @@
                       <c:pt idx="10" formatCode="General">
                         <c:v>4.3499999999999996</c:v>
                       </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>4.3899999999999997</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -11762,7 +11948,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-948159440"/>
+        <c:axId val="466196816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11796,7 +11982,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-948162160"/>
+        <c:crossAx val="466197904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11804,7 +11990,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-948162160"/>
+        <c:axId val="466197904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11814,7 +12000,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-948159440"/>
+        <c:crossAx val="466196816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11828,7 +12014,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12046,6 +12231,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -12142,6 +12330,9 @@
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
                   <c:v>7.54</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>7.62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12228,6 +12419,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -12324,6 +12518,9 @@
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
                   <c:v>8.6300000000000008</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>8.73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12410,6 +12607,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -12507,6 +12707,9 @@
                 <c:pt idx="10" formatCode="General">
                   <c:v>8.85</c:v>
                 </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>8.94</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -12521,11 +12724,11 @@
         </c:dLbls>
         <c:gapWidth val="315"/>
         <c:overlap val="-40"/>
-        <c:axId val="-1004204784"/>
-        <c:axId val="-1004203152"/>
+        <c:axId val="411559312"/>
+        <c:axId val="175311568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1004204784"/>
+        <c:axId val="411559312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12586,7 +12789,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1004203152"/>
+        <c:crossAx val="175311568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12594,7 +12797,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1004203152"/>
+        <c:axId val="175311568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12655,7 +12858,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1004204784"/>
+        <c:crossAx val="411559312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12921,6 +13124,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -13006,6 +13212,9 @@
                 <c:pt idx="10" formatCode="General">
                   <c:v>4.22</c:v>
                 </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -13042,8 +13251,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-948164880"/>
-        <c:axId val="-948161072"/>
+        <c:axId val="466208784"/>
+        <c:axId val="466195728"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -13200,6 +13409,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -13298,6 +13510,9 @@
                       </c:pt>
                       <c:pt idx="10" formatCode="General">
                         <c:v>3.99</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>4.0599999999999996</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -13459,6 +13674,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -13558,6 +13776,9 @@
                       <c:pt idx="10" formatCode="General">
                         <c:v>4.3499999999999996</c:v>
                       </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>4.3899999999999997</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -13568,7 +13789,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-948164880"/>
+        <c:axId val="466208784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13602,7 +13823,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-948161072"/>
+        <c:crossAx val="466195728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13610,7 +13831,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-948161072"/>
+        <c:axId val="466195728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13620,7 +13841,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-948164880"/>
+        <c:crossAx val="466208784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13881,6 +14102,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -13978,6 +14202,9 @@
                 <c:pt idx="10" formatCode="General">
                   <c:v>4.3499999999999996</c:v>
                 </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4.3899999999999997</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -14014,8 +14241,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-948163248"/>
-        <c:axId val="-948171952"/>
+        <c:axId val="466198448"/>
+        <c:axId val="466198992"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -14172,6 +14399,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -14270,6 +14500,9 @@
                       </c:pt>
                       <c:pt idx="10" formatCode="General">
                         <c:v>3.99</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>4.0599999999999996</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -14431,6 +14664,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -14518,6 +14754,9 @@
                       <c:pt idx="10" formatCode="General">
                         <c:v>4.22</c:v>
                       </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>4.25</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -14528,7 +14767,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-948163248"/>
+        <c:axId val="466198448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14562,7 +14801,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-948171952"/>
+        <c:crossAx val="466198992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14570,7 +14809,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-948171952"/>
+        <c:axId val="466198992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14580,7 +14819,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-948163248"/>
+        <c:crossAx val="466198448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14839,6 +15078,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -14936,6 +15178,9 @@
                 <c:pt idx="10" formatCode="General">
                   <c:v>7.54</c:v>
                 </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>7.62</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -14972,8 +15217,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-948164336"/>
-        <c:axId val="-948163792"/>
+        <c:axId val="466207152"/>
+        <c:axId val="466203344"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -15130,6 +15375,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -15228,6 +15476,9 @@
                       </c:pt>
                       <c:pt idx="10" formatCode="General">
                         <c:v>8.6300000000000008</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>8.73</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -15389,6 +15640,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -15488,6 +15742,9 @@
                       <c:pt idx="10" formatCode="General">
                         <c:v>8.85</c:v>
                       </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>8.94</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -15498,7 +15755,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-948164336"/>
+        <c:axId val="466207152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15532,7 +15789,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-948163792"/>
+        <c:crossAx val="466203344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15540,7 +15797,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-948163792"/>
+        <c:axId val="466203344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15550,7 +15807,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-948164336"/>
+        <c:crossAx val="466207152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15641,7 +15898,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15746,7 +16002,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -15809,6 +16064,9 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -15907,6 +16165,9 @@
                 <c:pt idx="10" formatCode="General">
                   <c:v>8.6300000000000008</c:v>
                 </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>8.73</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -15943,8 +16204,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-948160528"/>
-        <c:axId val="-948159984"/>
+        <c:axId val="466205520"/>
+        <c:axId val="466195184"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -16101,6 +16362,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -16199,6 +16463,9 @@
                       </c:pt>
                       <c:pt idx="10" formatCode="General">
                         <c:v>7.54</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>7.62</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -16360,6 +16627,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -16459,6 +16729,9 @@
                       <c:pt idx="10" formatCode="General">
                         <c:v>8.85</c:v>
                       </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>8.94</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -16469,7 +16742,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-948160528"/>
+        <c:axId val="466205520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16503,7 +16776,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-948159984"/>
+        <c:crossAx val="466195184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16511,7 +16784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-948159984"/>
+        <c:axId val="466195184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16521,7 +16794,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-948160528"/>
+        <c:crossAx val="466205520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16535,7 +16808,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16782,6 +17054,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -16879,6 +17154,9 @@
                 <c:pt idx="10" formatCode="General">
                   <c:v>8.85</c:v>
                 </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>8.94</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -16915,8 +17193,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-948170320"/>
-        <c:axId val="-948169776"/>
+        <c:axId val="466208240"/>
+        <c:axId val="466194640"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -17073,6 +17351,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -17171,6 +17452,9 @@
                       </c:pt>
                       <c:pt idx="10" formatCode="General">
                         <c:v>7.54</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>7.62</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -17332,6 +17616,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -17431,6 +17718,9 @@
                       <c:pt idx="10" formatCode="General">
                         <c:v>8.6300000000000008</c:v>
                       </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>8.73</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -17441,7 +17731,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-948170320"/>
+        <c:axId val="466208240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17475,7 +17765,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-948169776"/>
+        <c:crossAx val="466194640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17483,7 +17773,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-948169776"/>
+        <c:axId val="466194640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17493,7 +17783,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-948170320"/>
+        <c:crossAx val="466208240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17752,6 +18042,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -17849,6 +18142,9 @@
                 <c:pt idx="10">
                   <c:v>33.04</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>32.99</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -17885,8 +18181,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-948169232"/>
-        <c:axId val="-948168688"/>
+        <c:axId val="466196272"/>
+        <c:axId val="466197360"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -18043,6 +18339,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -18141,6 +18440,9 @@
                       </c:pt>
                       <c:pt idx="10">
                         <c:v>31.4</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>31.25</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -18302,6 +18604,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -18401,6 +18706,9 @@
                       <c:pt idx="10">
                         <c:v>33.25</c:v>
                       </c:pt>
+                      <c:pt idx="11">
+                        <c:v>33.090000000000003</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -18411,7 +18719,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-948169232"/>
+        <c:axId val="466196272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18445,7 +18753,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-948168688"/>
+        <c:crossAx val="466197360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18453,7 +18761,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-948168688"/>
+        <c:axId val="466197360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18463,7 +18771,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-948169232"/>
+        <c:crossAx val="466196272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18554,7 +18862,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18659,7 +18966,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -18722,6 +19028,9 @@
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -18820,6 +19129,9 @@
                 <c:pt idx="10">
                   <c:v>31.4</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>31.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -18856,8 +19168,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-948168144"/>
-        <c:axId val="-944581488"/>
+        <c:axId val="466209328"/>
+        <c:axId val="466199536"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -19014,6 +19326,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -19112,6 +19427,9 @@
                       </c:pt>
                       <c:pt idx="10">
                         <c:v>33.04</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>32.99</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -19273,6 +19591,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -19372,6 +19693,9 @@
                       <c:pt idx="10">
                         <c:v>33.25</c:v>
                       </c:pt>
+                      <c:pt idx="11">
+                        <c:v>33.090000000000003</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -19382,7 +19706,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-948168144"/>
+        <c:axId val="466209328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19416,7 +19740,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-944581488"/>
+        <c:crossAx val="466199536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19424,7 +19748,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-944581488"/>
+        <c:axId val="466199536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19434,7 +19758,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-948168144"/>
+        <c:crossAx val="466209328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19448,7 +19772,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19695,6 +20018,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -19792,6 +20118,9 @@
                 <c:pt idx="10">
                   <c:v>33.25</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>33.090000000000003</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -19828,8 +20157,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-944589648"/>
-        <c:axId val="-944580944"/>
+        <c:axId val="466200080"/>
+        <c:axId val="466203888"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -19986,6 +20315,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -20084,6 +20416,9 @@
                       </c:pt>
                       <c:pt idx="10">
                         <c:v>33.04</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>32.99</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -20245,6 +20580,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -20344,6 +20682,9 @@
                       <c:pt idx="10">
                         <c:v>31.4</c:v>
                       </c:pt>
+                      <c:pt idx="11">
+                        <c:v>31.25</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -20354,7 +20695,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-944589648"/>
+        <c:axId val="466200080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20388,7 +20729,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-944580944"/>
+        <c:crossAx val="466203888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20396,7 +20737,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-944580944"/>
+        <c:axId val="466203888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20406,7 +20747,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-944589648"/>
+        <c:crossAx val="466200080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20665,6 +21006,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -20762,6 +21106,9 @@
                 <c:pt idx="10">
                   <c:v>1108.6099999999999</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>1103.2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -20798,8 +21145,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-944580400"/>
-        <c:axId val="-944590192"/>
+        <c:axId val="466200624"/>
+        <c:axId val="466206064"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -20956,6 +21303,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -21054,6 +21404,9 @@
                       </c:pt>
                       <c:pt idx="10">
                         <c:v>826.16</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>824.79</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -21215,6 +21568,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -21314,6 +21670,9 @@
                       <c:pt idx="10">
                         <c:v>628.04999999999995</c:v>
                       </c:pt>
+                      <c:pt idx="11">
+                        <c:v>625.02</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -21324,7 +21683,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-944580400"/>
+        <c:axId val="466200624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21358,7 +21717,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-944590192"/>
+        <c:crossAx val="466206064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21366,7 +21725,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-944590192"/>
+        <c:axId val="466206064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21376,7 +21735,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-944580400"/>
+        <c:crossAx val="466200624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21634,6 +21993,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -21731,6 +22093,9 @@
                 <c:pt idx="10">
                   <c:v>628.04999999999995</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>625.02</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -21767,8 +22132,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-944579856"/>
-        <c:axId val="-944590736"/>
+        <c:axId val="466202256"/>
+        <c:axId val="466201168"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -21925,6 +22290,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -22023,6 +22391,9 @@
                       </c:pt>
                       <c:pt idx="10">
                         <c:v>826.16</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>824.79</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -22184,6 +22555,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -22283,6 +22657,9 @@
                       <c:pt idx="10">
                         <c:v>1108.6099999999999</c:v>
                       </c:pt>
+                      <c:pt idx="11">
+                        <c:v>1103.2</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -22293,7 +22670,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-944579856"/>
+        <c:axId val="466202256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22327,7 +22704,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-944590736"/>
+        <c:crossAx val="466201168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22335,7 +22712,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-944590736"/>
+        <c:axId val="466201168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22345,7 +22722,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-944579856"/>
+        <c:crossAx val="466202256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22603,6 +22980,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -22700,6 +23080,9 @@
                 <c:pt idx="10">
                   <c:v>52.77</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>52.56</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -22736,11 +23119,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1004211856"/>
-        <c:axId val="-1004203696"/>
+        <c:axId val="464129440"/>
+        <c:axId val="464135968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1004211856"/>
+        <c:axId val="464129440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22774,7 +23157,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1004203696"/>
+        <c:crossAx val="464135968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22782,7 +23165,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1004203696"/>
+        <c:axId val="464135968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22792,7 +23175,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1004211856"/>
+        <c:crossAx val="464129440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23050,6 +23433,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -23147,6 +23533,9 @@
                 <c:pt idx="10">
                   <c:v>826.16</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>824.79</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -23183,8 +23572,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-944584752"/>
-        <c:axId val="-944589104"/>
+        <c:axId val="466202800"/>
+        <c:axId val="466204976"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -23341,6 +23730,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -23439,6 +23831,9 @@
                       </c:pt>
                       <c:pt idx="10">
                         <c:v>628.04999999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>625.02</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -23600,6 +23995,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -23699,6 +24097,9 @@
                       <c:pt idx="10">
                         <c:v>1108.6099999999999</c:v>
                       </c:pt>
+                      <c:pt idx="11">
+                        <c:v>1103.2</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -23709,7 +24110,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-944584752"/>
+        <c:axId val="466202800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23743,7 +24144,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-944589104"/>
+        <c:crossAx val="466204976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23751,7 +24152,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-944589104"/>
+        <c:axId val="466204976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23761,7 +24162,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-944584752"/>
+        <c:crossAx val="466202800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -24029,6 +24430,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -24126,6 +24530,9 @@
                 <c:pt idx="10" formatCode="General">
                   <c:v>0.02</c:v>
                 </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>0.02</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -24163,11 +24570,11 @@
         </c:dropLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-944576048"/>
-        <c:axId val="-944579312"/>
+        <c:axId val="466206608"/>
+        <c:axId val="466209872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-944576048"/>
+        <c:axId val="466206608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24201,7 +24608,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-944579312"/>
+        <c:crossAx val="466209872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -24209,7 +24616,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-944579312"/>
+        <c:axId val="466209872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24219,7 +24626,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-944576048"/>
+        <c:crossAx val="466206608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -24449,6 +24856,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -24546,6 +24956,9 @@
                 <c:pt idx="10">
                   <c:v>101</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>101.02</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -24582,11 +24995,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-944588560"/>
-        <c:axId val="-944588016"/>
+        <c:axId val="468032192"/>
+        <c:axId val="468034912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-944588560"/>
+        <c:axId val="468032192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24620,7 +25033,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-944588016"/>
+        <c:crossAx val="468034912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -24628,7 +25041,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-944588016"/>
+        <c:axId val="468034912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24638,7 +25051,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-944588560"/>
+        <c:crossAx val="468032192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -24868,6 +25281,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -24965,6 +25381,9 @@
                 <c:pt idx="10">
                   <c:v>10100.08</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>10102.58</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -25001,11 +25420,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-944578768"/>
-        <c:axId val="-944587472"/>
+        <c:axId val="468041984"/>
+        <c:axId val="468034368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-944578768"/>
+        <c:axId val="468041984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25039,7 +25458,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-944587472"/>
+        <c:crossAx val="468034368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25047,7 +25466,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-944587472"/>
+        <c:axId val="468034368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25057,7 +25476,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-944578768"/>
+        <c:crossAx val="468041984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -25287,6 +25706,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -25384,6 +25806,9 @@
                 <c:pt idx="10">
                   <c:v>32.96</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>32.880000000000003</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -25420,11 +25845,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1004214032"/>
-        <c:axId val="-1004209680"/>
+        <c:axId val="464129984"/>
+        <c:axId val="464135424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1004214032"/>
+        <c:axId val="464129984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25458,7 +25883,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1004209680"/>
+        <c:crossAx val="464135424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25466,7 +25891,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1004209680"/>
+        <c:axId val="464135424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25476,7 +25901,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1004214032"/>
+        <c:crossAx val="464129984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -25734,6 +26159,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -25831,6 +26259,9 @@
                 <c:pt idx="10">
                   <c:v>1648.4</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>1644.1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -25867,11 +26298,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1004215664"/>
-        <c:axId val="-1004206416"/>
+        <c:axId val="464132704"/>
+        <c:axId val="464127808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1004215664"/>
+        <c:axId val="464132704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25905,7 +26336,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1004206416"/>
+        <c:crossAx val="464127808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25913,7 +26344,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1004206416"/>
+        <c:axId val="464127808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25923,7 +26354,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1004215664"/>
+        <c:crossAx val="464132704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -26181,6 +26612,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -26278,6 +26712,9 @@
                 <c:pt idx="10">
                   <c:v>1083.24</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>1078.3599999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -26314,11 +26751,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1004210768"/>
-        <c:axId val="-1004206960"/>
+        <c:axId val="464130528"/>
+        <c:axId val="464134336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1004210768"/>
+        <c:axId val="464130528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26352,7 +26789,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1004206960"/>
+        <c:crossAx val="464134336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -26360,7 +26797,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1004206960"/>
+        <c:axId val="464134336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26370,7 +26807,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1004210768"/>
+        <c:crossAx val="464130528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -26628,6 +27065,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -26725,6 +27165,9 @@
                 <c:pt idx="10">
                   <c:v>2638.82</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>2628.03</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -26761,8 +27204,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1004212944"/>
-        <c:axId val="-1004208592"/>
+        <c:axId val="464133248"/>
+        <c:axId val="464136512"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -26919,6 +27362,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -27017,6 +27463,9 @@
                       </c:pt>
                       <c:pt idx="10">
                         <c:v>1648.4</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>1644.1</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -27178,6 +27627,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -27277,6 +27729,9 @@
                       <c:pt idx="10">
                         <c:v>1083.24</c:v>
                       </c:pt>
+                      <c:pt idx="11">
+                        <c:v>1078.3599999999999</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -27287,7 +27742,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1004212944"/>
+        <c:axId val="464133248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27321,7 +27776,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1004208592"/>
+        <c:crossAx val="464136512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -27329,7 +27784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1004208592"/>
+        <c:axId val="464136512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27339,7 +27794,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1004212944"/>
+        <c:crossAx val="464133248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -27599,6 +28054,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -27696,6 +28154,9 @@
                 <c:pt idx="10" formatCode="General">
                   <c:v>4.3</c:v>
                 </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4.32</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -27732,8 +28193,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1004202608"/>
-        <c:axId val="-1004214576"/>
+        <c:axId val="464128352"/>
+        <c:axId val="464128896"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -27890,6 +28351,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -27988,6 +28452,9 @@
                       </c:pt>
                       <c:pt idx="10" formatCode="General">
                         <c:v>3.91</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>4</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -28149,6 +28616,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -28248,6 +28718,9 @@
                       <c:pt idx="10" formatCode="General">
                         <c:v>4.3</c:v>
                       </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>4.32</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -28258,7 +28731,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1004202608"/>
+        <c:axId val="464128352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28292,7 +28765,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1004214576"/>
+        <c:crossAx val="464128896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -28300,7 +28773,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1004214576"/>
+        <c:axId val="464128896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28310,7 +28783,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1004202608"/>
+        <c:crossAx val="464128352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -28569,6 +29042,9 @@
                   <c:pt idx="10">
                     <c:v>16/mai</c:v>
                   </c:pt>
+                  <c:pt idx="11">
+                    <c:v>17/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -28666,6 +29142,9 @@
                 <c:pt idx="10" formatCode="General">
                   <c:v>4.3</c:v>
                 </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>4.32</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -28702,8 +29181,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-1004212400"/>
-        <c:axId val="-1004213488"/>
+        <c:axId val="464133792"/>
+        <c:axId val="464131072"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -28860,6 +29339,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -28958,6 +29440,9 @@
                       </c:pt>
                       <c:pt idx="10" formatCode="General">
                         <c:v>3.91</c:v>
+                      </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>4</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -29119,6 +29604,9 @@
                         <c:pt idx="10">
                           <c:v>16/mai</c:v>
                         </c:pt>
+                        <c:pt idx="11">
+                          <c:v>17/mai</c:v>
+                        </c:pt>
                       </c:lvl>
                       <c:lvl>
                         <c:pt idx="0">
@@ -29218,6 +29706,9 @@
                       <c:pt idx="10" formatCode="General">
                         <c:v>4.3</c:v>
                       </c:pt>
+                      <c:pt idx="11" formatCode="General">
+                        <c:v>4.32</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -29228,7 +29719,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1004212400"/>
+        <c:axId val="464133792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -29262,7 +29753,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1004213488"/>
+        <c:crossAx val="464131072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -29270,7 +29761,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1004213488"/>
+        <c:axId val="464131072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -29280,7 +29771,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1004212400"/>
+        <c:crossAx val="464133792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -49738,13 +50229,255 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="157" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="157" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="157" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="157" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="157" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="182" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="183"/>
+      <c r="C2" s="183"/>
+      <c r="D2" s="183"/>
+      <c r="E2" s="183"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="138" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="139">
+        <v>45519</v>
+      </c>
+      <c r="C3" s="140">
+        <v>4</v>
+      </c>
+      <c r="D3" s="141">
+        <v>52.56</v>
+      </c>
+      <c r="E3" s="141">
+        <v>2628.03</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="138" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="139">
+        <v>49444</v>
+      </c>
+      <c r="C4" s="140">
+        <v>4.32</v>
+      </c>
+      <c r="D4" s="141">
+        <v>32.880000000000003</v>
+      </c>
+      <c r="E4" s="141">
+        <v>1644.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="138" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="139">
+        <v>53097</v>
+      </c>
+      <c r="C5" s="140">
+        <v>4.32</v>
+      </c>
+      <c r="D5" s="141">
+        <v>32.35</v>
+      </c>
+      <c r="E5" s="141">
+        <v>1078.3599999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="138" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="139">
+        <v>46249</v>
+      </c>
+      <c r="C6" s="140">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="D6" s="141">
+        <v>36.56</v>
+      </c>
+      <c r="E6" s="141">
+        <v>3656.64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="138" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="139">
+        <v>49444</v>
+      </c>
+      <c r="C7" s="140">
+        <v>4.25</v>
+      </c>
+      <c r="D7" s="141">
+        <v>38.69</v>
+      </c>
+      <c r="E7" s="141">
+        <v>3869.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="138" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="139">
+        <v>55015</v>
+      </c>
+      <c r="C8" s="140">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="D8" s="141">
+        <v>41.44</v>
+      </c>
+      <c r="E8" s="141">
+        <v>4144.42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="182" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="183"/>
+      <c r="C9" s="183"/>
+      <c r="D9" s="183"/>
+      <c r="E9" s="183"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="138" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="139">
+        <v>44562</v>
+      </c>
+      <c r="C10" s="140">
+        <v>7.62</v>
+      </c>
+      <c r="D10" s="141">
+        <v>32.99</v>
+      </c>
+      <c r="E10" s="141">
+        <v>824.79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="138" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="139">
+        <v>45658</v>
+      </c>
+      <c r="C11" s="140">
+        <v>8.73</v>
+      </c>
+      <c r="D11" s="141">
+        <v>31.25</v>
+      </c>
+      <c r="E11" s="141">
+        <v>625.02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="138" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="139">
+        <v>47119</v>
+      </c>
+      <c r="C12" s="140">
+        <v>8.94</v>
+      </c>
+      <c r="D12" s="141">
+        <v>33.090000000000003</v>
+      </c>
+      <c r="E12" s="141">
+        <v>1103.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="182" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="183"/>
+      <c r="C13" s="183"/>
+      <c r="D13" s="183"/>
+      <c r="E13" s="183"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="138" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="139">
+        <v>45717</v>
+      </c>
+      <c r="C14" s="140">
+        <v>0.02</v>
+      </c>
+      <c r="D14" s="141">
+        <v>101.02</v>
+      </c>
+      <c r="E14" s="141">
+        <v>10102.58</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B13:E13"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AU100"/>
   <sheetViews>
-    <sheetView topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AG18" sqref="AG18:AI19"/>
+    <sheetView topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AJ18" sqref="AJ18:AL19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -50096,9 +50829,15 @@
       <c r="AI3" s="29">
         <v>43601</v>
       </c>
-      <c r="AJ3" s="27"/>
-      <c r="AK3" s="28"/>
-      <c r="AL3" s="29"/>
+      <c r="AJ3" s="27">
+        <v>43602</v>
+      </c>
+      <c r="AK3" s="28">
+        <v>43602</v>
+      </c>
+      <c r="AL3" s="29">
+        <v>43602</v>
+      </c>
       <c r="AM3" s="27"/>
       <c r="AN3" s="28"/>
       <c r="AO3" s="28"/>
@@ -50215,9 +50954,15 @@
       <c r="AI4" s="144">
         <v>2638.82</v>
       </c>
-      <c r="AJ4" s="21"/>
-      <c r="AK4" s="12"/>
-      <c r="AL4" s="22"/>
+      <c r="AJ4" s="142">
+        <v>4</v>
+      </c>
+      <c r="AK4" s="143">
+        <v>52.56</v>
+      </c>
+      <c r="AL4" s="144">
+        <v>2628.03</v>
+      </c>
       <c r="AM4" s="21"/>
       <c r="AN4" s="12"/>
       <c r="AO4" s="12"/>
@@ -50334,9 +51079,15 @@
       <c r="AI5" s="146">
         <v>1648.4</v>
       </c>
-      <c r="AJ5" s="21"/>
-      <c r="AK5" s="12"/>
-      <c r="AL5" s="22"/>
+      <c r="AJ5" s="145">
+        <v>4.32</v>
+      </c>
+      <c r="AK5" s="141">
+        <v>32.880000000000003</v>
+      </c>
+      <c r="AL5" s="146">
+        <v>1644.1</v>
+      </c>
       <c r="AM5" s="21"/>
       <c r="AN5" s="12"/>
       <c r="AO5" s="12"/>
@@ -50453,9 +51204,15 @@
       <c r="AI6" s="146">
         <v>1083.24</v>
       </c>
-      <c r="AJ6" s="21"/>
-      <c r="AK6" s="12"/>
-      <c r="AL6" s="22"/>
+      <c r="AJ6" s="145">
+        <v>4.32</v>
+      </c>
+      <c r="AK6" s="141">
+        <v>32.35</v>
+      </c>
+      <c r="AL6" s="146">
+        <v>1078.3599999999999</v>
+      </c>
       <c r="AM6" s="21"/>
       <c r="AN6" s="12"/>
       <c r="AO6" s="12"/>
@@ -50572,9 +51329,15 @@
       <c r="AI7" s="146">
         <v>3669.81</v>
       </c>
-      <c r="AJ7" s="21"/>
-      <c r="AK7" s="12"/>
-      <c r="AL7" s="22"/>
+      <c r="AJ7" s="145">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="AK7" s="141">
+        <v>36.56</v>
+      </c>
+      <c r="AL7" s="146">
+        <v>3656.64</v>
+      </c>
       <c r="AM7" s="21"/>
       <c r="AN7" s="12"/>
       <c r="AO7" s="12"/>
@@ -50667,9 +51430,15 @@
       <c r="AI8" s="146">
         <v>3880.04</v>
       </c>
-      <c r="AJ8" s="21"/>
-      <c r="AK8" s="12"/>
-      <c r="AL8" s="22"/>
+      <c r="AJ8" s="145">
+        <v>4.25</v>
+      </c>
+      <c r="AK8" s="141">
+        <v>38.69</v>
+      </c>
+      <c r="AL8" s="146">
+        <v>3869.45</v>
+      </c>
       <c r="AM8" s="21"/>
       <c r="AN8" s="12"/>
       <c r="AO8" s="12"/>
@@ -50786,9 +51555,15 @@
       <c r="AI9" s="149">
         <v>4168.29</v>
       </c>
-      <c r="AJ9" s="21"/>
-      <c r="AK9" s="12"/>
-      <c r="AL9" s="22"/>
+      <c r="AJ9" s="147">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="AK9" s="148">
+        <v>41.44</v>
+      </c>
+      <c r="AL9" s="149">
+        <v>4144.42</v>
+      </c>
       <c r="AM9" s="21"/>
       <c r="AN9" s="12"/>
       <c r="AO9" s="12"/>
@@ -51097,9 +51872,15 @@
       <c r="AI12" s="29">
         <v>43601</v>
       </c>
-      <c r="AJ12" s="27"/>
-      <c r="AK12" s="28"/>
-      <c r="AL12" s="29"/>
+      <c r="AJ12" s="27">
+        <v>43602</v>
+      </c>
+      <c r="AK12" s="28">
+        <v>43602</v>
+      </c>
+      <c r="AL12" s="29">
+        <v>43602</v>
+      </c>
       <c r="AM12" s="27"/>
       <c r="AN12" s="28"/>
       <c r="AO12" s="28"/>
@@ -51216,9 +51997,15 @@
       <c r="AI13" s="144">
         <v>826.16</v>
       </c>
-      <c r="AJ13" s="21"/>
-      <c r="AK13" s="12"/>
-      <c r="AL13" s="22"/>
+      <c r="AJ13" s="142">
+        <v>7.62</v>
+      </c>
+      <c r="AK13" s="143">
+        <v>32.99</v>
+      </c>
+      <c r="AL13" s="144">
+        <v>824.79</v>
+      </c>
       <c r="AM13" s="21"/>
       <c r="AN13" s="12"/>
       <c r="AO13" s="12"/>
@@ -51335,9 +52122,15 @@
       <c r="AI14" s="146">
         <v>628.04999999999995</v>
       </c>
-      <c r="AJ14" s="21"/>
-      <c r="AK14" s="12"/>
-      <c r="AL14" s="22"/>
+      <c r="AJ14" s="145">
+        <v>8.73</v>
+      </c>
+      <c r="AK14" s="141">
+        <v>31.25</v>
+      </c>
+      <c r="AL14" s="146">
+        <v>625.02</v>
+      </c>
       <c r="AM14" s="21"/>
       <c r="AN14" s="12"/>
       <c r="AO14" s="12"/>
@@ -51454,9 +52247,15 @@
       <c r="AI15" s="149">
         <v>1108.6099999999999</v>
       </c>
-      <c r="AJ15" s="21"/>
-      <c r="AK15" s="12"/>
-      <c r="AL15" s="22"/>
+      <c r="AJ15" s="147">
+        <v>8.94</v>
+      </c>
+      <c r="AK15" s="148">
+        <v>33.090000000000003</v>
+      </c>
+      <c r="AL15" s="149">
+        <v>1103.2</v>
+      </c>
       <c r="AM15" s="21"/>
       <c r="AN15" s="12"/>
       <c r="AO15" s="12"/>
@@ -51765,9 +52564,15 @@
       <c r="AI18" s="29">
         <v>43601</v>
       </c>
-      <c r="AJ18" s="27"/>
-      <c r="AK18" s="28"/>
-      <c r="AL18" s="29"/>
+      <c r="AJ18" s="27">
+        <v>43602</v>
+      </c>
+      <c r="AK18" s="28">
+        <v>43602</v>
+      </c>
+      <c r="AL18" s="29">
+        <v>43602</v>
+      </c>
       <c r="AM18" s="27"/>
       <c r="AN18" s="28"/>
       <c r="AO18" s="28"/>
@@ -51884,9 +52689,15 @@
       <c r="AI19" s="152">
         <v>10100.08</v>
       </c>
-      <c r="AJ19" s="16"/>
-      <c r="AK19" s="17"/>
-      <c r="AL19" s="18"/>
+      <c r="AJ19" s="150">
+        <v>0.02</v>
+      </c>
+      <c r="AK19" s="151">
+        <v>101.02</v>
+      </c>
+      <c r="AL19" s="152">
+        <v>10102.58</v>
+      </c>
       <c r="AM19" s="16"/>
       <c r="AN19" s="17"/>
       <c r="AO19" s="17"/>
@@ -51990,12 +52801,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>
-    <sheetView topLeftCell="AB1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AG3" sqref="AG3:AI6"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AM4" sqref="AM4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -52035,12 +52846,18 @@
     <col min="33" max="33" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="28.85546875" customWidth="1"/>
     <col min="37" max="37" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -52341,9 +53158,15 @@
       <c r="AI3" s="29">
         <v>43601</v>
       </c>
-      <c r="AJ3" s="43"/>
-      <c r="AK3" s="44"/>
-      <c r="AL3" s="45"/>
+      <c r="AJ3" s="27">
+        <v>43602</v>
+      </c>
+      <c r="AK3" s="28">
+        <v>43602</v>
+      </c>
+      <c r="AL3" s="29">
+        <v>43602</v>
+      </c>
       <c r="AM3" s="43"/>
       <c r="AN3" s="44"/>
       <c r="AO3" s="45"/>
@@ -52460,9 +53283,15 @@
       <c r="AI4" s="144">
         <v>2638.82</v>
       </c>
-      <c r="AJ4" s="21"/>
-      <c r="AK4" s="12"/>
-      <c r="AL4" s="22"/>
+      <c r="AJ4" s="142">
+        <v>4</v>
+      </c>
+      <c r="AK4" s="143">
+        <v>52.56</v>
+      </c>
+      <c r="AL4" s="144">
+        <v>2628.03</v>
+      </c>
       <c r="AM4" s="21"/>
       <c r="AN4" s="12"/>
       <c r="AO4" s="22"/>
@@ -52579,9 +53408,15 @@
       <c r="AI5" s="146">
         <v>1648.4</v>
       </c>
-      <c r="AJ5" s="21"/>
-      <c r="AK5" s="12"/>
-      <c r="AL5" s="22"/>
+      <c r="AJ5" s="145">
+        <v>4.32</v>
+      </c>
+      <c r="AK5" s="141">
+        <v>32.880000000000003</v>
+      </c>
+      <c r="AL5" s="146">
+        <v>1644.1</v>
+      </c>
       <c r="AM5" s="21"/>
       <c r="AN5" s="12"/>
       <c r="AO5" s="22"/>
@@ -52689,18 +53524,24 @@
       <c r="AF6" s="149">
         <v>1082.96</v>
       </c>
-      <c r="AG6" s="145">
+      <c r="AG6" s="147">
         <v>4.3</v>
       </c>
-      <c r="AH6" s="141">
+      <c r="AH6" s="148">
         <v>32.49</v>
       </c>
-      <c r="AI6" s="146">
+      <c r="AI6" s="149">
         <v>1083.24</v>
       </c>
-      <c r="AJ6" s="16"/>
-      <c r="AK6" s="17"/>
-      <c r="AL6" s="18"/>
+      <c r="AJ6" s="147">
+        <v>4.32</v>
+      </c>
+      <c r="AK6" s="148">
+        <v>32.35</v>
+      </c>
+      <c r="AL6" s="149">
+        <v>1078.3599999999999</v>
+      </c>
       <c r="AM6" s="16"/>
       <c r="AN6" s="17"/>
       <c r="AO6" s="18"/>
@@ -52815,12 +53656,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>
     <sheetView topLeftCell="V1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AG4" sqref="AG4:AI6"/>
+      <selection sqref="A1:AU1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -52854,6 +53695,24 @@
     <col min="27" max="27" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -53154,9 +54013,15 @@
       <c r="AI3" s="29">
         <v>43601</v>
       </c>
-      <c r="AJ3" s="27"/>
-      <c r="AK3" s="28"/>
-      <c r="AL3" s="29"/>
+      <c r="AJ3" s="27">
+        <v>43602</v>
+      </c>
+      <c r="AK3" s="28">
+        <v>43602</v>
+      </c>
+      <c r="AL3" s="29">
+        <v>43602</v>
+      </c>
       <c r="AM3" s="27"/>
       <c r="AN3" s="28"/>
       <c r="AO3" s="29"/>
@@ -53273,9 +54138,15 @@
       <c r="AI4" s="144">
         <v>3669.81</v>
       </c>
-      <c r="AJ4" s="21"/>
-      <c r="AK4" s="12"/>
-      <c r="AL4" s="22"/>
+      <c r="AJ4" s="142">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="AK4" s="143">
+        <v>36.56</v>
+      </c>
+      <c r="AL4" s="144">
+        <v>3656.64</v>
+      </c>
       <c r="AM4" s="21"/>
       <c r="AN4" s="12"/>
       <c r="AO4" s="22"/>
@@ -53368,9 +54239,15 @@
       <c r="AI5" s="146">
         <v>3880.04</v>
       </c>
-      <c r="AJ5" s="21"/>
-      <c r="AK5" s="12"/>
-      <c r="AL5" s="22"/>
+      <c r="AJ5" s="145">
+        <v>4.25</v>
+      </c>
+      <c r="AK5" s="141">
+        <v>38.69</v>
+      </c>
+      <c r="AL5" s="146">
+        <v>3869.45</v>
+      </c>
       <c r="AM5" s="21"/>
       <c r="AN5" s="12"/>
       <c r="AO5" s="22"/>
@@ -53487,9 +54364,15 @@
       <c r="AI6" s="149">
         <v>4168.29</v>
       </c>
-      <c r="AJ6" s="16"/>
-      <c r="AK6" s="17"/>
-      <c r="AL6" s="18"/>
+      <c r="AJ6" s="147">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="AK6" s="148">
+        <v>41.44</v>
+      </c>
+      <c r="AL6" s="149">
+        <v>4144.42</v>
+      </c>
       <c r="AM6" s="16"/>
       <c r="AN6" s="17"/>
       <c r="AO6" s="18"/>
@@ -53604,32 +54487,32 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>
     <sheetView topLeftCell="AC1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AG3" sqref="AG3:AI6"/>
+      <selection activeCell="AJ2" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.85546875" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="28.85546875" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -53643,9 +54526,24 @@
     <col min="27" max="27" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -53946,9 +54844,15 @@
       <c r="AI3" s="29">
         <v>43601</v>
       </c>
-      <c r="AJ3" s="27"/>
-      <c r="AK3" s="28"/>
-      <c r="AL3" s="29"/>
+      <c r="AJ3" s="27">
+        <v>43602</v>
+      </c>
+      <c r="AK3" s="28">
+        <v>43602</v>
+      </c>
+      <c r="AL3" s="29">
+        <v>43602</v>
+      </c>
       <c r="AM3" s="27"/>
       <c r="AN3" s="28"/>
       <c r="AO3" s="29"/>
@@ -54065,9 +54969,15 @@
       <c r="AI4" s="144">
         <v>826.16</v>
       </c>
-      <c r="AJ4" s="21"/>
-      <c r="AK4" s="12"/>
-      <c r="AL4" s="22"/>
+      <c r="AJ4" s="142">
+        <v>7.62</v>
+      </c>
+      <c r="AK4" s="143">
+        <v>32.99</v>
+      </c>
+      <c r="AL4" s="144">
+        <v>824.79</v>
+      </c>
       <c r="AM4" s="21"/>
       <c r="AN4" s="12"/>
       <c r="AO4" s="22"/>
@@ -54184,9 +55094,15 @@
       <c r="AI5" s="146">
         <v>628.04999999999995</v>
       </c>
-      <c r="AJ5" s="21"/>
-      <c r="AK5" s="12"/>
-      <c r="AL5" s="22"/>
+      <c r="AJ5" s="145">
+        <v>8.73</v>
+      </c>
+      <c r="AK5" s="141">
+        <v>31.25</v>
+      </c>
+      <c r="AL5" s="146">
+        <v>625.02</v>
+      </c>
       <c r="AM5" s="21"/>
       <c r="AN5" s="12"/>
       <c r="AO5" s="22"/>
@@ -54303,9 +55219,15 @@
       <c r="AI6" s="149">
         <v>1108.6099999999999</v>
       </c>
-      <c r="AJ6" s="16"/>
-      <c r="AK6" s="17"/>
-      <c r="AL6" s="18"/>
+      <c r="AJ6" s="147">
+        <v>8.94</v>
+      </c>
+      <c r="AK6" s="148">
+        <v>33.090000000000003</v>
+      </c>
+      <c r="AL6" s="149">
+        <v>1103.2</v>
+      </c>
       <c r="AM6" s="16"/>
       <c r="AN6" s="17"/>
       <c r="AO6" s="18"/>
@@ -54420,12 +55342,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AG3" sqref="AG3:AI4"/>
+    <sheetView topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AJ3" sqref="AJ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -54459,9 +55381,24 @@
     <col min="27" max="27" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -54762,9 +55699,15 @@
       <c r="AI3" s="29">
         <v>43601</v>
       </c>
-      <c r="AJ3" s="27"/>
-      <c r="AK3" s="28"/>
-      <c r="AL3" s="29"/>
+      <c r="AJ3" s="27">
+        <v>43602</v>
+      </c>
+      <c r="AK3" s="28">
+        <v>43602</v>
+      </c>
+      <c r="AL3" s="29">
+        <v>43602</v>
+      </c>
       <c r="AM3" s="27"/>
       <c r="AN3" s="28"/>
       <c r="AO3" s="29"/>
@@ -54881,9 +55824,15 @@
       <c r="AI4" s="152">
         <v>10100.08</v>
       </c>
-      <c r="AJ4" s="16"/>
-      <c r="AK4" s="17"/>
-      <c r="AL4" s="18"/>
+      <c r="AJ4" s="150">
+        <v>0.02</v>
+      </c>
+      <c r="AK4" s="151">
+        <v>101.02</v>
+      </c>
+      <c r="AL4" s="152">
+        <v>10102.58</v>
+      </c>
       <c r="AM4" s="16"/>
       <c r="AN4" s="17"/>
       <c r="AO4" s="18"/>

</xml_diff>

<commit_message>
Criado planilha acompanhamento titulo
</commit_message>
<xml_diff>
--- a/TESOURO DIRETO_0519 - Compra.xlsx
+++ b/TESOURO DIRETO_0519 - Compra.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" firstSheet="14" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" firstSheet="10" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="020519" sheetId="21" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <sheet name="TESOURO PREFIXADOS" sheetId="7" r:id="rId17"/>
     <sheet name="TESOURO SELIC" sheetId="8" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1346,6 +1346,9 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="2" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1420,9 +1423,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3161,11 +3161,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="1401518992"/>
-        <c:axId val="1401520624"/>
+        <c:axId val="397891648"/>
+        <c:axId val="226988752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1401518992"/>
+        <c:axId val="397891648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3207,7 +3207,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1401520624"/>
+        <c:crossAx val="226988752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3215,7 +3215,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1401520624"/>
+        <c:axId val="226988752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3265,7 +3265,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1401518992"/>
+        <c:crossAx val="397891648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3683,8 +3683,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1632666656"/>
-        <c:axId val="1632670464"/>
+        <c:axId val="476690496"/>
+        <c:axId val="476689408"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -4233,7 +4233,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1632666656"/>
+        <c:axId val="476690496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4267,7 +4267,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1632670464"/>
+        <c:crossAx val="476689408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4275,7 +4275,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1632670464"/>
+        <c:axId val="476689408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4285,7 +4285,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1632666656"/>
+        <c:crossAx val="476690496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4376,7 +4376,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4481,7 +4480,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4690,8 +4688,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1632665568"/>
-        <c:axId val="1632666112"/>
+        <c:axId val="476693216"/>
+        <c:axId val="476679616"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -5240,7 +5238,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1632665568"/>
+        <c:axId val="476693216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5274,7 +5272,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1632666112"/>
+        <c:crossAx val="476679616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5282,7 +5280,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1632666112"/>
+        <c:axId val="476679616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5292,7 +5290,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1632665568"/>
+        <c:crossAx val="476693216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5306,7 +5304,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6249,11 +6246,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1632667200"/>
-        <c:axId val="1632658496"/>
+        <c:axId val="476689952"/>
+        <c:axId val="476679072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1632667200"/>
+        <c:axId val="476689952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6296,7 +6293,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1632658496"/>
+        <c:crossAx val="476679072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6304,7 +6301,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1632658496"/>
+        <c:axId val="476679072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6314,7 +6311,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1632667200"/>
+        <c:crossAx val="476689952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6721,11 +6718,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1632668288"/>
-        <c:axId val="1632661760"/>
+        <c:axId val="476693760"/>
+        <c:axId val="476681792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1632668288"/>
+        <c:axId val="476693760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6759,7 +6756,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1632661760"/>
+        <c:crossAx val="476681792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6767,7 +6764,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1632661760"/>
+        <c:axId val="476681792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6777,7 +6774,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1632668288"/>
+        <c:crossAx val="476693760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7168,8 +7165,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1632662848"/>
-        <c:axId val="1632671008"/>
+        <c:axId val="476691040"/>
+        <c:axId val="476691584"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -7718,7 +7715,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1632662848"/>
+        <c:axId val="476691040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7752,7 +7749,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1632671008"/>
+        <c:crossAx val="476691584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7760,7 +7757,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1632671008"/>
+        <c:axId val="476691584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7770,7 +7767,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1632662848"/>
+        <c:crossAx val="476691040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8173,8 +8170,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1632668832"/>
-        <c:axId val="1632671552"/>
+        <c:axId val="476692128"/>
+        <c:axId val="476692672"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -8711,7 +8708,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1632668832"/>
+        <c:axId val="476692128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8745,7 +8742,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1632671552"/>
+        <c:crossAx val="476692672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8753,7 +8750,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1632671552"/>
+        <c:axId val="476692672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8763,7 +8760,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1632668832"/>
+        <c:crossAx val="476692128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8854,7 +8851,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8959,7 +8955,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -9168,8 +9163,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1632672096"/>
-        <c:axId val="1644755808"/>
+        <c:axId val="476681248"/>
+        <c:axId val="480314336"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -9706,7 +9701,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1632672096"/>
+        <c:axId val="476681248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9740,7 +9735,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1644755808"/>
+        <c:crossAx val="480314336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9748,7 +9743,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1644755808"/>
+        <c:axId val="480314336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9758,7 +9753,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1632672096"/>
+        <c:crossAx val="476681248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9772,7 +9767,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9850,7 +9844,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9955,7 +9948,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -10152,8 +10144,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1644759616"/>
-        <c:axId val="1644748736"/>
+        <c:axId val="480313248"/>
+        <c:axId val="480324128"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -10702,7 +10694,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1644759616"/>
+        <c:axId val="480313248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10736,7 +10728,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1644748736"/>
+        <c:crossAx val="480324128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10744,7 +10736,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1644748736"/>
+        <c:axId val="480324128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10754,7 +10746,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1644759616"/>
+        <c:crossAx val="480313248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10768,7 +10760,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11158,11 +11149,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1644757440"/>
-        <c:axId val="1644754720"/>
+        <c:axId val="480312160"/>
+        <c:axId val="480309984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1644757440"/>
+        <c:axId val="480312160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11196,7 +11187,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1644754720"/>
+        <c:crossAx val="480309984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11204,7 +11195,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1644754720"/>
+        <c:axId val="480309984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11214,7 +11205,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1644757440"/>
+        <c:crossAx val="480312160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11617,8 +11608,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1644753632"/>
-        <c:axId val="1644750368"/>
+        <c:axId val="480320864"/>
+        <c:axId val="480321408"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -12155,7 +12146,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1644753632"/>
+        <c:axId val="480320864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12189,7 +12180,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1644750368"/>
+        <c:crossAx val="480321408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12197,7 +12188,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1644750368"/>
+        <c:axId val="480321408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12207,7 +12198,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1644753632"/>
+        <c:crossAx val="480320864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12949,11 +12940,11 @@
         </c:dLbls>
         <c:gapWidth val="315"/>
         <c:overlap val="-40"/>
-        <c:axId val="1632660672"/>
-        <c:axId val="1632663936"/>
+        <c:axId val="476682336"/>
+        <c:axId val="476682880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1632660672"/>
+        <c:axId val="476682336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13014,7 +13005,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1632663936"/>
+        <c:crossAx val="476682880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13022,7 +13013,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1632663936"/>
+        <c:axId val="476682880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13083,7 +13074,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1632660672"/>
+        <c:crossAx val="476682336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13180,7 +13171,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13285,7 +13275,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -13482,8 +13471,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1644744384"/>
-        <c:axId val="1644756896"/>
+        <c:axId val="480323584"/>
+        <c:axId val="480311616"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -14032,7 +14021,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1644744384"/>
+        <c:axId val="480323584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14066,7 +14055,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1644756896"/>
+        <c:crossAx val="480311616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14074,7 +14063,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1644756896"/>
+        <c:axId val="480311616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14084,7 +14073,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1644744384"/>
+        <c:crossAx val="480323584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14098,7 +14087,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14176,7 +14164,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14281,7 +14268,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -14490,8 +14476,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1644754176"/>
-        <c:axId val="1644756352"/>
+        <c:axId val="480309440"/>
+        <c:axId val="480312704"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -15028,7 +15014,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1644754176"/>
+        <c:axId val="480309440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15062,7 +15048,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1644756352"/>
+        <c:crossAx val="480312704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15070,7 +15056,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1644756352"/>
+        <c:axId val="480312704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15080,7 +15066,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1644754176"/>
+        <c:crossAx val="480309440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15094,7 +15080,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15484,8 +15469,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1644747104"/>
-        <c:axId val="1644744928"/>
+        <c:axId val="480310528"/>
+        <c:axId val="480319232"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -16034,7 +16019,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1644747104"/>
+        <c:axId val="480310528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16068,7 +16053,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1644744928"/>
+        <c:crossAx val="480319232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16076,7 +16061,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1644744928"/>
+        <c:axId val="480319232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16086,7 +16071,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1644747104"/>
+        <c:crossAx val="480310528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16489,8 +16474,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1644750912"/>
-        <c:axId val="1644757984"/>
+        <c:axId val="480313792"/>
+        <c:axId val="480319776"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -17039,7 +17024,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1644750912"/>
+        <c:axId val="480313792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17073,7 +17058,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1644757984"/>
+        <c:crossAx val="480319776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17081,7 +17066,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1644757984"/>
+        <c:axId val="480319776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17091,7 +17076,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1644750912"/>
+        <c:crossAx val="480313792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17182,7 +17167,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17287,7 +17271,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -17496,8 +17479,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1644749280"/>
-        <c:axId val="1644745472"/>
+        <c:axId val="480316512"/>
+        <c:axId val="480320320"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -18046,7 +18029,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1644749280"/>
+        <c:axId val="480316512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18080,7 +18063,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1644745472"/>
+        <c:crossAx val="480320320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18088,7 +18071,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1644745472"/>
+        <c:axId val="480320320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18098,7 +18081,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1644749280"/>
+        <c:crossAx val="480316512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18112,7 +18095,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18502,8 +18484,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1644758528"/>
-        <c:axId val="1644755264"/>
+        <c:axId val="480314880"/>
+        <c:axId val="480315424"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -19052,7 +19034,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1644758528"/>
+        <c:axId val="480314880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19086,7 +19068,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1644755264"/>
+        <c:crossAx val="480315424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19094,7 +19076,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1644755264"/>
+        <c:axId val="480315424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19104,7 +19086,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1644758528"/>
+        <c:crossAx val="480314880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19507,8 +19489,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1644759072"/>
-        <c:axId val="1644747648"/>
+        <c:axId val="480324672"/>
+        <c:axId val="480321952"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -20057,7 +20039,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1644759072"/>
+        <c:axId val="480324672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20091,7 +20073,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1644747648"/>
+        <c:crossAx val="480321952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20099,7 +20081,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1644747648"/>
+        <c:axId val="480321952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20109,7 +20091,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1644759072"/>
+        <c:crossAx val="480324672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20200,7 +20182,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20305,7 +20286,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -20514,8 +20494,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1644752000"/>
-        <c:axId val="1644746016"/>
+        <c:axId val="480315968"/>
+        <c:axId val="480317056"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -21064,7 +21044,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1644752000"/>
+        <c:axId val="480315968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21098,7 +21078,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1644746016"/>
+        <c:crossAx val="480317056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -21106,7 +21086,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1644746016"/>
+        <c:axId val="480317056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21116,7 +21096,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1644752000"/>
+        <c:crossAx val="480315968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21130,7 +21110,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21520,8 +21499,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1644746560"/>
-        <c:axId val="1644748192"/>
+        <c:axId val="480318688"/>
+        <c:axId val="480322496"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -22070,7 +22049,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1644746560"/>
+        <c:axId val="480318688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22104,7 +22083,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1644748192"/>
+        <c:crossAx val="480322496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22112,7 +22091,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1644748192"/>
+        <c:axId val="480322496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22122,7 +22101,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1644746560"/>
+        <c:crossAx val="480318688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22525,8 +22504,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1644749824"/>
-        <c:axId val="1644751456"/>
+        <c:axId val="480323040"/>
+        <c:axId val="480317600"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -23075,7 +23054,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1644749824"/>
+        <c:axId val="480323040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23109,7 +23088,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1644751456"/>
+        <c:crossAx val="480317600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23117,7 +23096,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1644751456"/>
+        <c:axId val="480317600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23127,7 +23106,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1644749824"/>
+        <c:crossAx val="480323040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23530,11 +23509,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1632665024"/>
-        <c:axId val="1632659584"/>
+        <c:axId val="476688864"/>
+        <c:axId val="476685600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1632665024"/>
+        <c:axId val="476688864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23568,7 +23547,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1632659584"/>
+        <c:crossAx val="476685600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23576,7 +23555,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1632659584"/>
+        <c:axId val="476685600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23586,7 +23565,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1632665024"/>
+        <c:crossAx val="476688864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23989,8 +23968,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1644752544"/>
-        <c:axId val="1644753088"/>
+        <c:axId val="480318144"/>
+        <c:axId val="480311072"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -24539,7 +24518,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1644752544"/>
+        <c:axId val="480318144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24573,7 +24552,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1644753088"/>
+        <c:crossAx val="480311072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -24581,7 +24560,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1644753088"/>
+        <c:axId val="480311072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24591,7 +24570,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1644752544"/>
+        <c:crossAx val="480318144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -25007,11 +24986,11 @@
         </c:dropLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1647624656"/>
-        <c:axId val="1647633904"/>
+        <c:axId val="477968432"/>
+        <c:axId val="477969520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1647624656"/>
+        <c:axId val="477968432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25045,7 +25024,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1647633904"/>
+        <c:crossAx val="477969520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25053,7 +25032,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1647633904"/>
+        <c:axId val="477969520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25063,7 +25042,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1647624656"/>
+        <c:crossAx val="477968432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -25440,11 +25419,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1647626288"/>
-        <c:axId val="1647621392"/>
+        <c:axId val="477978768"/>
+        <c:axId val="477973328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1647626288"/>
+        <c:axId val="477978768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25478,7 +25457,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1647621392"/>
+        <c:crossAx val="477973328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25486,7 +25465,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1647621392"/>
+        <c:axId val="477973328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25496,7 +25475,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1647626288"/>
+        <c:crossAx val="477978768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -25873,11 +25852,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1647624112"/>
-        <c:axId val="1647632272"/>
+        <c:axId val="477968976"/>
+        <c:axId val="477975504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1647624112"/>
+        <c:axId val="477968976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25911,7 +25890,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1647632272"/>
+        <c:crossAx val="477975504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25919,7 +25898,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1647632272"/>
+        <c:axId val="477975504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25929,7 +25908,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1647624112"/>
+        <c:crossAx val="477968976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -26304,11 +26283,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1632669376"/>
-        <c:axId val="1632662304"/>
+        <c:axId val="476685056"/>
+        <c:axId val="476680160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1632669376"/>
+        <c:axId val="476685056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26342,7 +26321,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1632662304"/>
+        <c:crossAx val="476680160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -26350,7 +26329,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1632662304"/>
+        <c:axId val="476680160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26360,7 +26339,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1632669376"/>
+        <c:crossAx val="476685056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -26763,11 +26742,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1632667744"/>
-        <c:axId val="1632672640"/>
+        <c:axId val="476683424"/>
+        <c:axId val="476678528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1632667744"/>
+        <c:axId val="476683424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26801,7 +26780,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1632672640"/>
+        <c:crossAx val="476678528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -26809,7 +26788,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1632672640"/>
+        <c:axId val="476678528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26819,7 +26798,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1632667744"/>
+        <c:crossAx val="476683424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -27222,11 +27201,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1632657408"/>
-        <c:axId val="1632659040"/>
+        <c:axId val="476684512"/>
+        <c:axId val="476683968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1632657408"/>
+        <c:axId val="476684512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27260,7 +27239,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1632659040"/>
+        <c:crossAx val="476683968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -27268,7 +27247,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1632659040"/>
+        <c:axId val="476683968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27278,7 +27257,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1632657408"/>
+        <c:crossAx val="476684512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -27681,8 +27660,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1632661216"/>
-        <c:axId val="1632664480"/>
+        <c:axId val="476680704"/>
+        <c:axId val="476686144"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -28231,7 +28210,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1632661216"/>
+        <c:axId val="476680704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28265,7 +28244,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1632664480"/>
+        <c:crossAx val="476686144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -28273,7 +28252,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1632664480"/>
+        <c:axId val="476686144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28283,7 +28262,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1632661216"/>
+        <c:crossAx val="476680704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -28374,7 +28353,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -28479,7 +28457,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -28688,8 +28665,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1632660128"/>
-        <c:axId val="1632657952"/>
+        <c:axId val="476688320"/>
+        <c:axId val="476686688"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -29238,7 +29215,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1632660128"/>
+        <c:axId val="476688320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -29272,7 +29249,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1632657952"/>
+        <c:crossAx val="476686688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -29280,7 +29257,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1632657952"/>
+        <c:axId val="476686688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -29290,7 +29267,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1632660128"/>
+        <c:crossAx val="476688320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -29304,7 +29281,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -29694,8 +29670,8 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="1632669920"/>
-        <c:axId val="1632663392"/>
+        <c:axId val="476687232"/>
+        <c:axId val="476687776"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -30244,7 +30220,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1632669920"/>
+        <c:axId val="476687232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -30278,7 +30254,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1632663392"/>
+        <c:crossAx val="476687776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -30286,7 +30262,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1632663392"/>
+        <c:axId val="476687776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -30296,7 +30272,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1632669920"/>
+        <c:crossAx val="476687232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -49914,7 +49890,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:E16"/>
+      <selection activeCell="F1" sqref="F1:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -49931,13 +49907,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="161" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="162"/>
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="163"/>
       <c r="F1" s="51" t="s">
         <v>19</v>
       </c>
@@ -50107,13 +50083,13 @@
       <c r="I8" s="52"/>
     </row>
     <row r="9" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="163" t="s">
+      <c r="A9" s="164" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="164"/>
-      <c r="C9" s="164"/>
-      <c r="D9" s="164"/>
-      <c r="E9" s="165"/>
+      <c r="B9" s="165"/>
+      <c r="C9" s="165"/>
+      <c r="D9" s="165"/>
+      <c r="E9" s="166"/>
       <c r="F9" s="52"/>
       <c r="G9" s="52"/>
       <c r="H9" s="52"/>
@@ -50204,13 +50180,13 @@
       <c r="I13" s="52"/>
     </row>
     <row r="14" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="163" t="s">
+      <c r="A14" s="164" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="164"/>
-      <c r="C14" s="164"/>
-      <c r="D14" s="164"/>
-      <c r="E14" s="165"/>
+      <c r="B14" s="165"/>
+      <c r="C14" s="165"/>
+      <c r="D14" s="165"/>
+      <c r="E14" s="166"/>
       <c r="F14" s="52"/>
       <c r="G14" s="52"/>
       <c r="H14" s="52"/>
@@ -50304,13 +50280,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="177" t="s">
+      <c r="A2" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="177"/>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="177"/>
+      <c r="B2" s="178"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="138" t="s">
@@ -50415,13 +50391,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="177" t="s">
+      <c r="A9" s="178" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="177"/>
-      <c r="C9" s="177"/>
-      <c r="D9" s="177"/>
-      <c r="E9" s="177"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="178"/>
+      <c r="D9" s="178"/>
+      <c r="E9" s="178"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="138" t="s">
@@ -50475,13 +50451,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="177" t="s">
+      <c r="A13" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="177"/>
-      <c r="C13" s="177"/>
-      <c r="D13" s="177"/>
-      <c r="E13" s="177"/>
+      <c r="B13" s="178"/>
+      <c r="C13" s="178"/>
+      <c r="D13" s="178"/>
+      <c r="E13" s="178"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="138" t="s">
@@ -50545,13 +50521,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="177" t="s">
+      <c r="A2" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="177"/>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="177"/>
+      <c r="B2" s="178"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="138" t="s">
@@ -50656,13 +50632,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="177" t="s">
+      <c r="A9" s="178" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="177"/>
-      <c r="C9" s="177"/>
-      <c r="D9" s="177"/>
-      <c r="E9" s="177"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="178"/>
+      <c r="D9" s="178"/>
+      <c r="E9" s="178"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="138" t="s">
@@ -50716,13 +50692,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="177" t="s">
+      <c r="A13" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="177"/>
-      <c r="C13" s="177"/>
-      <c r="D13" s="177"/>
-      <c r="E13" s="177"/>
+      <c r="B13" s="178"/>
+      <c r="C13" s="178"/>
+      <c r="D13" s="178"/>
+      <c r="E13" s="178"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="138" t="s">
@@ -50790,10 +50766,10 @@
       <c r="A2" s="158" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="178"/>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
-      <c r="E2" s="178"/>
+      <c r="B2" s="179"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="179"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="138" t="s">
@@ -50901,10 +50877,10 @@
       <c r="A9" s="158" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="178"/>
-      <c r="C9" s="178"/>
-      <c r="D9" s="178"/>
-      <c r="E9" s="178"/>
+      <c r="B9" s="179"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="138" t="s">
@@ -50961,10 +50937,10 @@
       <c r="A13" s="158" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="178"/>
-      <c r="C13" s="178"/>
-      <c r="D13" s="178"/>
-      <c r="E13" s="178"/>
+      <c r="B13" s="179"/>
+      <c r="C13" s="179"/>
+      <c r="D13" s="179"/>
+      <c r="E13" s="179"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="138" t="s">
@@ -51032,10 +51008,10 @@
       <c r="A2" s="159" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="178"/>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
-      <c r="E2" s="178"/>
+      <c r="B2" s="179"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="179"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="138" t="s">
@@ -51143,10 +51119,10 @@
       <c r="A9" s="159" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="178"/>
-      <c r="C9" s="178"/>
-      <c r="D9" s="178"/>
-      <c r="E9" s="178"/>
+      <c r="B9" s="179"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="138" t="s">
@@ -51203,10 +51179,10 @@
       <c r="A13" s="159" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="178"/>
-      <c r="C13" s="178"/>
-      <c r="D13" s="178"/>
-      <c r="E13" s="178"/>
+      <c r="B13" s="179"/>
+      <c r="C13" s="179"/>
+      <c r="D13" s="179"/>
+      <c r="E13" s="179"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="138" t="s">
@@ -51243,8 +51219,8 @@
   </sheetPr>
   <dimension ref="A1:AU100"/>
   <sheetViews>
-    <sheetView topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AM18" sqref="AM18:AO19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -51299,55 +51275,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="179" t="s">
+      <c r="A1" s="180" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="180"/>
-      <c r="G1" s="180"/>
-      <c r="H1" s="180"/>
-      <c r="I1" s="180"/>
-      <c r="J1" s="180"/>
-      <c r="K1" s="180"/>
-      <c r="L1" s="180"/>
-      <c r="M1" s="180"/>
-      <c r="N1" s="180"/>
-      <c r="O1" s="180"/>
-      <c r="P1" s="180"/>
-      <c r="Q1" s="180"/>
-      <c r="R1" s="180"/>
-      <c r="S1" s="180"/>
-      <c r="T1" s="180"/>
-      <c r="U1" s="180"/>
-      <c r="V1" s="180"/>
-      <c r="W1" s="180"/>
-      <c r="X1" s="180"/>
-      <c r="Y1" s="180"/>
-      <c r="Z1" s="180"/>
-      <c r="AA1" s="180"/>
-      <c r="AB1" s="180"/>
-      <c r="AC1" s="180"/>
-      <c r="AD1" s="180"/>
-      <c r="AE1" s="180"/>
-      <c r="AF1" s="180"/>
-      <c r="AG1" s="180"/>
-      <c r="AH1" s="180"/>
-      <c r="AI1" s="180"/>
-      <c r="AJ1" s="180"/>
-      <c r="AK1" s="180"/>
-      <c r="AL1" s="180"/>
-      <c r="AM1" s="180"/>
-      <c r="AN1" s="180"/>
-      <c r="AO1" s="180"/>
-      <c r="AP1" s="180"/>
-      <c r="AQ1" s="180"/>
-      <c r="AR1" s="180"/>
-      <c r="AS1" s="180"/>
-      <c r="AT1" s="180"/>
-      <c r="AU1" s="181"/>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="181"/>
+      <c r="E1" s="181"/>
+      <c r="F1" s="181"/>
+      <c r="G1" s="181"/>
+      <c r="H1" s="181"/>
+      <c r="I1" s="181"/>
+      <c r="J1" s="181"/>
+      <c r="K1" s="181"/>
+      <c r="L1" s="181"/>
+      <c r="M1" s="181"/>
+      <c r="N1" s="181"/>
+      <c r="O1" s="181"/>
+      <c r="P1" s="181"/>
+      <c r="Q1" s="181"/>
+      <c r="R1" s="181"/>
+      <c r="S1" s="181"/>
+      <c r="T1" s="181"/>
+      <c r="U1" s="181"/>
+      <c r="V1" s="181"/>
+      <c r="W1" s="181"/>
+      <c r="X1" s="181"/>
+      <c r="Y1" s="181"/>
+      <c r="Z1" s="181"/>
+      <c r="AA1" s="181"/>
+      <c r="AB1" s="181"/>
+      <c r="AC1" s="181"/>
+      <c r="AD1" s="181"/>
+      <c r="AE1" s="181"/>
+      <c r="AF1" s="181"/>
+      <c r="AG1" s="181"/>
+      <c r="AH1" s="181"/>
+      <c r="AI1" s="181"/>
+      <c r="AJ1" s="181"/>
+      <c r="AK1" s="181"/>
+      <c r="AL1" s="181"/>
+      <c r="AM1" s="181"/>
+      <c r="AN1" s="181"/>
+      <c r="AO1" s="181"/>
+      <c r="AP1" s="181"/>
+      <c r="AQ1" s="181"/>
+      <c r="AR1" s="181"/>
+      <c r="AS1" s="181"/>
+      <c r="AT1" s="181"/>
+      <c r="AU1" s="182"/>
     </row>
     <row r="2" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="129" t="s">
@@ -52384,55 +52360,55 @@
       <c r="AU9" s="18"/>
     </row>
     <row r="10" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="182" t="s">
+      <c r="A10" s="183" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="183"/>
-      <c r="C10" s="183"/>
-      <c r="D10" s="183"/>
-      <c r="E10" s="183"/>
-      <c r="F10" s="183"/>
-      <c r="G10" s="183"/>
-      <c r="H10" s="183"/>
-      <c r="I10" s="183"/>
-      <c r="J10" s="183"/>
-      <c r="K10" s="183"/>
-      <c r="L10" s="183"/>
-      <c r="M10" s="183"/>
-      <c r="N10" s="183"/>
-      <c r="O10" s="183"/>
-      <c r="P10" s="183"/>
-      <c r="Q10" s="183"/>
-      <c r="R10" s="183"/>
-      <c r="S10" s="183"/>
-      <c r="T10" s="183"/>
-      <c r="U10" s="183"/>
-      <c r="V10" s="183"/>
-      <c r="W10" s="183"/>
-      <c r="X10" s="183"/>
-      <c r="Y10" s="183"/>
-      <c r="Z10" s="183"/>
-      <c r="AA10" s="183"/>
-      <c r="AB10" s="183"/>
-      <c r="AC10" s="183"/>
-      <c r="AD10" s="183"/>
-      <c r="AE10" s="183"/>
-      <c r="AF10" s="183"/>
-      <c r="AG10" s="183"/>
-      <c r="AH10" s="183"/>
-      <c r="AI10" s="183"/>
-      <c r="AJ10" s="183"/>
-      <c r="AK10" s="183"/>
-      <c r="AL10" s="183"/>
-      <c r="AM10" s="183"/>
-      <c r="AN10" s="183"/>
-      <c r="AO10" s="183"/>
-      <c r="AP10" s="183"/>
-      <c r="AQ10" s="183"/>
-      <c r="AR10" s="183"/>
-      <c r="AS10" s="183"/>
-      <c r="AT10" s="183"/>
-      <c r="AU10" s="183"/>
+      <c r="B10" s="184"/>
+      <c r="C10" s="184"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="184"/>
+      <c r="F10" s="184"/>
+      <c r="G10" s="184"/>
+      <c r="H10" s="184"/>
+      <c r="I10" s="184"/>
+      <c r="J10" s="184"/>
+      <c r="K10" s="184"/>
+      <c r="L10" s="184"/>
+      <c r="M10" s="184"/>
+      <c r="N10" s="184"/>
+      <c r="O10" s="184"/>
+      <c r="P10" s="184"/>
+      <c r="Q10" s="184"/>
+      <c r="R10" s="184"/>
+      <c r="S10" s="184"/>
+      <c r="T10" s="184"/>
+      <c r="U10" s="184"/>
+      <c r="V10" s="184"/>
+      <c r="W10" s="184"/>
+      <c r="X10" s="184"/>
+      <c r="Y10" s="184"/>
+      <c r="Z10" s="184"/>
+      <c r="AA10" s="184"/>
+      <c r="AB10" s="184"/>
+      <c r="AC10" s="184"/>
+      <c r="AD10" s="184"/>
+      <c r="AE10" s="184"/>
+      <c r="AF10" s="184"/>
+      <c r="AG10" s="184"/>
+      <c r="AH10" s="184"/>
+      <c r="AI10" s="184"/>
+      <c r="AJ10" s="184"/>
+      <c r="AK10" s="184"/>
+      <c r="AL10" s="184"/>
+      <c r="AM10" s="184"/>
+      <c r="AN10" s="184"/>
+      <c r="AO10" s="184"/>
+      <c r="AP10" s="184"/>
+      <c r="AQ10" s="184"/>
+      <c r="AR10" s="184"/>
+      <c r="AS10" s="184"/>
+      <c r="AT10" s="184"/>
+      <c r="AU10" s="184"/>
     </row>
     <row r="11" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
@@ -53100,55 +53076,55 @@
       <c r="AU15" s="18"/>
     </row>
     <row r="16" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="182" t="s">
+      <c r="A16" s="183" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="183"/>
-      <c r="C16" s="183"/>
-      <c r="D16" s="183"/>
-      <c r="E16" s="183"/>
-      <c r="F16" s="183"/>
-      <c r="G16" s="183"/>
-      <c r="H16" s="183"/>
-      <c r="I16" s="183"/>
-      <c r="J16" s="183"/>
-      <c r="K16" s="183"/>
-      <c r="L16" s="183"/>
-      <c r="M16" s="183"/>
-      <c r="N16" s="183"/>
-      <c r="O16" s="183"/>
-      <c r="P16" s="183"/>
-      <c r="Q16" s="183"/>
-      <c r="R16" s="183"/>
-      <c r="S16" s="183"/>
-      <c r="T16" s="183"/>
-      <c r="U16" s="183"/>
-      <c r="V16" s="183"/>
-      <c r="W16" s="183"/>
-      <c r="X16" s="183"/>
-      <c r="Y16" s="183"/>
-      <c r="Z16" s="183"/>
-      <c r="AA16" s="183"/>
-      <c r="AB16" s="183"/>
-      <c r="AC16" s="183"/>
-      <c r="AD16" s="183"/>
-      <c r="AE16" s="183"/>
-      <c r="AF16" s="183"/>
-      <c r="AG16" s="183"/>
-      <c r="AH16" s="183"/>
-      <c r="AI16" s="183"/>
-      <c r="AJ16" s="183"/>
-      <c r="AK16" s="183"/>
-      <c r="AL16" s="183"/>
-      <c r="AM16" s="183"/>
-      <c r="AN16" s="183"/>
-      <c r="AO16" s="183"/>
-      <c r="AP16" s="183"/>
-      <c r="AQ16" s="183"/>
-      <c r="AR16" s="183"/>
-      <c r="AS16" s="183"/>
-      <c r="AT16" s="183"/>
-      <c r="AU16" s="183"/>
+      <c r="B16" s="184"/>
+      <c r="C16" s="184"/>
+      <c r="D16" s="184"/>
+      <c r="E16" s="184"/>
+      <c r="F16" s="184"/>
+      <c r="G16" s="184"/>
+      <c r="H16" s="184"/>
+      <c r="I16" s="184"/>
+      <c r="J16" s="184"/>
+      <c r="K16" s="184"/>
+      <c r="L16" s="184"/>
+      <c r="M16" s="184"/>
+      <c r="N16" s="184"/>
+      <c r="O16" s="184"/>
+      <c r="P16" s="184"/>
+      <c r="Q16" s="184"/>
+      <c r="R16" s="184"/>
+      <c r="S16" s="184"/>
+      <c r="T16" s="184"/>
+      <c r="U16" s="184"/>
+      <c r="V16" s="184"/>
+      <c r="W16" s="184"/>
+      <c r="X16" s="184"/>
+      <c r="Y16" s="184"/>
+      <c r="Z16" s="184"/>
+      <c r="AA16" s="184"/>
+      <c r="AB16" s="184"/>
+      <c r="AC16" s="184"/>
+      <c r="AD16" s="184"/>
+      <c r="AE16" s="184"/>
+      <c r="AF16" s="184"/>
+      <c r="AG16" s="184"/>
+      <c r="AH16" s="184"/>
+      <c r="AI16" s="184"/>
+      <c r="AJ16" s="184"/>
+      <c r="AK16" s="184"/>
+      <c r="AL16" s="184"/>
+      <c r="AM16" s="184"/>
+      <c r="AN16" s="184"/>
+      <c r="AO16" s="184"/>
+      <c r="AP16" s="184"/>
+      <c r="AQ16" s="184"/>
+      <c r="AR16" s="184"/>
+      <c r="AS16" s="184"/>
+      <c r="AT16" s="184"/>
+      <c r="AU16" s="184"/>
     </row>
     <row r="17" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
@@ -53406,7 +53382,7 @@
       <c r="AL18" s="29">
         <v>43602</v>
       </c>
-      <c r="AM18" s="185">
+      <c r="AM18" s="160">
         <v>43605</v>
       </c>
       <c r="AN18" s="28">
@@ -53706,55 +53682,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="182" t="s">
+      <c r="A1" s="183" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="183"/>
-      <c r="C1" s="183"/>
-      <c r="D1" s="183"/>
-      <c r="E1" s="183"/>
-      <c r="F1" s="183"/>
-      <c r="G1" s="183"/>
-      <c r="H1" s="183"/>
-      <c r="I1" s="183"/>
-      <c r="J1" s="183"/>
-      <c r="K1" s="183"/>
-      <c r="L1" s="183"/>
-      <c r="M1" s="183"/>
-      <c r="N1" s="183"/>
-      <c r="O1" s="183"/>
-      <c r="P1" s="183"/>
-      <c r="Q1" s="183"/>
-      <c r="R1" s="183"/>
-      <c r="S1" s="183"/>
-      <c r="T1" s="183"/>
-      <c r="U1" s="183"/>
-      <c r="V1" s="183"/>
-      <c r="W1" s="183"/>
-      <c r="X1" s="183"/>
-      <c r="Y1" s="183"/>
-      <c r="Z1" s="183"/>
-      <c r="AA1" s="183"/>
-      <c r="AB1" s="183"/>
-      <c r="AC1" s="183"/>
-      <c r="AD1" s="183"/>
-      <c r="AE1" s="183"/>
-      <c r="AF1" s="183"/>
-      <c r="AG1" s="183"/>
-      <c r="AH1" s="183"/>
-      <c r="AI1" s="183"/>
-      <c r="AJ1" s="183"/>
-      <c r="AK1" s="183"/>
-      <c r="AL1" s="183"/>
-      <c r="AM1" s="183"/>
-      <c r="AN1" s="183"/>
-      <c r="AO1" s="183"/>
-      <c r="AP1" s="183"/>
-      <c r="AQ1" s="183"/>
-      <c r="AR1" s="183"/>
-      <c r="AS1" s="183"/>
-      <c r="AT1" s="183"/>
-      <c r="AU1" s="183"/>
+      <c r="B1" s="184"/>
+      <c r="C1" s="184"/>
+      <c r="D1" s="184"/>
+      <c r="E1" s="184"/>
+      <c r="F1" s="184"/>
+      <c r="G1" s="184"/>
+      <c r="H1" s="184"/>
+      <c r="I1" s="184"/>
+      <c r="J1" s="184"/>
+      <c r="K1" s="184"/>
+      <c r="L1" s="184"/>
+      <c r="M1" s="184"/>
+      <c r="N1" s="184"/>
+      <c r="O1" s="184"/>
+      <c r="P1" s="184"/>
+      <c r="Q1" s="184"/>
+      <c r="R1" s="184"/>
+      <c r="S1" s="184"/>
+      <c r="T1" s="184"/>
+      <c r="U1" s="184"/>
+      <c r="V1" s="184"/>
+      <c r="W1" s="184"/>
+      <c r="X1" s="184"/>
+      <c r="Y1" s="184"/>
+      <c r="Z1" s="184"/>
+      <c r="AA1" s="184"/>
+      <c r="AB1" s="184"/>
+      <c r="AC1" s="184"/>
+      <c r="AD1" s="184"/>
+      <c r="AE1" s="184"/>
+      <c r="AF1" s="184"/>
+      <c r="AG1" s="184"/>
+      <c r="AH1" s="184"/>
+      <c r="AI1" s="184"/>
+      <c r="AJ1" s="184"/>
+      <c r="AK1" s="184"/>
+      <c r="AL1" s="184"/>
+      <c r="AM1" s="184"/>
+      <c r="AN1" s="184"/>
+      <c r="AO1" s="184"/>
+      <c r="AP1" s="184"/>
+      <c r="AQ1" s="184"/>
+      <c r="AR1" s="184"/>
+      <c r="AS1" s="184"/>
+      <c r="AT1" s="184"/>
+      <c r="AU1" s="184"/>
     </row>
     <row r="2" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
@@ -54585,55 +54561,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="184" t="s">
+      <c r="A1" s="185" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="184"/>
-      <c r="C1" s="184"/>
-      <c r="D1" s="184"/>
-      <c r="E1" s="184"/>
-      <c r="F1" s="184"/>
-      <c r="G1" s="184"/>
-      <c r="H1" s="184"/>
-      <c r="I1" s="184"/>
-      <c r="J1" s="184"/>
-      <c r="K1" s="184"/>
-      <c r="L1" s="184"/>
-      <c r="M1" s="184"/>
-      <c r="N1" s="184"/>
-      <c r="O1" s="184"/>
-      <c r="P1" s="184"/>
-      <c r="Q1" s="184"/>
-      <c r="R1" s="184"/>
-      <c r="S1" s="184"/>
-      <c r="T1" s="184"/>
-      <c r="U1" s="184"/>
-      <c r="V1" s="184"/>
-      <c r="W1" s="184"/>
-      <c r="X1" s="184"/>
-      <c r="Y1" s="184"/>
-      <c r="Z1" s="184"/>
-      <c r="AA1" s="184"/>
-      <c r="AB1" s="184"/>
-      <c r="AC1" s="184"/>
-      <c r="AD1" s="184"/>
-      <c r="AE1" s="184"/>
-      <c r="AF1" s="184"/>
-      <c r="AG1" s="184"/>
-      <c r="AH1" s="184"/>
-      <c r="AI1" s="184"/>
-      <c r="AJ1" s="184"/>
-      <c r="AK1" s="184"/>
-      <c r="AL1" s="184"/>
-      <c r="AM1" s="184"/>
-      <c r="AN1" s="184"/>
-      <c r="AO1" s="184"/>
-      <c r="AP1" s="184"/>
-      <c r="AQ1" s="184"/>
-      <c r="AR1" s="184"/>
-      <c r="AS1" s="184"/>
-      <c r="AT1" s="184"/>
-      <c r="AU1" s="184"/>
+      <c r="B1" s="185"/>
+      <c r="C1" s="185"/>
+      <c r="D1" s="185"/>
+      <c r="E1" s="185"/>
+      <c r="F1" s="185"/>
+      <c r="G1" s="185"/>
+      <c r="H1" s="185"/>
+      <c r="I1" s="185"/>
+      <c r="J1" s="185"/>
+      <c r="K1" s="185"/>
+      <c r="L1" s="185"/>
+      <c r="M1" s="185"/>
+      <c r="N1" s="185"/>
+      <c r="O1" s="185"/>
+      <c r="P1" s="185"/>
+      <c r="Q1" s="185"/>
+      <c r="R1" s="185"/>
+      <c r="S1" s="185"/>
+      <c r="T1" s="185"/>
+      <c r="U1" s="185"/>
+      <c r="V1" s="185"/>
+      <c r="W1" s="185"/>
+      <c r="X1" s="185"/>
+      <c r="Y1" s="185"/>
+      <c r="Z1" s="185"/>
+      <c r="AA1" s="185"/>
+      <c r="AB1" s="185"/>
+      <c r="AC1" s="185"/>
+      <c r="AD1" s="185"/>
+      <c r="AE1" s="185"/>
+      <c r="AF1" s="185"/>
+      <c r="AG1" s="185"/>
+      <c r="AH1" s="185"/>
+      <c r="AI1" s="185"/>
+      <c r="AJ1" s="185"/>
+      <c r="AK1" s="185"/>
+      <c r="AL1" s="185"/>
+      <c r="AM1" s="185"/>
+      <c r="AN1" s="185"/>
+      <c r="AO1" s="185"/>
+      <c r="AP1" s="185"/>
+      <c r="AQ1" s="185"/>
+      <c r="AR1" s="185"/>
+      <c r="AS1" s="185"/>
+      <c r="AT1" s="185"/>
+      <c r="AU1" s="185"/>
     </row>
     <row r="2" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -55440,55 +55416,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="184" t="s">
+      <c r="A1" s="185" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="184"/>
-      <c r="C1" s="184"/>
-      <c r="D1" s="184"/>
-      <c r="E1" s="184"/>
-      <c r="F1" s="184"/>
-      <c r="G1" s="184"/>
-      <c r="H1" s="184"/>
-      <c r="I1" s="184"/>
-      <c r="J1" s="184"/>
-      <c r="K1" s="184"/>
-      <c r="L1" s="184"/>
-      <c r="M1" s="184"/>
-      <c r="N1" s="184"/>
-      <c r="O1" s="184"/>
-      <c r="P1" s="184"/>
-      <c r="Q1" s="184"/>
-      <c r="R1" s="184"/>
-      <c r="S1" s="184"/>
-      <c r="T1" s="184"/>
-      <c r="U1" s="184"/>
-      <c r="V1" s="184"/>
-      <c r="W1" s="184"/>
-      <c r="X1" s="184"/>
-      <c r="Y1" s="184"/>
-      <c r="Z1" s="184"/>
-      <c r="AA1" s="184"/>
-      <c r="AB1" s="184"/>
-      <c r="AC1" s="184"/>
-      <c r="AD1" s="184"/>
-      <c r="AE1" s="184"/>
-      <c r="AF1" s="184"/>
-      <c r="AG1" s="184"/>
-      <c r="AH1" s="184"/>
-      <c r="AI1" s="184"/>
-      <c r="AJ1" s="184"/>
-      <c r="AK1" s="184"/>
-      <c r="AL1" s="184"/>
-      <c r="AM1" s="184"/>
-      <c r="AN1" s="184"/>
-      <c r="AO1" s="184"/>
-      <c r="AP1" s="184"/>
-      <c r="AQ1" s="184"/>
-      <c r="AR1" s="184"/>
-      <c r="AS1" s="184"/>
-      <c r="AT1" s="184"/>
-      <c r="AU1" s="184"/>
+      <c r="B1" s="185"/>
+      <c r="C1" s="185"/>
+      <c r="D1" s="185"/>
+      <c r="E1" s="185"/>
+      <c r="F1" s="185"/>
+      <c r="G1" s="185"/>
+      <c r="H1" s="185"/>
+      <c r="I1" s="185"/>
+      <c r="J1" s="185"/>
+      <c r="K1" s="185"/>
+      <c r="L1" s="185"/>
+      <c r="M1" s="185"/>
+      <c r="N1" s="185"/>
+      <c r="O1" s="185"/>
+      <c r="P1" s="185"/>
+      <c r="Q1" s="185"/>
+      <c r="R1" s="185"/>
+      <c r="S1" s="185"/>
+      <c r="T1" s="185"/>
+      <c r="U1" s="185"/>
+      <c r="V1" s="185"/>
+      <c r="W1" s="185"/>
+      <c r="X1" s="185"/>
+      <c r="Y1" s="185"/>
+      <c r="Z1" s="185"/>
+      <c r="AA1" s="185"/>
+      <c r="AB1" s="185"/>
+      <c r="AC1" s="185"/>
+      <c r="AD1" s="185"/>
+      <c r="AE1" s="185"/>
+      <c r="AF1" s="185"/>
+      <c r="AG1" s="185"/>
+      <c r="AH1" s="185"/>
+      <c r="AI1" s="185"/>
+      <c r="AJ1" s="185"/>
+      <c r="AK1" s="185"/>
+      <c r="AL1" s="185"/>
+      <c r="AM1" s="185"/>
+      <c r="AN1" s="185"/>
+      <c r="AO1" s="185"/>
+      <c r="AP1" s="185"/>
+      <c r="AQ1" s="185"/>
+      <c r="AR1" s="185"/>
+      <c r="AS1" s="185"/>
+      <c r="AT1" s="185"/>
+      <c r="AU1" s="185"/>
     </row>
     <row r="2" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -56263,7 +56239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AM3" sqref="AM3:AO4"/>
     </sheetView>
   </sheetViews>
@@ -56319,55 +56295,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="179" t="s">
+      <c r="A1" s="180" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="180"/>
-      <c r="G1" s="180"/>
-      <c r="H1" s="180"/>
-      <c r="I1" s="180"/>
-      <c r="J1" s="180"/>
-      <c r="K1" s="180"/>
-      <c r="L1" s="180"/>
-      <c r="M1" s="180"/>
-      <c r="N1" s="180"/>
-      <c r="O1" s="180"/>
-      <c r="P1" s="180"/>
-      <c r="Q1" s="180"/>
-      <c r="R1" s="180"/>
-      <c r="S1" s="180"/>
-      <c r="T1" s="180"/>
-      <c r="U1" s="180"/>
-      <c r="V1" s="180"/>
-      <c r="W1" s="180"/>
-      <c r="X1" s="180"/>
-      <c r="Y1" s="180"/>
-      <c r="Z1" s="180"/>
-      <c r="AA1" s="180"/>
-      <c r="AB1" s="180"/>
-      <c r="AC1" s="180"/>
-      <c r="AD1" s="180"/>
-      <c r="AE1" s="180"/>
-      <c r="AF1" s="180"/>
-      <c r="AG1" s="180"/>
-      <c r="AH1" s="180"/>
-      <c r="AI1" s="180"/>
-      <c r="AJ1" s="180"/>
-      <c r="AK1" s="180"/>
-      <c r="AL1" s="180"/>
-      <c r="AM1" s="180"/>
-      <c r="AN1" s="180"/>
-      <c r="AO1" s="180"/>
-      <c r="AP1" s="180"/>
-      <c r="AQ1" s="180"/>
-      <c r="AR1" s="180"/>
-      <c r="AS1" s="180"/>
-      <c r="AT1" s="180"/>
-      <c r="AU1" s="181"/>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="181"/>
+      <c r="E1" s="181"/>
+      <c r="F1" s="181"/>
+      <c r="G1" s="181"/>
+      <c r="H1" s="181"/>
+      <c r="I1" s="181"/>
+      <c r="J1" s="181"/>
+      <c r="K1" s="181"/>
+      <c r="L1" s="181"/>
+      <c r="M1" s="181"/>
+      <c r="N1" s="181"/>
+      <c r="O1" s="181"/>
+      <c r="P1" s="181"/>
+      <c r="Q1" s="181"/>
+      <c r="R1" s="181"/>
+      <c r="S1" s="181"/>
+      <c r="T1" s="181"/>
+      <c r="U1" s="181"/>
+      <c r="V1" s="181"/>
+      <c r="W1" s="181"/>
+      <c r="X1" s="181"/>
+      <c r="Y1" s="181"/>
+      <c r="Z1" s="181"/>
+      <c r="AA1" s="181"/>
+      <c r="AB1" s="181"/>
+      <c r="AC1" s="181"/>
+      <c r="AD1" s="181"/>
+      <c r="AE1" s="181"/>
+      <c r="AF1" s="181"/>
+      <c r="AG1" s="181"/>
+      <c r="AH1" s="181"/>
+      <c r="AI1" s="181"/>
+      <c r="AJ1" s="181"/>
+      <c r="AK1" s="181"/>
+      <c r="AL1" s="181"/>
+      <c r="AM1" s="181"/>
+      <c r="AN1" s="181"/>
+      <c r="AO1" s="181"/>
+      <c r="AP1" s="181"/>
+      <c r="AQ1" s="181"/>
+      <c r="AR1" s="181"/>
+      <c r="AS1" s="181"/>
+      <c r="AT1" s="181"/>
+      <c r="AU1" s="182"/>
     </row>
     <row r="2" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
@@ -56625,7 +56601,7 @@
       <c r="AL3" s="29">
         <v>43602</v>
       </c>
-      <c r="AM3" s="185">
+      <c r="AM3" s="160">
         <v>43605</v>
       </c>
       <c r="AN3" s="28">
@@ -56929,13 +56905,13 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="166" t="s">
+      <c r="A2" s="167" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="167"/>
-      <c r="C2" s="167"/>
-      <c r="D2" s="167"/>
-      <c r="E2" s="168"/>
+      <c r="B2" s="168"/>
+      <c r="C2" s="168"/>
+      <c r="D2" s="168"/>
+      <c r="E2" s="169"/>
       <c r="F2" s="52"/>
       <c r="G2" s="52"/>
       <c r="H2" s="52"/>
@@ -57076,13 +57052,13 @@
       <c r="I8" s="52"/>
     </row>
     <row r="9" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="169" t="s">
+      <c r="A9" s="170" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="170"/>
-      <c r="C9" s="170"/>
-      <c r="D9" s="170"/>
-      <c r="E9" s="171"/>
+      <c r="B9" s="171"/>
+      <c r="C9" s="171"/>
+      <c r="D9" s="171"/>
+      <c r="E9" s="172"/>
       <c r="F9" s="52"/>
       <c r="G9" s="52"/>
       <c r="H9" s="52"/>
@@ -57152,13 +57128,13 @@
       <c r="I12" s="52"/>
     </row>
     <row r="13" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="166" t="s">
+      <c r="A13" s="167" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="167"/>
-      <c r="C13" s="167"/>
-      <c r="D13" s="167"/>
-      <c r="E13" s="168"/>
+      <c r="B13" s="168"/>
+      <c r="C13" s="168"/>
+      <c r="D13" s="168"/>
+      <c r="E13" s="169"/>
       <c r="F13" s="52"/>
       <c r="G13" s="52"/>
       <c r="H13" s="52"/>
@@ -57247,13 +57223,13 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="172" t="s">
+      <c r="A2" s="173" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="173"/>
-      <c r="C2" s="173"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="173"/>
+      <c r="B2" s="174"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
       <c r="F2" s="52"/>
       <c r="G2" s="52"/>
       <c r="H2" s="52"/>
@@ -57394,13 +57370,13 @@
       <c r="I8" s="52"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="174" t="s">
+      <c r="A9" s="175" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="175"/>
-      <c r="C9" s="175"/>
-      <c r="D9" s="175"/>
-      <c r="E9" s="175"/>
+      <c r="B9" s="176"/>
+      <c r="C9" s="176"/>
+      <c r="D9" s="176"/>
+      <c r="E9" s="176"/>
       <c r="F9" s="52"/>
       <c r="G9" s="52"/>
       <c r="H9" s="52"/>
@@ -57470,13 +57446,13 @@
       <c r="I12" s="52"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="174" t="s">
+      <c r="A13" s="175" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="175"/>
-      <c r="C13" s="175"/>
-      <c r="D13" s="175"/>
-      <c r="E13" s="175"/>
+      <c r="B13" s="176"/>
+      <c r="C13" s="176"/>
+      <c r="D13" s="176"/>
+      <c r="E13" s="176"/>
       <c r="F13" s="52"/>
       <c r="G13" s="52"/>
       <c r="H13" s="52"/>
@@ -57548,13 +57524,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="177" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="138" t="s">
@@ -57659,13 +57635,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="177" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="176"/>
-      <c r="C9" s="176"/>
-      <c r="D9" s="176"/>
-      <c r="E9" s="176"/>
+      <c r="B9" s="177"/>
+      <c r="C9" s="177"/>
+      <c r="D9" s="177"/>
+      <c r="E9" s="177"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="138" t="s">
@@ -57719,13 +57695,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="176" t="s">
+      <c r="A13" s="177" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="176"/>
-      <c r="C13" s="176"/>
-      <c r="D13" s="176"/>
-      <c r="E13" s="176"/>
+      <c r="B13" s="177"/>
+      <c r="C13" s="177"/>
+      <c r="D13" s="177"/>
+      <c r="E13" s="177"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="138" t="s">
@@ -57790,13 +57766,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="177" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="138" t="s">
@@ -57901,13 +57877,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="177" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="176"/>
-      <c r="C9" s="176"/>
-      <c r="D9" s="176"/>
-      <c r="E9" s="176"/>
+      <c r="B9" s="177"/>
+      <c r="C9" s="177"/>
+      <c r="D9" s="177"/>
+      <c r="E9" s="177"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="138" t="s">
@@ -57961,13 +57937,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="176" t="s">
+      <c r="A13" s="177" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="176"/>
-      <c r="C13" s="176"/>
-      <c r="D13" s="176"/>
-      <c r="E13" s="176"/>
+      <c r="B13" s="177"/>
+      <c r="C13" s="177"/>
+      <c r="D13" s="177"/>
+      <c r="E13" s="177"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="138" t="s">
@@ -58033,13 +58009,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="177" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
     </row>
     <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="138" t="s">
@@ -58127,13 +58103,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="177" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="176"/>
-      <c r="C8" s="176"/>
-      <c r="D8" s="176"/>
-      <c r="E8" s="176"/>
+      <c r="B8" s="177"/>
+      <c r="C8" s="177"/>
+      <c r="D8" s="177"/>
+      <c r="E8" s="177"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="138" t="s">
@@ -58187,13 +58163,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="176" t="s">
+      <c r="A12" s="177" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="176"/>
-      <c r="C12" s="176"/>
-      <c r="D12" s="176"/>
-      <c r="E12" s="176"/>
+      <c r="B12" s="177"/>
+      <c r="C12" s="177"/>
+      <c r="D12" s="177"/>
+      <c r="E12" s="177"/>
     </row>
     <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="138" t="s">
@@ -58259,13 +58235,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="177" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
     </row>
     <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="138" t="s">
@@ -58353,13 +58329,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="177" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="176"/>
-      <c r="C8" s="176"/>
-      <c r="D8" s="176"/>
-      <c r="E8" s="176"/>
+      <c r="B8" s="177"/>
+      <c r="C8" s="177"/>
+      <c r="D8" s="177"/>
+      <c r="E8" s="177"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="138" t="s">
@@ -58413,13 +58389,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="176" t="s">
+      <c r="A12" s="177" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="176"/>
-      <c r="C12" s="176"/>
-      <c r="D12" s="176"/>
-      <c r="E12" s="176"/>
+      <c r="B12" s="177"/>
+      <c r="C12" s="177"/>
+      <c r="D12" s="177"/>
+      <c r="E12" s="177"/>
     </row>
     <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="138" t="s">
@@ -58483,13 +58459,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="177" t="s">
+      <c r="A2" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="177"/>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="177"/>
+      <c r="B2" s="178"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="138" t="s">
@@ -58577,13 +58553,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="177" t="s">
+      <c r="A8" s="178" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="177"/>
-      <c r="C8" s="177"/>
-      <c r="D8" s="177"/>
-      <c r="E8" s="177"/>
+      <c r="B8" s="178"/>
+      <c r="C8" s="178"/>
+      <c r="D8" s="178"/>
+      <c r="E8" s="178"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="138" t="s">
@@ -58637,13 +58613,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="177" t="s">
+      <c r="A12" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="177"/>
-      <c r="C12" s="177"/>
-      <c r="D12" s="177"/>
-      <c r="E12" s="177"/>
+      <c r="B12" s="178"/>
+      <c r="C12" s="178"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="178"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="138" t="s">
@@ -58708,13 +58684,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="177" t="s">
+      <c r="A2" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="177"/>
-      <c r="C2" s="177"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="177"/>
+      <c r="B2" s="178"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="138" t="s">
@@ -58802,13 +58778,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="177" t="s">
+      <c r="A8" s="178" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="177"/>
-      <c r="C8" s="177"/>
-      <c r="D8" s="177"/>
-      <c r="E8" s="177"/>
+      <c r="B8" s="178"/>
+      <c r="C8" s="178"/>
+      <c r="D8" s="178"/>
+      <c r="E8" s="178"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="138" t="s">
@@ -58862,13 +58838,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="177" t="s">
+      <c r="A12" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="177"/>
-      <c r="C12" s="177"/>
-      <c r="D12" s="177"/>
-      <c r="E12" s="177"/>
+      <c r="B12" s="178"/>
+      <c r="C12" s="178"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="178"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="138" t="s">

</xml_diff>